<commit_message>
:construction: White tasting deck created
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,10 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Wine making" sheetId="2" r:id="rId1"/>
+    <sheet name="Wine tasting" sheetId="1" r:id="rId2"/>
+    <sheet name="Wine vocabulary" sheetId="3" r:id="rId3"/>
+    <sheet name="European designations" sheetId="4" r:id="rId4"/>
+    <sheet name="Wine temperature" sheetId="8" r:id="rId5"/>
+    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId6"/>
+    <sheet name="Varieties of designations" sheetId="6" r:id="rId7"/>
+    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -16,6 +23,155 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>Harvesting</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t>Crushing</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t>Fermentation</t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t>Ageing</t>
+  </si>
+  <si>
+    <t>Step 5</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
+    <t>1. Harvesting</t>
+  </si>
+  <si>
+    <t>2. Crushing (Red wine)</t>
+  </si>
+  <si>
+    <t>2. Crushing (White wine)</t>
+  </si>
+  <si>
+    <t>3. Fermentation</t>
+  </si>
+  <si>
+    <t>4. Ageing</t>
+  </si>
+  <si>
+    <t>Grapes are harvested</t>
+  </si>
+  <si>
+    <t>Grapes are crushed. Juice, seed, and skins are put into a tank.</t>
+  </si>
+  <si>
+    <t>Grapes are pressed. Only the juice is kept. Skins and seeds are removed.</t>
+  </si>
+  <si>
+    <t>The wine can be put in barrel to get in contact with the wood.</t>
+  </si>
+  <si>
+    <t>5. Packaging</t>
+  </si>
+  <si>
+    <t>The wine is put into bottles.</t>
+  </si>
+  <si>
+    <t>Red color</t>
+  </si>
+  <si>
+    <t>The yiest of the juice starts to turn the sugar into alcohol.</t>
+  </si>
+  <si>
+    <t>The wine goes red through the tannins of the skin (for Red Wine). You can make White wine with red grapes since you remove the skin</t>
+  </si>
+  <si>
+    <t>Why is sulphite added?</t>
+  </si>
+  <si>
+    <t>To stop the wine from turning into vinegar</t>
+  </si>
+  <si>
+    <t>Oak barrel</t>
+  </si>
+  <si>
+    <t>Often use for wine ageing especially for white wine</t>
+  </si>
+  <si>
+    <t>Rosé wine</t>
+  </si>
+  <si>
+    <t>Rosé wine is done like the red wine but the juice is taken earlier</t>
+  </si>
+  <si>
+    <t>Between 8,5% and 15%</t>
+  </si>
+  <si>
+    <t>Fortified wine</t>
+  </si>
+  <si>
+    <t>More than 15%</t>
+  </si>
+  <si>
+    <t>Fortified wine (like porto wine) are made by adding alcohol at the end to stop the fermentation process</t>
+  </si>
+  <si>
+    <t>Table wine alcohol level</t>
+  </si>
+  <si>
+    <t>Fortified wine alcohol level</t>
+  </si>
+  <si>
+    <t>Sparkling wine</t>
+  </si>
+  <si>
+    <t>During the fermentation, gaz is made, by blocking it into the bottle with the cap, the gaz enters into the wine to turn it into sparkle wine</t>
+  </si>
+  <si>
+    <t>Two basic rules</t>
+  </si>
+  <si>
+    <t>Take your time. Be attentive</t>
+  </si>
+  <si>
+    <t>The smell (the nose)</t>
+  </si>
+  <si>
+    <t>The look (the robe)</t>
+  </si>
+  <si>
+    <t>The taste (the mouth)</t>
+  </si>
+  <si>
+    <t>The feeling</t>
+  </si>
+  <si>
+    <t>1. Look</t>
+  </si>
+  <si>
+    <t>2. Smell</t>
+  </si>
+  <si>
+    <t>3. Taste</t>
+  </si>
+  <si>
+    <t>4. Feel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +270,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +305,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,11 +487,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
:construction: Wine tasting deck added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -9,12 +9,11 @@
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
     <sheet name="Wine tasting" sheetId="1" r:id="rId2"/>
-    <sheet name="Wine vocabulary" sheetId="3" r:id="rId3"/>
-    <sheet name="European designations" sheetId="4" r:id="rId4"/>
-    <sheet name="Wine temperature" sheetId="8" r:id="rId5"/>
-    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId6"/>
-    <sheet name="Varieties of designations" sheetId="6" r:id="rId7"/>
-    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId8"/>
+    <sheet name="European designations" sheetId="4" r:id="rId3"/>
+    <sheet name="Wine temperature" sheetId="8" r:id="rId4"/>
+    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId5"/>
+    <sheet name="Varieties of designations" sheetId="6" r:id="rId6"/>
+    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
   <si>
     <t>Step 1</t>
   </si>
@@ -169,7 +168,163 @@
     <t>3. Taste</t>
   </si>
   <si>
-    <t>4. Feel</t>
+    <t>The clarity and the color</t>
+  </si>
+  <si>
+    <t>Clarity</t>
+  </si>
+  <si>
+    <t>Brilliant - Bright - Clear - Dull - Hazy - Cloudy / Sediment? Crystals?</t>
+  </si>
+  <si>
+    <t>Color (White wine)</t>
+  </si>
+  <si>
+    <t>dilute, v. pale straw, pale straw, medium straw, yellow, lt. gold, medium gold, amber, tawny, adobe, brown</t>
+  </si>
+  <si>
+    <t>Color (Red wine)</t>
+  </si>
+  <si>
+    <t>light / medium / dark: garnet, ruby red, purplish-red, or combinations / tawny, brown edge, any rim variation?</t>
+  </si>
+  <si>
+    <t>Old color</t>
+  </si>
+  <si>
+    <t>The older is a wine (white or red), the closer to the brown will the color be</t>
+  </si>
+  <si>
+    <t>First sniff, swirling and Second sniff</t>
+  </si>
+  <si>
+    <t>Is the wine presentable? Fresh nose or aged-developed bouquet? OK to proceed? Any FAULTS? Corked, vinegary, oxidized / stale, stinky / eggy, sulfites</t>
+  </si>
+  <si>
+    <t>First sniff</t>
+  </si>
+  <si>
+    <t>Second sniff</t>
+  </si>
+  <si>
+    <t>Swirling</t>
+  </si>
+  <si>
+    <t>Needs a good wine glass, makes the flavor easier to smell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruity / floral / spicy / berry / ripeness-level: under ripe through jammy, raisiny / estery / herbaceous / vegetal / grassy / nutty / minerally? Also think about intensity. Woody: fresh woody, vanilla, caramel, brown sugar, smoky-char,coconut </t>
+  </si>
+  <si>
+    <t>Basic Tastes</t>
+  </si>
+  <si>
+    <t>Retro-Odors</t>
+  </si>
+  <si>
+    <t>Mouthfeel / Body</t>
+  </si>
+  <si>
+    <t>Sweetness, Acidity (sourness), Bitterness (think about balance)</t>
+  </si>
+  <si>
+    <t>Do the retro-nasal odors while on your palate confirm the ortho-nasal odors? Any new odors?</t>
+  </si>
+  <si>
+    <t>The wine's weight (lt. body, medium body, full body) Mouthfeel: smooth or rough, astringent? Hotness from alcohol?</t>
+  </si>
+  <si>
+    <t>4. Feeling</t>
+  </si>
+  <si>
+    <t>Did you like it? How much would you rank it (compare to other similar ones)</t>
+  </si>
+  <si>
+    <t>Blind tasting</t>
+  </si>
+  <si>
+    <t>Tasting without seeing the bottle, and without knowing the price</t>
+  </si>
+  <si>
+    <t>Tears</t>
+  </si>
+  <si>
+    <t>The tears you see from the wine does not mean that the wine is good or bad</t>
+  </si>
+  <si>
+    <t>Tricks for smelling</t>
+  </si>
+  <si>
+    <t>Tricks for looking</t>
+  </si>
+  <si>
+    <t>Put a white background, a paper is good, and a reflection of sun light would be the best</t>
+  </si>
+  <si>
+    <t>Don't wear a perfume, train identifying every flavor to train your nose</t>
+  </si>
+  <si>
+    <t>Find the basic tastes, the retro odors, and identify the mouthfeel (body), and mesure the persistence</t>
+  </si>
+  <si>
+    <t>Persistence</t>
+  </si>
+  <si>
+    <t>Short (under 30 sec), medium (up to a minute), or long finish (a few minutes)</t>
+  </si>
+  <si>
+    <t>Sweet</t>
+  </si>
+  <si>
+    <t>Acidity</t>
+  </si>
+  <si>
+    <t>Tanin</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Lenght</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Typicality</t>
+  </si>
+  <si>
+    <t>What is a bad wine</t>
+  </si>
+  <si>
+    <t>It is the opposite of dry. If you eat a grape and you remove the skin you will find what sweet is. Be careful sweet doesn't mean fruity.</t>
+  </si>
+  <si>
+    <t>The sourness of the wine. In white wine it compensate the sweet taste. It generates saliva in your mouth.</t>
+  </si>
+  <si>
+    <t>The bitterness of the red wine, it comes from the skin. If you eat the skin only of a grape you will find this taste. It generate the dry taste.</t>
+  </si>
+  <si>
+    <t>A wine is balanced if sweet, acidity, tanin, and alcohol are compensating each other</t>
+  </si>
+  <si>
+    <t>The way the wine is doing in your palate</t>
+  </si>
+  <si>
+    <t>The layers of taste and aromas of the wine</t>
+  </si>
+  <si>
+    <t>A wine is complex if it has a good lenght and depth</t>
+  </si>
+  <si>
+    <t>If it taste like a rotten fruit, like vinegar, chemical, oxyde, burnt or cork</t>
+  </si>
+  <si>
+    <t>If the tastes are similar to the other ones of the same race</t>
   </si>
 </sst>
 </file>
@@ -654,10 +809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -698,28 +853,232 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B20" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -785,16 +1144,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
:construction: Cepages are in work in progress
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
     <sheet name="Wine tasting" sheetId="1" r:id="rId2"/>
-    <sheet name="European designations" sheetId="4" r:id="rId3"/>
-    <sheet name="Wine temperature" sheetId="8" r:id="rId4"/>
-    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId5"/>
-    <sheet name="Varieties of designations" sheetId="6" r:id="rId6"/>
-    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId7"/>
+    <sheet name="Nobles varieties" sheetId="11" r:id="rId3"/>
+    <sheet name="European designations" sheetId="4" r:id="rId4"/>
+    <sheet name="Wine temperature" sheetId="8" r:id="rId5"/>
+    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId6"/>
+    <sheet name="Varieties of designations" sheetId="6" r:id="rId7"/>
+    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="133">
   <si>
     <t>Step 1</t>
   </si>
@@ -108,9 +109,6 @@
     <t>Oak barrel</t>
   </si>
   <si>
-    <t>Often use for wine ageing especially for white wine</t>
-  </si>
-  <si>
     <t>Rosé wine</t>
   </si>
   <si>
@@ -325,6 +323,108 @@
   </si>
   <si>
     <t>If the tastes are similar to the other ones of the same race</t>
+  </si>
+  <si>
+    <t>Often use for wine ageing, and for white wine it can also be used during the fermentation</t>
+  </si>
+  <si>
+    <t>Vinifera</t>
+  </si>
+  <si>
+    <t>The type of grapes that can be used to produce wine. There are more than 10 000 varieties.</t>
+  </si>
+  <si>
+    <t>Caracteristics of grapes</t>
+  </si>
+  <si>
+    <t>Colors, aromas, acidity, skin thickness. It makes the wine taste different</t>
+  </si>
+  <si>
+    <t>Caracterestic of vines</t>
+  </si>
+  <si>
+    <t>Density of grapes, quantity of leafs</t>
+  </si>
+  <si>
+    <t>Nobles varieties</t>
+  </si>
+  <si>
+    <t>Varieties that can make a great ranked wine</t>
+  </si>
+  <si>
+    <t>Bourgogne et Champagne</t>
+  </si>
+  <si>
+    <t>Cabernet-Sauvignon et Merlot</t>
+  </si>
+  <si>
+    <t>Bordeaux</t>
+  </si>
+  <si>
+    <t>Syrah</t>
+  </si>
+  <si>
+    <t>Vallée du Rhône</t>
+  </si>
+  <si>
+    <t>Chenin Blanc</t>
+  </si>
+  <si>
+    <t>Vallée de la Loire</t>
+  </si>
+  <si>
+    <t>Nebbiolo</t>
+  </si>
+  <si>
+    <t>Italian Piémont</t>
+  </si>
+  <si>
+    <t>Toscane</t>
+  </si>
+  <si>
+    <t>Sangiovese</t>
+  </si>
+  <si>
+    <t>Riesling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moselle &amp; Rhin in Germany and Alsace </t>
+  </si>
+  <si>
+    <t>Chardonnay et Pinot noir</t>
+  </si>
+  <si>
+    <t>Wood piece</t>
+  </si>
+  <si>
+    <t>Some cheap wines uses wood pieces instead of oak barrel to simulate the wooden taste</t>
+  </si>
+  <si>
+    <t>Chardonnay</t>
+  </si>
+  <si>
+    <t>From the oak: Smoked, Grilled, Nuts, Vanilla; From the grapes: Apple, tropical fruits, ananas; Sometime: Earthy, Minerals, Mushrooms</t>
+  </si>
+  <si>
+    <t>Gewurztraminer</t>
+  </si>
+  <si>
+    <t>Intense color and aromas; Rose and litchi aromas</t>
+  </si>
+  <si>
+    <t>Pinot gris</t>
+  </si>
+  <si>
+    <t>Darker than most of the white wines; Medium body; Low acidity; Neutral aromas of fruits' skin such as peach or orange</t>
+  </si>
+  <si>
+    <t>Light and refreshing; Strong acidity; Aromas of Fruits, flowers and minerals</t>
+  </si>
+  <si>
+    <t>Sauvignon Blanc</t>
+  </si>
+  <si>
+    <t>Very acid, Aromas and flavours: herbal, minerals, grass, fruits such as melon In California it has Oak taste</t>
   </si>
 </sst>
 </file>
@@ -360,8 +460,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -759,47 +862,79 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
         <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -811,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -822,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -830,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -838,7 +973,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -846,239 +981,239 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
         <v>60</v>
-      </c>
-      <c r="B12" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
         <v>80</v>
-      </c>
-      <c r="B18" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
         <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
         <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
         <v>73</v>
-      </c>
-      <c r="B22" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
         <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1088,12 +1223,79 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1124,12 +1326,55 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1144,4 +1389,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
:construction: Work in progress
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -13,8 +13,8 @@
     <sheet name="European designations" sheetId="4" r:id="rId4"/>
     <sheet name="Wine temperature" sheetId="8" r:id="rId5"/>
     <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId6"/>
-    <sheet name="Varieties of designations" sheetId="6" r:id="rId7"/>
-    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId8"/>
+    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId7"/>
+    <sheet name="Varieties of designations" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
   <si>
     <t>Step 1</t>
   </si>
@@ -425,6 +425,57 @@
   </si>
   <si>
     <t>Very acid, Aromas and flavours: herbal, minerals, grass, fruits such as melon In California it has Oak taste</t>
+  </si>
+  <si>
+    <t>Clams, Octopus Salad</t>
+  </si>
+  <si>
+    <t>Vinho Verde Albariño</t>
+  </si>
+  <si>
+    <t>Assyrtiko</t>
+  </si>
+  <si>
+    <t>Good acidity</t>
+  </si>
+  <si>
+    <t>Seafood, fishes</t>
+  </si>
+  <si>
+    <t>Fiano di Avellino</t>
+  </si>
+  <si>
+    <t>Delicate, subtil, with flower flavours</t>
+  </si>
+  <si>
+    <t>Fish, and seafood pastas</t>
+  </si>
+  <si>
+    <t>Greco di Tufo</t>
+  </si>
+  <si>
+    <t>Very fresh, mineral, intense, white flowers and white fruits aromas</t>
+  </si>
+  <si>
+    <t>Shellfishes, Fish with white flesh</t>
+  </si>
+  <si>
+    <t>Grüner Veltliner</t>
+  </si>
+  <si>
+    <t>White pepper, mellifère (nectar plants) aromas</t>
+  </si>
+  <si>
+    <t>White meat, wild game meat</t>
+  </si>
+  <si>
+    <t>Petite arvine</t>
+  </si>
+  <si>
+    <t>Exotic or salin aromas</t>
+  </si>
+  <si>
+    <t>River fishes, Exotic fruits soufflés, Safran ice cream, White truffle risotto</t>
   </si>
 </sst>
 </file>
@@ -1326,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1374,6 +1425,51 @@
         <v>132</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>1410</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1381,12 +1477,63 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
:construction: First list of white varieties added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="172">
   <si>
     <t>Step 1</t>
   </si>
@@ -403,30 +403,15 @@
     <t>Chardonnay</t>
   </si>
   <si>
-    <t>From the oak: Smoked, Grilled, Nuts, Vanilla; From the grapes: Apple, tropical fruits, ananas; Sometime: Earthy, Minerals, Mushrooms</t>
-  </si>
-  <si>
     <t>Gewurztraminer</t>
   </si>
   <si>
-    <t>Intense color and aromas; Rose and litchi aromas</t>
-  </si>
-  <si>
     <t>Pinot gris</t>
   </si>
   <si>
-    <t>Darker than most of the white wines; Medium body; Low acidity; Neutral aromas of fruits' skin such as peach or orange</t>
-  </si>
-  <si>
-    <t>Light and refreshing; Strong acidity; Aromas of Fruits, flowers and minerals</t>
-  </si>
-  <si>
     <t>Sauvignon Blanc</t>
   </si>
   <si>
-    <t>Very acid, Aromas and flavours: herbal, minerals, grass, fruits such as melon In California it has Oak taste</t>
-  </si>
-  <si>
     <t>Clams, Octopus Salad</t>
   </si>
   <si>
@@ -436,46 +421,127 @@
     <t>Assyrtiko</t>
   </si>
   <si>
-    <t>Good acidity</t>
-  </si>
-  <si>
     <t>Seafood, fishes</t>
   </si>
   <si>
     <t>Fiano di Avellino</t>
   </si>
   <si>
-    <t>Delicate, subtil, with flower flavours</t>
-  </si>
-  <si>
     <t>Fish, and seafood pastas</t>
   </si>
   <si>
     <t>Greco di Tufo</t>
   </si>
   <si>
-    <t>Very fresh, mineral, intense, white flowers and white fruits aromas</t>
-  </si>
-  <si>
     <t>Shellfishes, Fish with white flesh</t>
   </si>
   <si>
     <t>Grüner Veltliner</t>
   </si>
   <si>
-    <t>White pepper, mellifère (nectar plants) aromas</t>
-  </si>
-  <si>
     <t>White meat, wild game meat</t>
   </si>
   <si>
     <t>Petite arvine</t>
   </si>
   <si>
-    <t>Exotic or salin aromas</t>
-  </si>
-  <si>
     <t>River fishes, Exotic fruits soufflés, Safran ice cream, White truffle risotto</t>
+  </si>
+  <si>
+    <t>Petit manseng</t>
+  </si>
+  <si>
+    <t>Pinapple or apple desserts with white truffle ice cream</t>
+  </si>
+  <si>
+    <t>Roussane</t>
+  </si>
+  <si>
+    <t>Vermentino</t>
+  </si>
+  <si>
+    <t>Mediterranéean rock fish, Mushroom risotto</t>
+  </si>
+  <si>
+    <t>Viognier</t>
+  </si>
+  <si>
+    <t>Good for aperitif, Oriental dishes with river fishes or foie gras</t>
+  </si>
+  <si>
+    <t>Müller-Thurgau</t>
+  </si>
+  <si>
+    <t>Muscat</t>
+  </si>
+  <si>
+    <t>Pinot blanc</t>
+  </si>
+  <si>
+    <t>Sémillon</t>
+  </si>
+  <si>
+    <t>Trebbiano</t>
+  </si>
+  <si>
+    <t>From the oak: Smoked, Grilled, Nuts, Vanilla; From the grapes: Apple, tropical fruits, ananas; Sometime: Earthy, Minerals, Mushrooms (White wine)</t>
+  </si>
+  <si>
+    <t>Intense color and aromas; Rose and litchi aromas (White wine)</t>
+  </si>
+  <si>
+    <t>Darker than most of the white wines; Medium body; Low acidity; Neutral aromas of fruits' skin such as peach or orange (White wine)</t>
+  </si>
+  <si>
+    <t>Light and refreshing; Strong acidity; Aromas of Fruits, flowers and minerals (White wine)</t>
+  </si>
+  <si>
+    <t>Very acid, Aromas and flavours: herbal, minerals, grass, fruits such as melon In California it has Oak taste (White wine)</t>
+  </si>
+  <si>
+    <t>Good acidity (White wine)</t>
+  </si>
+  <si>
+    <t>Delicate, subtil, with flower flavours (White wine)</t>
+  </si>
+  <si>
+    <t>Very fresh, mineral, intense, white flowers and white fruits aromas (White wine)</t>
+  </si>
+  <si>
+    <t>White pepper, mellifère (nectar plants) aromas (White wine)</t>
+  </si>
+  <si>
+    <t>Exotic or salin aromas (White wine)</t>
+  </si>
+  <si>
+    <t>Sweet but always lively with candied pinapple, vanilla, and white truffle aromas (White wine)</t>
+  </si>
+  <si>
+    <t>Smooth aromas, candied pinapple  (White wine)</t>
+  </si>
+  <si>
+    <t>Floral aromas, Mellifère and a little bit mineral (White wine)</t>
+  </si>
+  <si>
+    <t>Dry apricot aromas, violet, and licorice (White wine)</t>
+  </si>
+  <si>
+    <t>Fresh (White wine)</t>
+  </si>
+  <si>
+    <t>Floral aromas (White wine)</t>
+  </si>
+  <si>
+    <t>Neutral aromas, strong acidity, and low sweetness (White wine)</t>
+  </si>
+  <si>
+    <t>Low acidity, lanolin, and vegetal flavours (White wine)</t>
+  </si>
+  <si>
+    <t>Strong acidity, low level of sweet, neutral taste (White wine)</t>
+  </si>
+  <si>
+    <t>XXXX Red wine below --- Add mention "(Red wine)"</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1343,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1377,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1390,23 +1456,23 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1414,60 +1480,132 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>147</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>1410</v>
+      <c r="B16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1477,60 +1615,84 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: More cards added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="188">
   <si>
     <t>Step 1</t>
   </si>
@@ -542,6 +542,54 @@
   </si>
   <si>
     <t>XXXX Red wine below --- Add mention "(Red wine)"</t>
+  </si>
+  <si>
+    <t>Cabernet-Sauvignon</t>
+  </si>
+  <si>
+    <t>Merlot</t>
+  </si>
+  <si>
+    <t>Pinot Noir</t>
+  </si>
+  <si>
+    <t>Syrah/Shiraz</t>
+  </si>
+  <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>Aglianico</t>
+  </si>
+  <si>
+    <t>Gamay</t>
+  </si>
+  <si>
+    <t>Barbera</t>
+  </si>
+  <si>
+    <t>Cabernet franc</t>
+  </si>
+  <si>
+    <t>Corvina veronese</t>
+  </si>
+  <si>
+    <t>Grenache</t>
+  </si>
+  <si>
+    <t>Malbec</t>
+  </si>
+  <si>
+    <t>Mourvèdre</t>
+  </si>
+  <si>
+    <t>Nerello Mascalese</t>
+  </si>
+  <si>
+    <t>Nero d’Avola</t>
+  </si>
+  <si>
+    <t>Tempranillo</t>
   </si>
 </sst>
 </file>
@@ -1443,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1606,6 +1654,96 @@
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Red wines added to varieties
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="207">
   <si>
     <t>Step 1</t>
   </si>
@@ -590,6 +590,63 @@
   </si>
   <si>
     <t>Tempranillo</t>
+  </si>
+  <si>
+    <t>Hare civet, Truffle risotto</t>
+  </si>
+  <si>
+    <t>Strong tanin taste, strong to medium strenght, cassis aromas, and sometime vegetal aromas, or sometime other fruits; Can age (Red wine)</t>
+  </si>
+  <si>
+    <t>Deep color, deep body, strong level of alcohol and low tanin taste; Plum or chocolate aromas;(Red wine)</t>
+  </si>
+  <si>
+    <t>Strong tanin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
+  </si>
+  <si>
+    <t>Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries and earthy or wooden aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Low to medium acidity; Medium tanin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Dark color; Very robust; Strong tanin level; Aromas: smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
+  </si>
+  <si>
+    <t>Rich wine; High level of alcohol; Medium to high level of tanin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
+  </si>
+  <si>
+    <t>Powerful wines; Can age well (Red wine)</t>
+  </si>
+  <si>
+    <t>Light color; Low tanin; Fruity aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Light wines; Delicates, fruity; Good acidity and low tanin; (Red wine)</t>
+  </si>
+  <si>
+    <t>Elegant tanin structure, nice aromas, very fruity; good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>Powerful aromas and spicy; Sweet (Red wine)</t>
+  </si>
+  <si>
+    <t>Powerful and rich with great fineness (Red wine)</t>
+  </si>
+  <si>
+    <t>Fruits and violet aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Spicy and fruity aromas; Good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>Subtil and delicate; Similar to cabernet franc (Red wine)</t>
+  </si>
+  <si>
+    <t>Strong, structured, robust, pulpy fruits, rich, sappy with bitter almond notes  (Red wine)</t>
+  </si>
+  <si>
+    <t>Kirsch aromas (Red wine)</t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1660,90 +1717,144 @@
       <c r="A23" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="B23" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>173</v>
       </c>
+      <c r="B24" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>115</v>
       </c>
+      <c r="B25" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>174</v>
       </c>
+      <c r="B26" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>118</v>
       </c>
+      <c r="B27" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>175</v>
       </c>
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>176</v>
       </c>
+      <c r="B29" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>177</v>
       </c>
+      <c r="B30" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>178</v>
       </c>
+      <c r="B31" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>187</v>
+      </c>
+      <c r="B40" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1753,10 +1864,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1831,6 +1942,14 @@
       </c>
       <c r="B9" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Part about designation compelted
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
     <sheet name="Wine tasting" sheetId="1" r:id="rId2"/>
     <sheet name="Nobles varieties" sheetId="11" r:id="rId3"/>
-    <sheet name="European designations" sheetId="4" r:id="rId4"/>
-    <sheet name="Wine temperature" sheetId="8" r:id="rId5"/>
-    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId6"/>
-    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId7"/>
-    <sheet name="Varieties of designations" sheetId="6" r:id="rId8"/>
+    <sheet name="Wine &amp; naming convention" sheetId="12" r:id="rId4"/>
+    <sheet name="European design. &amp; varieties" sheetId="4" r:id="rId5"/>
+    <sheet name="Wine Storage &amp; Service" sheetId="8" r:id="rId6"/>
+    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId7"/>
+    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId8"/>
+    <sheet name="Varieties of designations" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="262">
   <si>
     <t>Step 1</t>
   </si>
@@ -541,9 +542,6 @@
     <t>Strong acidity, low level of sweet, neutral taste (White wine)</t>
   </si>
   <si>
-    <t>XXXX Red wine below --- Add mention "(Red wine)"</t>
-  </si>
-  <si>
     <t>Cabernet-Sauvignon</t>
   </si>
   <si>
@@ -647,6 +645,174 @@
   </si>
   <si>
     <t>Kirsch aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>AOP / PDO</t>
+  </si>
+  <si>
+    <t>Protected Designation of Origin - Geographic areas, where the wine can be produced with very specific quantities of varieties</t>
+  </si>
+  <si>
+    <t>IGP / PGI</t>
+  </si>
+  <si>
+    <t>Protected Geographical Indication - Like AOP / PDO with more flexibility</t>
+  </si>
+  <si>
+    <t>Country wine</t>
+  </si>
+  <si>
+    <t>Wine produced in the country</t>
+  </si>
+  <si>
+    <t>Table wine</t>
+  </si>
+  <si>
+    <t>Wine mixing varieties coming from different countries</t>
+  </si>
+  <si>
+    <t>Wine of variety</t>
+  </si>
+  <si>
+    <t>Wine of designation</t>
+  </si>
+  <si>
+    <t>Old world wine</t>
+  </si>
+  <si>
+    <t>New world wine</t>
+  </si>
+  <si>
+    <t>Wine made in europe and the mediterranean basin; They discovered the wine first;</t>
+  </si>
+  <si>
+    <t>Wine made in countried than are not from Europe / Mediterranean basin such as America (North and South), Australia, South Africa</t>
+  </si>
+  <si>
+    <t>Wine of one variety only such as Merlot or Chardonnay, this naming is usually used in the New World</t>
+  </si>
+  <si>
+    <t>Wine of many varieties, its name come from a designation, for example Bordeaux or Bourgogne, it comes from it's region and the varieties are defined by national rules</t>
+  </si>
+  <si>
+    <t>Riesling, Gewurztraminer, Pinot gris et noir</t>
+  </si>
+  <si>
+    <t>Corvina, Molinara, Rondinella</t>
+  </si>
+  <si>
+    <t>Sangiovese (80 % minimum)</t>
+  </si>
+  <si>
+    <t>Alsace, France</t>
+  </si>
+  <si>
+    <t>Bardolino, Italy</t>
+  </si>
+  <si>
+    <t>Beaujolais (Red), France</t>
+  </si>
+  <si>
+    <t>Bordeaux (Red), France</t>
+  </si>
+  <si>
+    <t>Bordeaux sec (White), France</t>
+  </si>
+  <si>
+    <t>Bourgogne (Red), France</t>
+  </si>
+  <si>
+    <t>Bourgogne (White), France</t>
+  </si>
+  <si>
+    <t>Chablis, France</t>
+  </si>
+  <si>
+    <t>Champagne, France</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape, France</t>
+  </si>
+  <si>
+    <t>Chianti, Italy</t>
+  </si>
+  <si>
+    <t>Grenache, Mourvèdre, Syrah and others</t>
+  </si>
+  <si>
+    <t>Chardonnay, Pinot Noir, Pinot Meunier</t>
+  </si>
+  <si>
+    <t>Sauvignon Blanc, Sémillon, Muscadelle</t>
+  </si>
+  <si>
+    <t>Cabernet-Sauvignon, Merlot, Cabernet-Franc</t>
+  </si>
+  <si>
+    <t>Palomino</t>
+  </si>
+  <si>
+    <t>Garganega et autres</t>
+  </si>
+  <si>
+    <t>Sémillon, Sauvignon Blanc, Muscadelle</t>
+  </si>
+  <si>
+    <t>Tempranillo, Grenache et autres</t>
+  </si>
+  <si>
+    <t>Riesling and others</t>
+  </si>
+  <si>
+    <t>Touriga Nacional, Tinta Barroca, Touriga Francesa, Tinta Roriz, Tinto Cão and others</t>
+  </si>
+  <si>
+    <t>Grenache, Mourvèdre, Carignan and others</t>
+  </si>
+  <si>
+    <t>Côtes du Rhône méridionnaux, France</t>
+  </si>
+  <si>
+    <t>Côtes du Rhône septentrionnaux, France</t>
+  </si>
+  <si>
+    <t>Porto, Portugal</t>
+  </si>
+  <si>
+    <t>Pouilly-Fuissé, France</t>
+  </si>
+  <si>
+    <t>Rhin (Rheingau, Rheinhessen), Germany</t>
+  </si>
+  <si>
+    <t>Rioja (Red), Spain</t>
+  </si>
+  <si>
+    <t>Sancerre, France</t>
+  </si>
+  <si>
+    <t>Sauternes, France</t>
+  </si>
+  <si>
+    <t>Sherry (Jerez), Spain</t>
+  </si>
+  <si>
+    <t>Soave, Italy</t>
+  </si>
+  <si>
+    <t>Valpolicella, Italy</t>
+  </si>
+  <si>
+    <t>Geographical denomination levels</t>
+  </si>
+  <si>
+    <t>Country; Region ; District; Sub-district; Common; Vineyard or plot.</t>
+  </si>
+  <si>
+    <t>Storage direction</t>
+  </si>
+  <si>
+    <t>Bottles should be kept lying flat to maintain the cork in contact with the wine in order to prevent drying out.</t>
   </si>
 </sst>
 </file>
@@ -970,7 +1136,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1524,34 +1690,312 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>255</v>
+      </c>
+      <c r="B20" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1708,153 +2152,148 @@
         <v>170</v>
       </c>
     </row>
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>115</v>
+      </c>
+      <c r="B22" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="1" t="s">
-        <v>172</v>
+      <c r="A23" t="s">
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B28" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>185</v>
-      </c>
-      <c r="B38" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>186</v>
-      </c>
-      <c r="B39" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>187</v>
-      </c>
-      <c r="B40" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1862,7 +2301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -1946,10 +2385,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1957,7 +2396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
:construction: Storage information added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="288">
   <si>
     <t>Step 1</t>
   </si>
@@ -813,6 +813,84 @@
   </si>
   <si>
     <t>Bottles should be kept lying flat to maintain the cork in contact with the wine in order to prevent drying out.</t>
+  </si>
+  <si>
+    <t>The more the wine is young and has a lot of tanin the longer it should be airy; In general 1 hour is enough; The older it is the more careful you should be;</t>
+  </si>
+  <si>
+    <t>If the wine is dark you can give it some air; If it's brick red or grenat, it reached maturity so no need of aeration</t>
+  </si>
+  <si>
+    <t>Wine aeration (Red)</t>
+  </si>
+  <si>
+    <t>Wine aeration and colors (Red)</t>
+  </si>
+  <si>
+    <t>Wine aeration (White)</t>
+  </si>
+  <si>
+    <t>Aeration can be good for good white wines such as White Bordeaux, White Bourgogne, or the best wines from Alsace</t>
+  </si>
+  <si>
+    <t>Wine aeration (Fortified wine)</t>
+  </si>
+  <si>
+    <t>Fortified wines need at least 8 hours of aeration; For old porto 4 hours is needed</t>
+  </si>
+  <si>
+    <t>Wine aeration for wine with low level of tanin</t>
+  </si>
+  <si>
+    <t>No need of long period of aeration for wine with a medium body and low level of tanin such as Pinot noir, Beaujolais, some Côte du Rhône, Dolcetto Barbera, light Chianti, Zinfandel red</t>
+  </si>
+  <si>
+    <t>Wine aeration for cheap wine</t>
+  </si>
+  <si>
+    <t>For the wine cheaper than 5 € there is no need of aeration usually because there is a low level of tanin</t>
+  </si>
+  <si>
+    <t>Great white wine temperature</t>
+  </si>
+  <si>
+    <t>Simple white wine temperature</t>
+  </si>
+  <si>
+    <t>Rosé wine temperature</t>
+  </si>
+  <si>
+    <t>Sweet wine temperature</t>
+  </si>
+  <si>
+    <t>Dessert wine temperature</t>
+  </si>
+  <si>
+    <t>Champagne temperature</t>
+  </si>
+  <si>
+    <t>Red wine temperature</t>
+  </si>
+  <si>
+    <t>16 - 18 ° C</t>
+  </si>
+  <si>
+    <t>14 - 16 ° C</t>
+  </si>
+  <si>
+    <t>9 - 13 ° C</t>
+  </si>
+  <si>
+    <t>10 - 12 ° C</t>
+  </si>
+  <si>
+    <t>9 - 12 ° C</t>
+  </si>
+  <si>
+    <t>14 - 16 ° C (Sauterne); 16 - 18 ° C (Porto)</t>
+  </si>
+  <si>
+    <t>8 ° C</t>
   </si>
 </sst>
 </file>
@@ -1969,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1983,6 +2061,110 @@
       </c>
       <c r="B1" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: More information added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="312">
   <si>
     <t>Step 1</t>
   </si>
@@ -891,6 +891,78 @@
   </si>
   <si>
     <t>8 ° C</t>
+  </si>
+  <si>
+    <t>Bottle's label mandatory information</t>
+  </si>
+  <si>
+    <t>Denomination; Origin; Alcohol percentage; Bottler identity (or importer); Volume; Lot number; Pregnancy avertissement; Allergen information</t>
+  </si>
+  <si>
+    <t>PDO equivalent in France</t>
+  </si>
+  <si>
+    <t>AOC - Appellation d’origine contrôlée</t>
+  </si>
+  <si>
+    <t>VDQS - Vin délimité de qualité supérieure.</t>
+  </si>
+  <si>
+    <t>PDO equivalent in Italy</t>
+  </si>
+  <si>
+    <t>PGI equivalent in France</t>
+  </si>
+  <si>
+    <t>PGI equivalent in Italy</t>
+  </si>
+  <si>
+    <t>DOC -  Denominazione di Origine Controllata</t>
+  </si>
+  <si>
+    <t>DOCG - Denominazione di Origine Controllata e Garantita</t>
+  </si>
+  <si>
+    <t>PDO equivalent in Spain</t>
+  </si>
+  <si>
+    <t>PGI equivalent in Spain</t>
+  </si>
+  <si>
+    <t>DO - Denominaciòn de Origen</t>
+  </si>
+  <si>
+    <t>DOCa - Denominaciòn d’Origen Calificada</t>
+  </si>
+  <si>
+    <t>PDO equivalent in Portugal</t>
+  </si>
+  <si>
+    <t>PDO equivalent in Germany</t>
+  </si>
+  <si>
+    <t>DOC - Denominação de Origem Controlada</t>
+  </si>
+  <si>
+    <t>QBA - Qualitätswein bestimmter Anbaugebiete</t>
+  </si>
+  <si>
+    <t>Millésime</t>
+  </si>
+  <si>
+    <t>A wine can have a millesime mention if 95% of the grapes come from the same year in USA, and 85% in Europe</t>
+  </si>
+  <si>
+    <t>Tasting order</t>
+  </si>
+  <si>
+    <t>If you taste different wine, here is the recommended order: 1. Sparkling wine; 2. White wine, rosés; 3. Young red; 4. Strong white or sweet wine; 5. Strong red wine; 6. Fortified wine</t>
+  </si>
+  <si>
+    <t>Spitting</t>
+  </si>
+  <si>
+    <t>Spitting is recommended to stay fully lucid while tasting different wine</t>
   </si>
 </sst>
 </file>
@@ -1410,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1612,74 +1684,90 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>310</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
         <v>89</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>308</v>
+      </c>
+      <c r="B35" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1768,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1846,6 +1934,86 @@
       </c>
       <c r="B9" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>290</v>
+      </c>
+      <c r="B11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+      <c r="B12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>293</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>299</v>
+      </c>
+      <c r="B16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B19" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2049,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
:construction: Some varieties added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="318">
   <si>
     <t>Step 1</t>
   </si>
@@ -488,15 +488,9 @@
     <t>From the oak: Smoked, Grilled, Nuts, Vanilla; From the grapes: Apple, tropical fruits, ananas; Sometime: Earthy, Minerals, Mushrooms (White wine)</t>
   </si>
   <si>
-    <t>Intense color and aromas; Rose and litchi aromas (White wine)</t>
-  </si>
-  <si>
     <t>Darker than most of the white wines; Medium body; Low acidity; Neutral aromas of fruits' skin such as peach or orange (White wine)</t>
   </si>
   <si>
-    <t>Light and refreshing; Strong acidity; Aromas of Fruits, flowers and minerals (White wine)</t>
-  </si>
-  <si>
     <t>Very acid, Aromas and flavours: herbal, minerals, grass, fruits such as melon In California it has Oak taste (White wine)</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>Floral aromas, Mellifère and a little bit mineral (White wine)</t>
   </si>
   <si>
-    <t>Dry apricot aromas, violet, and licorice (White wine)</t>
-  </si>
-  <si>
     <t>Fresh (White wine)</t>
   </si>
   <si>
@@ -536,9 +527,6 @@
     <t>Neutral aromas, strong acidity, and low sweetness (White wine)</t>
   </si>
   <si>
-    <t>Low acidity, lanolin, and vegetal flavours (White wine)</t>
-  </si>
-  <si>
     <t>Strong acidity, low level of sweet, neutral taste (White wine)</t>
   </si>
   <si>
@@ -593,45 +581,24 @@
     <t>Hare civet, Truffle risotto</t>
   </si>
   <si>
-    <t>Strong tanin taste, strong to medium strenght, cassis aromas, and sometime vegetal aromas, or sometime other fruits; Can age (Red wine)</t>
-  </si>
-  <si>
-    <t>Deep color, deep body, strong level of alcohol and low tanin taste; Plum or chocolate aromas;(Red wine)</t>
-  </si>
-  <si>
     <t>Strong tanin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
   </si>
   <si>
-    <t>Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries and earthy or wooden aromas (Red wine)</t>
-  </si>
-  <si>
     <t>Low to medium acidity; Medium tanin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
   </si>
   <si>
-    <t>Dark color; Very robust; Strong tanin level; Aromas: smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
-  </si>
-  <si>
     <t>Rich wine; High level of alcohol; Medium to high level of tanin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
   </si>
   <si>
     <t>Powerful wines; Can age well (Red wine)</t>
   </si>
   <si>
-    <t>Light color; Low tanin; Fruity aromas (Red wine)</t>
-  </si>
-  <si>
     <t>Light wines; Delicates, fruity; Good acidity and low tanin; (Red wine)</t>
   </si>
   <si>
-    <t>Elegant tanin structure, nice aromas, very fruity; good ageing capacity (Red wine)</t>
-  </si>
-  <si>
     <t>Powerful aromas and spicy; Sweet (Red wine)</t>
   </si>
   <si>
-    <t>Powerful and rich with great fineness (Red wine)</t>
-  </si>
-  <si>
     <t>Fruits and violet aromas (Red wine)</t>
   </si>
   <si>
@@ -963,6 +930,57 @@
   </si>
   <si>
     <t>Spitting is recommended to stay fully lucid while tasting different wine</t>
+  </si>
+  <si>
+    <t>Aligoté</t>
+  </si>
+  <si>
+    <t>To drink young; Fresh, fruity</t>
+  </si>
+  <si>
+    <t>Marsanne</t>
+  </si>
+  <si>
+    <t>Makes dry wines; Floral with cloves notes</t>
+  </si>
+  <si>
+    <t>Light and refreshing; Strong acidity; Aromas of Fruits: lemon, grapefruit, peach, apple, lime, lemongrass; flowers and minerals (White wine)</t>
+  </si>
+  <si>
+    <t>Intense color and aromas; Rose, litchi, cinnamon, pepper aromas (White wine)</t>
+  </si>
+  <si>
+    <t>Low acidity, lanolin, citrus, honey and vegetal flavours (White wine)</t>
+  </si>
+  <si>
+    <t>Dry apricot aromas, violet, musc, tobacco, and licorice (White wine)</t>
+  </si>
+  <si>
+    <t>Elegant tanin structure, nice aromas, very fruity: cassis, currant), violet, vegetal; good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>Strong tanin taste, strong to medium strenght, cassis aromas, and sometime vegetal aromas, violet, or sometime other fruits; Can age (Red wine)</t>
+  </si>
+  <si>
+    <t>Cinsault</t>
+  </si>
+  <si>
+    <t>Strong wine, age fast, floral aromas</t>
+  </si>
+  <si>
+    <t>Light color; Low tanin; Red fruits aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
+  </si>
+  <si>
+    <t>Deep color, deep body, strong level of alcohol and low tanin taste; Red fruits, Plum, chocolate or mushrooms aromas;(Red wine)</t>
+  </si>
+  <si>
+    <t>Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries, cherry and earthy or wooden aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Dark color; Very robust; Strong tanin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1684,10 +1702,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B25" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1764,10 +1782,10 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B35" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1866,154 +1884,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B12" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B13" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B14" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B15" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="B17" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="B18" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B19" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2034,55 +2052,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" t="s">
         <v>228</v>
-      </c>
-      <c r="B4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
         <v>124</v>
@@ -2090,7 +2108,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
         <v>124</v>
@@ -2098,39 +2116,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
@@ -2138,15 +2156,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B15" t="s">
         <v>124</v>
@@ -2154,23 +2172,23 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B16" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B18" t="s">
         <v>127</v>
@@ -2178,34 +2196,34 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B20" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B21" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2225,114 +2243,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="B1" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B14" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2342,10 +2360,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2363,7 +2381,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2371,7 +2389,7 @@
         <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2379,7 +2397,7 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2387,7 +2405,7 @@
         <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2395,7 +2413,7 @@
         <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2403,7 +2421,7 @@
         <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2411,7 +2429,7 @@
         <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2419,7 +2437,7 @@
         <v>136</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2427,7 +2445,7 @@
         <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2435,7 +2453,7 @@
         <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2443,7 +2461,7 @@
         <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2451,7 +2469,7 @@
         <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2459,7 +2477,7 @@
         <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2467,7 +2485,7 @@
         <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2475,7 +2493,7 @@
         <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2483,7 +2501,7 @@
         <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2491,7 +2509,7 @@
         <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2499,23 +2517,23 @@
         <v>151</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2523,15 +2541,15 @@
         <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>191</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2539,111 +2557,135 @@
         <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>193</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B27" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>196</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>198</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B35" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B36" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>301</v>
+      </c>
+      <c r="B38" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>303</v>
+      </c>
+      <c r="B39" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>311</v>
+      </c>
+      <c r="B40" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -2735,10 +2777,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: French appelation added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="343">
   <si>
     <t>Step 1</t>
   </si>
@@ -662,24 +662,15 @@
     <t>Wine of many varieties, its name come from a designation, for example Bordeaux or Bourgogne, it comes from it's region and the varieties are defined by national rules</t>
   </si>
   <si>
-    <t>Riesling, Gewurztraminer, Pinot gris et noir</t>
-  </si>
-  <si>
     <t>Corvina, Molinara, Rondinella</t>
   </si>
   <si>
     <t>Sangiovese (80 % minimum)</t>
   </si>
   <si>
-    <t>Alsace, France</t>
-  </si>
-  <si>
     <t>Bardolino, Italy</t>
   </si>
   <si>
-    <t>Beaujolais (Red), France</t>
-  </si>
-  <si>
     <t>Bordeaux (Red), France</t>
   </si>
   <si>
@@ -713,9 +704,6 @@
     <t>Sauvignon Blanc, Sémillon, Muscadelle</t>
   </si>
   <si>
-    <t>Cabernet-Sauvignon, Merlot, Cabernet-Franc</t>
-  </si>
-  <si>
     <t>Palomino</t>
   </si>
   <si>
@@ -737,12 +725,6 @@
     <t>Grenache, Mourvèdre, Carignan and others</t>
   </si>
   <si>
-    <t>Côtes du Rhône méridionnaux, France</t>
-  </si>
-  <si>
-    <t>Côtes du Rhône septentrionnaux, France</t>
-  </si>
-  <si>
     <t>Porto, Portugal</t>
   </si>
   <si>
@@ -755,9 +737,6 @@
     <t>Rioja (Red), Spain</t>
   </si>
   <si>
-    <t>Sancerre, France</t>
-  </si>
-  <si>
     <t>Sauternes, France</t>
   </si>
   <si>
@@ -981,6 +960,102 @@
   </si>
   <si>
     <t>Dark color; Very robust; Strong tanin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
+  </si>
+  <si>
+    <t>Merlot, Cabernet-Sauvignon, Cabernet-Franc, Malbec, Petit Verdot</t>
+  </si>
+  <si>
+    <t>Beaujolais (White), France</t>
+  </si>
+  <si>
+    <t>Grenache blanc, Grenache Gris, Clairette</t>
+  </si>
+  <si>
+    <t>Grenache, Cinsaut, Syrah, Mourvèdre…</t>
+  </si>
+  <si>
+    <t>Beaujolais (Red), Bourgogne, France</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape (White), Rhône, France</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape (Red), Rhône, France</t>
+  </si>
+  <si>
+    <t>Hermitage (Red), Rhône, France</t>
+  </si>
+  <si>
+    <t>Hermitage (White), Rhône, France</t>
+  </si>
+  <si>
+    <t>Côte rotie (Red), Rhône, France</t>
+  </si>
+  <si>
+    <t>Condrieu (White), Rhône, France</t>
+  </si>
+  <si>
+    <t>Côtes du Rhône méridionnaux, Rhône, France</t>
+  </si>
+  <si>
+    <t>Côtes du Rhône septentrionnaux, Rhône, France</t>
+  </si>
+  <si>
+    <t>Côte du Rhône (White), Rhône, France</t>
+  </si>
+  <si>
+    <t>Côte du Rhône (Red), Rhône, France</t>
+  </si>
+  <si>
+    <t>Sancerre, Menetou-Salon (Red), Loire, France</t>
+  </si>
+  <si>
+    <t>Sancerre, Menetou-Salon (White), Loire, France</t>
+  </si>
+  <si>
+    <t>Pouilly-Fumé (White), Loire, France</t>
+  </si>
+  <si>
+    <t>Vouvray, Montlouis (White), Loire, France</t>
+  </si>
+  <si>
+    <t>Muscadet (White), Loire, France</t>
+  </si>
+  <si>
+    <t>Alsace (White), France</t>
+  </si>
+  <si>
+    <t>Alsace (Red), France</t>
+  </si>
+  <si>
+    <t>Languedoc-Roussillon (White), France</t>
+  </si>
+  <si>
+    <t>Languedoc-Roussillon (Red), France</t>
+  </si>
+  <si>
+    <t>Marsanne, Roussanne</t>
+  </si>
+  <si>
+    <t>Syrah, Viognier</t>
+  </si>
+  <si>
+    <t>Marsanne, Roussanne, Bourboulenc, Clairette, Grenache Blanc, Viognier</t>
+  </si>
+  <si>
+    <t>Grenache, Syrah, Mourvèdre, Cinsaut, Carignan</t>
+  </si>
+  <si>
+    <t>Melon de Bourgogne</t>
+  </si>
+  <si>
+    <t>Riesling, Gewurztraminer, Pinot Blanc, Pinot Gris, Sylvaner</t>
+  </si>
+  <si>
+    <t>Vermentino (ou Rolle), Piquepoul, Clairette, Bourboulenc, Grenache blanc, Grenache Gris, Marsanne, Roussanne, Macabeu, Viognier</t>
+  </si>
+  <si>
+    <t>Syrah, Carignan, Grenache, Mourvèdre, Cinsaut</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1777,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B25" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -1782,10 +1857,10 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B35" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -1948,90 +2023,90 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B12" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B15" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B16" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B17" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B18" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B19" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2042,17 +2117,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" t="s">
         <v>211</v>
@@ -2060,15 +2135,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>312</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>315</v>
       </c>
       <c r="B3" t="s">
         <v>173</v>
@@ -2076,23 +2151,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
         <v>169</v>
@@ -2100,7 +2175,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>124</v>
@@ -2108,7 +2183,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B8" t="s">
         <v>124</v>
@@ -2116,39 +2191,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>322</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>323</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
@@ -2156,15 +2231,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B15" t="s">
         <v>124</v>
@@ -2172,58 +2247,186 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s">
-        <v>127</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B19" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>246</v>
+        <v>316</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B23" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>319</v>
+      </c>
+      <c r="B24" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>318</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>320</v>
+      </c>
+      <c r="B26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>321</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>324</v>
+      </c>
+      <c r="B28" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>325</v>
+      </c>
+      <c r="B29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>327</v>
+      </c>
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>326</v>
+      </c>
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>329</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>330</v>
+      </c>
+      <c r="B34" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>331</v>
+      </c>
+      <c r="B35" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>332</v>
+      </c>
+      <c r="B36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>333</v>
+      </c>
+      <c r="B37" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>334</v>
+      </c>
+      <c r="B38" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2243,114 +2446,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B8" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B13" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B14" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -2362,8 +2565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2381,7 +2584,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2397,7 +2600,7 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2477,7 +2680,7 @@
         <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2509,7 +2712,7 @@
         <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2525,7 +2728,7 @@
         <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2533,7 +2736,7 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2549,7 +2752,7 @@
         <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2565,7 +2768,7 @@
         <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2589,7 +2792,7 @@
         <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2605,7 +2808,7 @@
         <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2621,7 +2824,7 @@
         <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2666,26 +2869,26 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B38" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B39" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="B40" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: More regions added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="348">
   <si>
     <t>Step 1</t>
   </si>
@@ -1056,6 +1056,21 @@
   </si>
   <si>
     <t>Syrah, Carignan, Grenache, Mourvèdre, Cinsaut</t>
+  </si>
+  <si>
+    <t>Bordeaux (Red)</t>
+  </si>
+  <si>
+    <t>Lamb, game meat, beef, roasted, grilled, stewed; when tanin are round it goes well with chocolate desserts, brownies</t>
+  </si>
+  <si>
+    <t>Mâcon (Red), Bourgogne, France</t>
+  </si>
+  <si>
+    <t>Mâcon (White), Bourgogne, France</t>
+  </si>
+  <si>
+    <t>Gamay, Pinot noir</t>
   </si>
 </sst>
 </file>
@@ -2117,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2427,6 +2442,22 @@
       </c>
       <c r="B38" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>345</v>
+      </c>
+      <c r="B39" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>346</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2898,10 +2929,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2984,6 +3015,14 @@
       </c>
       <c r="B10" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Italien denomination added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -12,10 +12,11 @@
     <sheet name="Nobles varieties" sheetId="11" r:id="rId3"/>
     <sheet name="Wine &amp; naming convention" sheetId="12" r:id="rId4"/>
     <sheet name="European design. &amp; varieties" sheetId="4" r:id="rId5"/>
-    <sheet name="Wine Storage &amp; Service" sheetId="8" r:id="rId6"/>
-    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId7"/>
-    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId8"/>
-    <sheet name="Varieties of designations" sheetId="6" r:id="rId9"/>
+    <sheet name="Wine to discover (todo)" sheetId="13" r:id="rId6"/>
+    <sheet name="Wine Storage &amp; Service" sheetId="8" r:id="rId7"/>
+    <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId8"/>
+    <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId9"/>
+    <sheet name="Varieties of designations" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="375">
   <si>
     <t>Step 1</t>
   </si>
@@ -1071,6 +1072,87 @@
   </si>
   <si>
     <t>Gamay, Pinot noir</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Kindle</t>
+  </si>
+  <si>
+    <t>Region / Appellation</t>
+  </si>
+  <si>
+    <t>Gavi, Piedmont (White)</t>
+  </si>
+  <si>
+    <t>Gattinara (Red), Piedmont, Italy</t>
+  </si>
+  <si>
+    <t>Barbaresco (Red), Piedmont, Italy</t>
+  </si>
+  <si>
+    <t>Barolo (Red), Piedmont, Italy</t>
+  </si>
+  <si>
+    <t>Roero arneis (White), Piedmont, Italy</t>
+  </si>
+  <si>
+    <t>Nebbiolo, Bonarda</t>
+  </si>
+  <si>
+    <t>Cortese</t>
+  </si>
+  <si>
+    <t>Arneis</t>
+  </si>
+  <si>
+    <t>Chianti, Chianti classico (Red), Tuscany, Italy</t>
+  </si>
+  <si>
+    <t>Brunello di Montalcino (Red), Tuscany, Italy</t>
+  </si>
+  <si>
+    <t>Vernaccia di San Gimignano (White), Tuscany, Italy</t>
+  </si>
+  <si>
+    <t>Vino noble di Montepulciano (Red), Tuscany, Italy</t>
+  </si>
+  <si>
+    <t>Carmignano (Red), Tuscany, Italy</t>
+  </si>
+  <si>
+    <t>Super-toscans (Red), Tuscany, Italy</t>
+  </si>
+  <si>
+    <t>Soave (White), Veneto, Italy</t>
+  </si>
+  <si>
+    <t>Amarone (Red), Veneto, Italy</t>
+  </si>
+  <si>
+    <t>Bianco di Custoza (White), Veneto, Italy</t>
+  </si>
+  <si>
+    <t>Luagana (White), Veneto, Italy</t>
+  </si>
+  <si>
+    <t>Sangiovese, Canaiolo and others</t>
+  </si>
+  <si>
+    <t>Vernaccia</t>
+  </si>
+  <si>
+    <t>Sangiovese, Cabernet Sauvignon, Canaiolo and others</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cabernet Sauvignon, Sangiovese, and others</t>
+  </si>
+  <si>
+    <t>Garganega, Trebbiano et autres</t>
+  </si>
+  <si>
+    <t>Trebbiano, Garganega, Tocai</t>
   </si>
 </sst>
 </file>
@@ -1588,6 +1670,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
@@ -2132,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2460,12 +2554,161 @@
         <v>124</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>354</v>
+      </c>
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>353</v>
+      </c>
+      <c r="B42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>352</v>
+      </c>
+      <c r="B43" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>351</v>
+      </c>
+      <c r="B44" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>355</v>
+      </c>
+      <c r="B45" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>359</v>
+      </c>
+      <c r="B46" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>360</v>
+      </c>
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>361</v>
+      </c>
+      <c r="B48" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>362</v>
+      </c>
+      <c r="B49" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>363</v>
+      </c>
+      <c r="B50" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>364</v>
+      </c>
+      <c r="B51" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>365</v>
+      </c>
+      <c r="B52" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>366</v>
+      </c>
+      <c r="B53" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>367</v>
+      </c>
+      <c r="B54" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>368</v>
+      </c>
+      <c r="B55" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1">
+        <v>4981</v>
+      </c>
+      <c r="C1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2592,7 +2835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -2927,7 +3170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -3028,16 +3271,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
:construction: Italian wines added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="379">
   <si>
     <t>Step 1</t>
   </si>
@@ -1153,6 +1153,18 @@
   </si>
   <si>
     <t>Trebbiano, Garganega, Tocai</t>
+  </si>
+  <si>
+    <t>Lombardie (Red), Valtellina, Italy</t>
+  </si>
+  <si>
+    <t>Latium (White)</t>
+  </si>
+  <si>
+    <t>Frascati</t>
+  </si>
+  <si>
+    <t>White wines</t>
   </si>
 </sst>
 </file>
@@ -2226,10 +2238,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2674,6 +2686,22 @@
         <v>151</v>
       </c>
     </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>375</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>376</v>
+      </c>
+      <c r="B57" t="s">
+        <v>377</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2681,9 +2709,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2700,6 +2728,20 @@
         <v>349</v>
       </c>
       <c r="D1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2">
+        <v>5357</v>
+      </c>
+      <c r="C2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" t="s">
         <v>350</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:construction: Spanish wines added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="391">
   <si>
     <t>Step 1</t>
   </si>
@@ -1165,6 +1165,42 @@
   </si>
   <si>
     <t>White wines</t>
+  </si>
+  <si>
+    <t>Ribera-del-duero (Red), Spain</t>
+  </si>
+  <si>
+    <t>Tempranillo, Cabernet Sauvignon</t>
+  </si>
+  <si>
+    <t>Penedès, Spain</t>
+  </si>
+  <si>
+    <t>Grenache, Syrah, Monastrell, Merlot, Pinot Noir, Cabernet Sauvignon, Samsó, Ull de Llebre</t>
+  </si>
+  <si>
+    <t>Tempranillo, Grenache, Cabernet sauvignon, Merlot</t>
+  </si>
+  <si>
+    <t>Navarra (Red), Spain</t>
+  </si>
+  <si>
+    <t>Rueda (White), Spain</t>
+  </si>
+  <si>
+    <t>Verdejo</t>
+  </si>
+  <si>
+    <t>Rías Baixas, Spain</t>
+  </si>
+  <si>
+    <t>Albariño</t>
+  </si>
+  <si>
+    <t>Barca Velha (Red), Portugal</t>
+  </si>
+  <si>
+    <t>Touriga Franca, Touriga Nacional,Tinta Roriz, Tinto Cão</t>
   </si>
 </sst>
 </file>
@@ -2238,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2700,6 +2736,54 @@
       </c>
       <c r="B57" t="s">
         <v>377</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>379</v>
+      </c>
+      <c r="B58" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>381</v>
+      </c>
+      <c r="B59" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>384</v>
+      </c>
+      <c r="B60" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>385</v>
+      </c>
+      <c r="B61" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>387</v>
+      </c>
+      <c r="B62" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>389</v>
+      </c>
+      <c r="B63" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Germany added to the cepage names
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="398">
   <si>
     <t>Step 1</t>
   </si>
@@ -1201,6 +1201,27 @@
   </si>
   <si>
     <t>Touriga Franca, Touriga Nacional,Tinta Roriz, Tinto Cão</t>
+  </si>
+  <si>
+    <t>Mosel-Saar-Ruwer (White), Germany</t>
+  </si>
+  <si>
+    <t>Rheingau (White), Germany</t>
+  </si>
+  <si>
+    <t>Riesling, Pinot noir</t>
+  </si>
+  <si>
+    <t>Müller-Thurgau, Sylvaner</t>
+  </si>
+  <si>
+    <t>Rheinhessen, Germany</t>
+  </si>
+  <si>
+    <t>Pfalz, Germany</t>
+  </si>
+  <si>
+    <t>Müller-Thurgau, Riesling, Sylvaner, Kerner, Scheurebe and Spätburgunder (Pinot Noir)</t>
   </si>
 </sst>
 </file>
@@ -2274,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:A66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2784,6 +2805,38 @@
       </c>
       <c r="B63" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>391</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>392</v>
+      </c>
+      <c r="B65" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>395</v>
+      </c>
+      <c r="B66" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>396</v>
+      </c>
+      <c r="B67" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Flash cards updated
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
     <sheet name="Wine tasting" sheetId="1" r:id="rId2"/>
     <sheet name="Nobles varieties" sheetId="11" r:id="rId3"/>
     <sheet name="Wine &amp; naming convention" sheetId="12" r:id="rId4"/>
-    <sheet name="European design. &amp; varieties" sheetId="4" r:id="rId5"/>
+    <sheet name="Varieties of designations" sheetId="4" r:id="rId5"/>
     <sheet name="Wine to discover (todo)" sheetId="13" r:id="rId6"/>
     <sheet name="Wine Storage &amp; Service" sheetId="8" r:id="rId7"/>
     <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId8"/>
     <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId9"/>
-    <sheet name="Varieties of designations" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1739,25 +1738,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2050,9 +2035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2129,8 +2112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2297,9 +2280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2848,9 +2829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>

</xml_diff>

<commit_message>
:construction: Food wine pairing added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="491">
   <si>
     <t>Step 1</t>
   </si>
@@ -662,6 +662,12 @@
     <t>Wine of many varieties, its name come from a designation, for example Bordeaux or Bourgogne, it comes from it's region and the varieties are defined by national rules</t>
   </si>
   <si>
+    <t>Chablis</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape</t>
+  </si>
+  <si>
     <t>Corvina, Molinara, Rondinella</t>
   </si>
   <si>
@@ -695,6 +701,9 @@
     <t>Chianti, Italy</t>
   </si>
   <si>
+    <t>Sauternes</t>
+  </si>
+  <si>
     <t>Grenache, Mourvèdre, Syrah and others</t>
   </si>
   <si>
@@ -1221,6 +1230,276 @@
   </si>
   <si>
     <t>Müller-Thurgau, Riesling, Sylvaner, Kerner, Scheurebe and Spätburgunder (Pinot Noir)</t>
+  </si>
+  <si>
+    <t>Red wines</t>
+  </si>
+  <si>
+    <t>Wine with strong acidity</t>
+  </si>
+  <si>
+    <t>Wine with a strong alcohol level</t>
+  </si>
+  <si>
+    <t>Crusty or chewy meals, not liquid</t>
+  </si>
+  <si>
+    <t>Wine with a lot of tanin</t>
+  </si>
+  <si>
+    <t>Fatty dish, or puff pastry</t>
+  </si>
+  <si>
+    <t>Consistent or fatty dish, red meat is a good fit</t>
+  </si>
+  <si>
+    <t>Sweet wine</t>
+  </si>
+  <si>
+    <t>Avoid sweet desserts, better go for desserts with a bit of acidity with agrums, mango, pineapple, or apricot, or with a blue cheese like roquefort</t>
+  </si>
+  <si>
+    <t>Old wine with tanin leaving with age</t>
+  </si>
+  <si>
+    <t>Meat in a casserole, confit or pulled</t>
+  </si>
+  <si>
+    <t>Young red wine</t>
+  </si>
+  <si>
+    <t>Grilled red meat</t>
+  </si>
+  <si>
+    <t>Creative dishes with mousse or gelée</t>
+  </si>
+  <si>
+    <t>Porto or Maury</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Fruity and aromatic wine</t>
+  </si>
+  <si>
+    <t>Dish with a lot of lemon</t>
+  </si>
+  <si>
+    <t>Vegetables</t>
+  </si>
+  <si>
+    <t>Not a tannic wine, better a white or a rosé</t>
+  </si>
+  <si>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Structured red wine</t>
+  </si>
+  <si>
+    <t>Dish with more than 3 flavours</t>
+  </si>
+  <si>
+    <t>Better go for water instead of wine</t>
+  </si>
+  <si>
+    <t>Reduce the feeling of sweet of the food; Seems sweeter and softer with a dish full of proteines such as meat; Seems less bitter but more tannic with salty dishes; Seems dry with spicy food</t>
+  </si>
+  <si>
+    <t>Seems less sweet with salty food; Makes salty dishes more enjoyable; Goes well with sweet food if they are themself acid enough; Can make sweet dish too sweet</t>
+  </si>
+  <si>
+    <t>Relation between sweet wine and  food</t>
+  </si>
+  <si>
+    <t>Relation between tannic wine and food</t>
+  </si>
+  <si>
+    <t>Relation between acid wine and food</t>
+  </si>
+  <si>
+    <t>Seems less acid with salty food; Seems less acid with slightly sweet food; Can make feel salty food more salty; Can balance too fatty dishes</t>
+  </si>
+  <si>
+    <t>Relation between strong wine (with a lot of alcohol) and food</t>
+  </si>
+  <si>
+    <t>Can hide subtil flavours of dishes; Goes well with slightly sweet dishes</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>Pauillac lamb</t>
+  </si>
+  <si>
+    <t>Andouillette (sausage)</t>
+  </si>
+  <si>
+    <t>Green asparagus</t>
+  </si>
+  <si>
+    <t>White asparagus</t>
+  </si>
+  <si>
+    <t>Camembert</t>
+  </si>
+  <si>
+    <t>Caviar</t>
+  </si>
+  <si>
+    <t>Comté</t>
+  </si>
+  <si>
+    <t>Red fruits cramble</t>
+  </si>
+  <si>
+    <t>Dark chocolate dessert</t>
+  </si>
+  <si>
+    <t>Dry fruits dessert</t>
+  </si>
+  <si>
+    <t>Pan friend foie gras</t>
+  </si>
+  <si>
+    <t>Goat cheese</t>
+  </si>
+  <si>
+    <t>Oysters</t>
+  </si>
+  <si>
+    <t>Osso-buco</t>
+  </si>
+  <si>
+    <t>Parmesan</t>
+  </si>
+  <si>
+    <t>Dish with white truffle</t>
+  </si>
+  <si>
+    <t>Dish with black truffle</t>
+  </si>
+  <si>
+    <t>Leek vinaigrette</t>
+  </si>
+  <si>
+    <t>Roasted chicken</t>
+  </si>
+  <si>
+    <t>Quiche lorraine</t>
+  </si>
+  <si>
+    <t>Roquefort</t>
+  </si>
+  <si>
+    <t>Roasted beef</t>
+  </si>
+  <si>
+    <t>Grilled goatfish</t>
+  </si>
+  <si>
+    <t>Smoked salmon</t>
+  </si>
+  <si>
+    <t>Cheese soufflé</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>Lemon confit chicken tajine</t>
+  </si>
+  <si>
+    <t>Tomato pie</t>
+  </si>
+  <si>
+    <t>Game meat pie</t>
+  </si>
+  <si>
+    <t>Champagne rosé</t>
+  </si>
+  <si>
+    <t>Médoc</t>
+  </si>
+  <si>
+    <t>Riesling ou Muscat</t>
+  </si>
+  <si>
+    <t>Savennières</t>
+  </si>
+  <si>
+    <t>Cassis blanc</t>
+  </si>
+  <si>
+    <t>Grilled bass fish</t>
+  </si>
+  <si>
+    <t>Cider</t>
+  </si>
+  <si>
+    <t>Champagne millésimé vieux</t>
+  </si>
+  <si>
+    <t>Vin jaune</t>
+  </si>
+  <si>
+    <t>Pineau des Charentes rosé</t>
+  </si>
+  <si>
+    <t>Banyuls ou Porto Vintage</t>
+  </si>
+  <si>
+    <t>Porto ruby</t>
+  </si>
+  <si>
+    <t>Foie gras (terrine)</t>
+  </si>
+  <si>
+    <t>Fresh: Bourgueil, Chinon ou Gevrey-Chambertin (rouges); Semi-dry: Sancerre ou Pouilly-Fumé ; Fine: Vouvray demi-sec</t>
+  </si>
+  <si>
+    <t>Muscadet ou Sylvaner</t>
+  </si>
+  <si>
+    <t>Barbera d’Alba</t>
+  </si>
+  <si>
+    <t>Amarone</t>
+  </si>
+  <si>
+    <t>vieux Barolo ou Châteauneuf-du-Pape blanc</t>
+  </si>
+  <si>
+    <t>vieux Pomerol</t>
+  </si>
+  <si>
+    <t>Verdelho (Madère)</t>
+  </si>
+  <si>
+    <t>Pinot-Gris</t>
+  </si>
+  <si>
+    <t>Porto, Maury ou Banyuls</t>
+  </si>
+  <si>
+    <t>Rosés de Provence</t>
+  </si>
+  <si>
+    <t>Chablis grand cru, Sancerre ou Pouilly-Fumé</t>
+  </si>
+  <si>
+    <t>Champagne (10 years old)</t>
+  </si>
+  <si>
+    <t>Madère Sercial or xérès amontillado sec</t>
+  </si>
+  <si>
+    <t>Languedoc-montpeyroux ou Tavel</t>
+  </si>
+  <si>
+    <t>Rosé de provence</t>
   </si>
 </sst>
 </file>
@@ -1940,10 +2219,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B25" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2020,10 +2299,10 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B35" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2184,90 +2463,90 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B11" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B12" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B13" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B14" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B16" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B17" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B18" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B19" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2280,21 +2559,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" t="s">
         <v>213</v>
-      </c>
-      <c r="B1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B2" t="s">
         <v>124</v>
@@ -2302,7 +2581,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s">
         <v>173</v>
@@ -2310,23 +2589,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s">
         <v>169</v>
@@ -2334,7 +2613,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s">
         <v>124</v>
@@ -2342,7 +2621,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B8" t="s">
         <v>124</v>
@@ -2350,39 +2629,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
@@ -2390,15 +2669,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B14" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
         <v>124</v>
@@ -2406,79 +2685,79 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>319</v>
+      </c>
+      <c r="B22" t="s">
         <v>316</v>
-      </c>
-      <c r="B22" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
+        <v>320</v>
+      </c>
+      <c r="B23" t="s">
         <v>317</v>
-      </c>
-      <c r="B23" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B24" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -2486,15 +2765,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B26" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B27" t="s">
         <v>145</v>
@@ -2502,23 +2781,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B28" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B29" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="B30" t="s">
         <v>127</v>
@@ -2526,7 +2805,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B31" t="s">
         <v>169</v>
@@ -2534,7 +2813,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B32" t="s">
         <v>127</v>
@@ -2542,7 +2821,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B33" t="s">
         <v>113</v>
@@ -2550,23 +2829,23 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B34" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B35" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B36" t="s">
         <v>169</v>
@@ -2574,31 +2853,31 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B37" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B38" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B39" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B40" t="s">
         <v>124</v>
@@ -2606,7 +2885,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="B41" t="s">
         <v>115</v>
@@ -2614,7 +2893,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B42" t="s">
         <v>115</v>
@@ -2622,39 +2901,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B43" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B44" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B45" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B46" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B47" t="s">
         <v>118</v>
@@ -2662,63 +2941,63 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B48" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B49" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B50" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B51" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B52" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B54" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B55" t="s">
         <v>151</v>
@@ -2726,7 +3005,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
@@ -2734,63 +3013,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B57" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B58" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="B59" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B60" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B61" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B62" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B63" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B64" t="s">
         <v>119</v>
@@ -2798,26 +3077,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B65" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B66" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B67" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -2827,38 +3106,54 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1">
         <v>4981</v>
       </c>
       <c r="C1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B2">
         <v>5357</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B3">
+        <v>6495</v>
+      </c>
+      <c r="C3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D3" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2878,114 +3173,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B8" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B13" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -3016,7 +3311,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3032,7 +3327,7 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3112,7 +3407,7 @@
         <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3144,7 +3439,7 @@
         <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3160,7 +3455,7 @@
         <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3168,7 +3463,7 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3184,7 +3479,7 @@
         <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3200,7 +3495,7 @@
         <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3224,7 +3519,7 @@
         <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3240,7 +3535,7 @@
         <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3256,7 +3551,7 @@
         <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3301,26 +3596,26 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B38" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B39" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B40" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3330,100 +3625,481 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>428</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="1" t="s">
-        <v>130</v>
+      <c r="A2" t="s">
+        <v>427</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>429</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>431</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>402</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>403</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1" t="s">
-        <v>140</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>405</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>433</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>434</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>435</v>
       </c>
       <c r="B10" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>343</v>
+        <v>436</v>
       </c>
       <c r="B11" t="s">
-        <v>344</v>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B12" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>468</v>
+      </c>
+      <c r="B13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>439</v>
+      </c>
+      <c r="B15" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>440</v>
+      </c>
+      <c r="B16" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>441</v>
+      </c>
+      <c r="B17" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>442</v>
+      </c>
+      <c r="B18" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>443</v>
+      </c>
+      <c r="B19" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>475</v>
+      </c>
+      <c r="B20" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>445</v>
+      </c>
+      <c r="B22" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>446</v>
+      </c>
+      <c r="B23" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>447</v>
+      </c>
+      <c r="B24" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>448</v>
+      </c>
+      <c r="B25" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>449</v>
+      </c>
+      <c r="B26" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>450</v>
+      </c>
+      <c r="B27" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>451</v>
+      </c>
+      <c r="B28" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>452</v>
+      </c>
+      <c r="B29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>453</v>
+      </c>
+      <c r="B30" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>454</v>
+      </c>
+      <c r="B31" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>455</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>456</v>
+      </c>
+      <c r="B33" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>457</v>
+      </c>
+      <c r="B34" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>458</v>
+      </c>
+      <c r="B35" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>459</v>
+      </c>
+      <c r="B36" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>460</v>
+      </c>
+      <c r="B37" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>461</v>
+      </c>
+      <c r="B38" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>462</v>
+      </c>
+      <c r="B39" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>408</v>
+      </c>
+      <c r="B40" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>410</v>
+      </c>
+      <c r="B41" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>412</v>
+      </c>
+      <c r="B42" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>414</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>416</v>
+      </c>
+      <c r="B44" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>418</v>
+      </c>
+      <c r="B45" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>419</v>
+      </c>
+      <c r="B46" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>421</v>
+      </c>
+      <c r="B47" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>423</v>
+      </c>
+      <c r="B48" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>346</v>
+      </c>
+      <c r="B59" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Food / wine pairing added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="535">
   <si>
     <t>Step 1</t>
   </si>
@@ -1500,6 +1500,139 @@
   </si>
   <si>
     <t>Rosé de provence</t>
+  </si>
+  <si>
+    <t>Bourgogne-Aligoté, Chardonnay de Bourgogne (Chablis, St Véran, Pouilly-Fuissé), Muscat, Chasselas, Pinot Gris, Gewurztraminer, Sancerre, Pouilly-Fumé, Coteaux-du-Layon, Savennières, Coteaux-de-l’Aubance, Jasnières, IGP Côtes de Gascogne.</t>
+  </si>
+  <si>
+    <t>Oysters and shells</t>
+  </si>
+  <si>
+    <t>Gros-Plant, Muscadet, Bourgogne-Aligoté, Chablis, Alsace Riesling, Alsace Sylvaner, Sancerre, Coteaux Champenois, Alsace Pinot Blanc, Cassis, Graves, Entre-Deux-Mers, Bergerac.</t>
+  </si>
+  <si>
+    <t>Grilled fishes</t>
+  </si>
+  <si>
+    <t>Fishes with sauce</t>
+  </si>
+  <si>
+    <t>Cow cheese, and soft cheese (cantal, comté)</t>
+  </si>
+  <si>
+    <t>Strong cheese (munster, maroilles)</t>
+  </si>
+  <si>
+    <t>Dessert (not too sweet, like fruit salad)</t>
+  </si>
+  <si>
+    <t>Dessert (sweet, like red fruit pie)</t>
+  </si>
+  <si>
+    <t>Aperitif (red wine)</t>
+  </si>
+  <si>
+    <t>Charcuterie</t>
+  </si>
+  <si>
+    <t>Poultry or white meat (white wine)</t>
+  </si>
+  <si>
+    <t>Poultry or white meat (red wine)</t>
+  </si>
+  <si>
+    <t>Wild game meat</t>
+  </si>
+  <si>
+    <t>Red meat</t>
+  </si>
+  <si>
+    <t>Cow cheese (red wine)</t>
+  </si>
+  <si>
+    <t>Sheep cheese</t>
+  </si>
+  <si>
+    <t>Desserts with nuts, chocolate, praline</t>
+  </si>
+  <si>
+    <t>Aperitif (rosé wine)</t>
+  </si>
+  <si>
+    <t>Starters</t>
+  </si>
+  <si>
+    <t>Seafood and fish</t>
+  </si>
+  <si>
+    <t>Poultry or white meat and grilled meat (rosé wine)</t>
+  </si>
+  <si>
+    <t>Muscadet, Anjou, Mâcon, Saumur, Chablis, Bourgogne-Aligoté, Vouvray, Pouilly-Fumé, Alsace Klevener, Beaujolais, Jurançon sec, coteaux d’Aix-en-Provence, Chassagne-Montrachet, Hermitage, Montlouis, Coteaux-Varois, Tursan, Montravel.</t>
+  </si>
+  <si>
+    <t>Chablis, Pouligny-Montrachet, Pouilly-Fuissé, Alsace Pinot Gris, Sancerre, Pouilly-Fumé, Meursault, Bourgogne Aligoté, Pessac-Léognan, Seyssel (Savoie), Croze-Hermitage, Auxey-Duresses, Côtes de Duras, St-Joseph, Patrimonio (Corse), Savennières, Vouvray, Montlouis, Picpoul de Pinet, Beaune, Monthélie.</t>
+  </si>
+  <si>
+    <t>Warm starters (puff pastry, quenelles, sweetbreads, quiches, bechamel dishes)</t>
+  </si>
+  <si>
+    <t>Sancerre, Pouilly-Fumé, Meursault, Chablis, Corton-Charlemagne, Puligny-Montrachet, Vouvray demi-sec, Côteaux-de-l’Aubance, Saussignac, Cadillac, St-Croix-du-Mont</t>
+  </si>
+  <si>
+    <t>Meursault, Arbois blanc, Alsace Riesling, Pouilly-sur-Loire, Pouilly-Fumé, Pouilly-Fuissé, St-Véran, Quincy, Menetou-Salon, Monthélie, Alsace Pinot Gris.</t>
+  </si>
+  <si>
+    <t>Chignin-Bergeron (Savoie), Meursault, Côtes-du-Rhône, Arbois blanc, Graves, Buzet, vin jaune de Jura.</t>
+  </si>
+  <si>
+    <t>Alsace Gewurztraminer vendanges tardives, Sauternes, Alsace Pinot Gris vendanges tardives, Coteaux-du-Layon, Monbazillac, Jurançon, Loupiac, St-Croix-du-Mont, Bonnezeaux, Chaume, Quart-de-Chaume</t>
+  </si>
+  <si>
+    <t>Sancerre, Pouilly-Fumé, Patrimonio, Côteaux-de-l’Aubance, Vouvray demi-sec, Condrieu, Quincy, Menetou-Salon, Reuilly, Cheverny.</t>
+  </si>
+  <si>
+    <t>Alsace Gewurztraminer vendanges tardives, Sauternes, Côteaux-du-Layon, Muscat de Beaume de Venise, St-Croix-du-Mont, Cérons, Bonnezeaux, Pacherenc du Vic-Bilh, vin de paille (Jura), Muscat de Lunel, Jurançon</t>
+  </si>
+  <si>
+    <t>Vouvray demi-sec, Rivesaltes, pineau des Charentes, Montlouis demi-sec, Cadillac, Côteaux-de-l’Aubance, Floc de Gascogne</t>
+  </si>
+  <si>
+    <t>Coteaux Champenois (Bouzy), Reuilly rouge, Sancerre rouge, Alsace Pinot Noir, Castillon-Côtes de Bordeaux, St Nicolas de Bourgueil, Saumur-Champigny.</t>
+  </si>
+  <si>
+    <t>Juliénas, Régnié, Chiroubles (beaujolais), Saumur-Champigny, Cheverny, Côtes du Rhône-Villages, Menetou-Salon, Fleurie, Chénas (beaujolais), Arbois rouge, bourgogne Passetougrains, Irancy (Côte-roannaise).</t>
+  </si>
+  <si>
+    <t>Morgon, Moulin à Vent (beaujolais), Chinon, Anjou, St-Émilion, Coteaux du Lyonnais, Tursan (vin des Landes), Lubéron, Touraine.</t>
+  </si>
+  <si>
+    <t>Pommard, Aloxe-Corton (bourgogne), Pauillac, St-Estèphe, Pomerol, Fronsac, Graves (bordeaux), Châteauneuf-du-Pape, Cornas, Côte Rôtie, Hermitage, Pécharmant, Madiran, Gigondas, Bandol, Faugères, Saint-Chinian, Corbières, Rasteau.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gevrey-Chambertin, Nuits-St-Georges, Corton, Mercurey (bourgogne), Margaux, St-Julien, Pessac-Léognan (bordeaux), Chinon, Anjou-Villages, Cahors, Auxey-Duresses, Morey St Denis, Chambolle-Musigny (bourgogne), Castillon-Côtes de Bordeaux, Canon-Fronsac, Côtes de Bourg, Moulis (bordeaux), Collioure, Minervois, Faugères, Corbières, Pécharmant, Gaillac, Patrimonio, Irouléguy, Cairanne.
+GERBOD, Catherine. Le Vin pour les Nuls, 9e édition (French Edition) (Emplacements du Kindle 9101-9104). edi8. Édition du Kindle. </t>
+  </si>
+  <si>
+    <t>Juliénas, Morgon (beaujolais), St Nicolas de Bourgueil, Côtes de Beaune, Santenay, Côtes du Rhône, Costières-de-Nimes, St-Joseph, Alsace Pinot Noir, Côteaux d’Aix-en-Provence, Languedoc, Bergerac.</t>
+  </si>
+  <si>
+    <t>Lalande de Pomerol, Côtes de Provence rouge, Côte de Blaye, Sancerre, Régnié (beaujolais), Reuilly, Cheverny, Irouléguy, Patrimonio, Madiran, St Chinian.</t>
+  </si>
+  <si>
+    <t>Rivesaltes, Banuyls, Maury, Pineau des Charentes rouge, Floc de Gasgogne rouge, Châteauneuf-du-Pape, Cahors</t>
+  </si>
+  <si>
+    <t>Côtes-de-Provence, Baux-de-Provence, Lubéron, Ventoux, Sancerre, Corse-Figari, Beaujolais rosé, Côtes-d’Auvergne-Corent, Côte-Roannaise, Saint-Pourçain, Gris-de-Toul, Collioure, Reuilly.</t>
+  </si>
+  <si>
+    <t>Côtes de Provence, Coteaux d’Aix-en-Provence, bordeaux rosé, Patrimonio, Bandol, Sancerre, Gris de Toul, Collioure, Cassis, Côtes-du-Roussillon, Minervois, Corbières, Bergerac, Tursan, Chinon, Reuilly.</t>
+  </si>
+  <si>
+    <t>Côtes de Provence, Bandol, Corse, Sancerre, Tavel, Cassis, Collioure, beaujolais, Cabardès, Marsannay.</t>
+  </si>
+  <si>
+    <t>Sancerre, Touraine, Tavel, Corse-Figari, bordeaux, Bellet, Palette, Baux-de-Provence, St Chinian, Marsannay, Bugey rosé (vin du Jura), Arbois Poulsard.</t>
   </si>
 </sst>
 </file>
@@ -3625,10 +3758,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4102,6 +4235,190 @@
         <v>347</v>
       </c>
     </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>500</v>
+      </c>
+      <c r="B60" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>492</v>
+      </c>
+      <c r="B61" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>494</v>
+      </c>
+      <c r="B62" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>495</v>
+      </c>
+      <c r="B63" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>515</v>
+      </c>
+      <c r="B64" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>502</v>
+      </c>
+      <c r="B65" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>496</v>
+      </c>
+      <c r="B66" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>497</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>445</v>
+      </c>
+      <c r="B68" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>498</v>
+      </c>
+      <c r="B69" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>499</v>
+      </c>
+      <c r="B70" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>500</v>
+      </c>
+      <c r="B71" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>501</v>
+      </c>
+      <c r="B72" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>503</v>
+      </c>
+      <c r="B73" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>504</v>
+      </c>
+      <c r="B74" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>505</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>506</v>
+      </c>
+      <c r="B76" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>507</v>
+      </c>
+      <c r="B77" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>508</v>
+      </c>
+      <c r="B78" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>509</v>
+      </c>
+      <c r="B79" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>510</v>
+      </c>
+      <c r="B80" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>511</v>
+      </c>
+      <c r="B81" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>512</v>
+      </c>
+      <c r="B82" t="s">
+        <v>534</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
:construction: Food pairing added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="597">
   <si>
     <t>Step 1</t>
   </si>
@@ -1633,6 +1633,193 @@
   </si>
   <si>
     <t>Sancerre, Touraine, Tavel, Corse-Figari, bordeaux, Bellet, Palette, Baux-de-Provence, St Chinian, Marsannay, Bugey rosé (vin du Jura), Arbois Poulsard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauerkraut
+</t>
+  </si>
+  <si>
+    <t>Riesling, Pinot Blanc, Sylvaner, Moselle blanc.</t>
+  </si>
+  <si>
+    <t>Snails stuffed with garlic and butter</t>
+  </si>
+  <si>
+    <t>Chablis, Pernand-Vergelesses blanc</t>
+  </si>
+  <si>
+    <t>Mirabelle pie</t>
+  </si>
+  <si>
+    <t>Bourguignon beef</t>
+  </si>
+  <si>
+    <t>Beaune rouge, Pommard, Aloxe-Corton.</t>
+  </si>
+  <si>
+    <t>Fondue bourgignonne</t>
+  </si>
+  <si>
+    <t>Marsannay rouge, Mercurey rouge, Irancy.</t>
+  </si>
+  <si>
+    <t>Raclette, tartiflette, fondue savoyarde</t>
+  </si>
+  <si>
+    <t>Roussette de Savoie, Seyssel, Chignin, Abymes</t>
+  </si>
+  <si>
+    <t>Bouillabaisse</t>
+  </si>
+  <si>
+    <t>Basilic pasta</t>
+  </si>
+  <si>
+    <t>Vegetables tian</t>
+  </si>
+  <si>
+    <t>Aubergines, tomato, and stuffed pepper</t>
+  </si>
+  <si>
+    <t>Côtes-de-Provence blanc, Bandol blanc, Cassis blanc or rosé, Bellet blanc or rosé, Palette blanc or rosé.</t>
+  </si>
+  <si>
+    <t>Bandol or Cassis rosé.</t>
+  </si>
+  <si>
+    <t>Bellet or Palette rouge.</t>
+  </si>
+  <si>
+    <t>Coteaux d’Aix, or Côtes de Provence rouge.</t>
+  </si>
+  <si>
+    <t>Bandol or Cassis blanc.</t>
+  </si>
+  <si>
+    <t>Cassoulet</t>
+  </si>
+  <si>
+    <t>Duck with orange or cherry</t>
+  </si>
+  <si>
+    <t>Madiran or Cahors</t>
+  </si>
+  <si>
+    <t>Duck breast or truffle sauce</t>
+  </si>
+  <si>
+    <t>Pécharmant</t>
+  </si>
+  <si>
+    <t>Cahors, un Madiran, Pécharmant, Bergerac, Gaillac, St-Mont</t>
+  </si>
+  <si>
+    <t>Beaufort</t>
+  </si>
+  <si>
+    <t>Sheep basque</t>
+  </si>
+  <si>
+    <t>Brie</t>
+  </si>
+  <si>
+    <t>Cantal or laguiole</t>
+  </si>
+  <si>
+    <t>Chaource</t>
+  </si>
+  <si>
+    <t>Cîteaux</t>
+  </si>
+  <si>
+    <t>Coulommiers</t>
+  </si>
+  <si>
+    <t>Crottin de Chavignol sec</t>
+  </si>
+  <si>
+    <t>Époisses</t>
+  </si>
+  <si>
+    <t>Fourme d’Ambert</t>
+  </si>
+  <si>
+    <t>Mimolette</t>
+  </si>
+  <si>
+    <t>Mont d’Or</t>
+  </si>
+  <si>
+    <t>Pérail de brebis</t>
+  </si>
+  <si>
+    <t>Pont-l’évêque</t>
+  </si>
+  <si>
+    <t>Reblochon</t>
+  </si>
+  <si>
+    <t>Rigote</t>
+  </si>
+  <si>
+    <t>Sainte-maure</t>
+  </si>
+  <si>
+    <t>Saint-marcellin</t>
+  </si>
+  <si>
+    <t>Tomme de Savoie</t>
+  </si>
+  <si>
+    <t>Saint-nectaire</t>
+  </si>
+  <si>
+    <t>Jurançon</t>
+  </si>
+  <si>
+    <t>Coteaux champenois</t>
+  </si>
+  <si>
+    <t>Vin de paille du Jura ou un rouge souple type</t>
+  </si>
+  <si>
+    <t>Meursault</t>
+  </si>
+  <si>
+    <t>Sancerre rouge</t>
+  </si>
+  <si>
+    <t>Vouvray moelleux</t>
+  </si>
+  <si>
+    <t>Corton-Charlemagne</t>
+  </si>
+  <si>
+    <t>Côte roannaise rouge ou côtes du Forez</t>
+  </si>
+  <si>
+    <t>Bordeaux rouge</t>
+  </si>
+  <si>
+    <t>Gamay de Chautagne</t>
+  </si>
+  <si>
+    <t>Gaillac rouge souple</t>
+  </si>
+  <si>
+    <t>Altesse de Savoie</t>
+  </si>
+  <si>
+    <t>Condrieu</t>
+  </si>
+  <si>
+    <t>Sancerre or Pouilly-Fumé</t>
+  </si>
+  <si>
+    <t>Saint-joseph rouge</t>
+  </si>
+  <si>
+    <t>Chignin-Bergeron</t>
   </si>
 </sst>
 </file>
@@ -3758,10 +3945,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4419,6 +4606,278 @@
         <v>534</v>
       </c>
     </row>
+    <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B83" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>537</v>
+      </c>
+      <c r="B84" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>539</v>
+      </c>
+      <c r="B85" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>540</v>
+      </c>
+      <c r="B86" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>542</v>
+      </c>
+      <c r="B87" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>544</v>
+      </c>
+      <c r="B88" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>546</v>
+      </c>
+      <c r="B89" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>547</v>
+      </c>
+      <c r="B90" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>548</v>
+      </c>
+      <c r="B91" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>549</v>
+      </c>
+      <c r="B92" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>494</v>
+      </c>
+      <c r="B93" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>556</v>
+      </c>
+      <c r="B94" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>558</v>
+      </c>
+      <c r="B95" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>555</v>
+      </c>
+      <c r="B96" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>561</v>
+      </c>
+      <c r="B97" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>562</v>
+      </c>
+      <c r="B98" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>563</v>
+      </c>
+      <c r="B99" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>564</v>
+      </c>
+      <c r="B100" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>565</v>
+      </c>
+      <c r="B101" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>566</v>
+      </c>
+      <c r="B102" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>567</v>
+      </c>
+      <c r="B103" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="s">
+        <v>568</v>
+      </c>
+      <c r="B104" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="s">
+        <v>569</v>
+      </c>
+      <c r="B105" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>570</v>
+      </c>
+      <c r="B106" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="s">
+        <v>571</v>
+      </c>
+      <c r="B107" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="s">
+        <v>572</v>
+      </c>
+      <c r="B108" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="s">
+        <v>573</v>
+      </c>
+      <c r="B109" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
+        <v>574</v>
+      </c>
+      <c r="B110" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
+        <v>575</v>
+      </c>
+      <c r="B111" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>576</v>
+      </c>
+      <c r="B112" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>577</v>
+      </c>
+      <c r="B113" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>578</v>
+      </c>
+      <c r="B114" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
+        <v>580</v>
+      </c>
+      <c r="B115" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" t="s">
+        <v>579</v>
+      </c>
+      <c r="B116" t="s">
+        <v>596</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
:construction: Wine to try added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="652">
   <si>
     <t>Step 1</t>
   </si>
@@ -1082,9 +1082,6 @@
     <t>Gamay, Pinot noir</t>
   </si>
   <si>
-    <t>French</t>
-  </si>
-  <si>
     <t>Kindle</t>
   </si>
   <si>
@@ -1170,9 +1167,6 @@
   </si>
   <si>
     <t>Frascati</t>
-  </si>
-  <si>
-    <t>White wines</t>
   </si>
   <si>
     <t>Ribera-del-duero (Red), Spain</t>
@@ -1820,6 +1814,177 @@
   </si>
   <si>
     <t>Chignin-Bergeron</t>
+  </si>
+  <si>
+    <t>Chardonnay, Bourgogne, France</t>
+  </si>
+  <si>
+    <t>Chardonnay Bourgogne, Côte de Beaune, France</t>
+  </si>
+  <si>
+    <t>Chardonnay, Bourgogne Côte de Beaune, France</t>
+  </si>
+  <si>
+    <t>Viognier, Côtes du Rhône nord, France</t>
+  </si>
+  <si>
+    <t>Marsanne, Roussanne Côtes du Rhône nord, France</t>
+  </si>
+  <si>
+    <t>Clairette, Provence, France</t>
+  </si>
+  <si>
+    <t>Roussanne, Marsanne Côtes du Rhône sud, France</t>
+  </si>
+  <si>
+    <t>Vermentino, Corse, France</t>
+  </si>
+  <si>
+    <t>Sauvignon, Loire, France</t>
+  </si>
+  <si>
+    <t>Chenin, Loire, France</t>
+  </si>
+  <si>
+    <t>Sémillon, Bordelais Sauternes, France</t>
+  </si>
+  <si>
+    <t>Sémillon, Sauvignon Bordelais Graves, France</t>
+  </si>
+  <si>
+    <t>Riesling, Alsace, France</t>
+  </si>
+  <si>
+    <t>Riesling, Rheingau, Germany</t>
+  </si>
+  <si>
+    <t>Riesling, Moselle, Germany</t>
+  </si>
+  <si>
+    <t>Riesling, Austria</t>
+  </si>
+  <si>
+    <t>Marsanne, Victoria, Australia</t>
+  </si>
+  <si>
+    <t>Chardonnay, Napa Valley St Helena, USA</t>
+  </si>
+  <si>
+    <t>Sauvignon blanc, Marlborough, New-zeland</t>
+  </si>
+  <si>
+    <t>Chardonnay, Knights Valley Calistoga, Californie, USA</t>
+  </si>
+  <si>
+    <t>Sauvignon, Chardonnay, Pinot Gris, Riesling italico Frioul, Italy</t>
+  </si>
+  <si>
+    <t>Trebbiano d’Abruzzo, trebbiano toscano, passerina, cococciola Abruzzes, Italy</t>
+  </si>
+  <si>
+    <t>Sémillon Hunter Valley, Australia</t>
+  </si>
+  <si>
+    <t>Chardonnay, Margaret River, Australia</t>
+  </si>
+  <si>
+    <t>Chablis Grand Cru Les Preuses Vincent Dauvissat (White)</t>
+  </si>
+  <si>
+    <t>Corton Charlemagne Coche-Dury (White)</t>
+  </si>
+  <si>
+    <t>Montrachet Domaine de la Romanée Conti (White)</t>
+  </si>
+  <si>
+    <t>Condrieu Coteau de Vernon Georges Vernay (White)</t>
+  </si>
+  <si>
+    <t>Condrieu André Perret Clos Chanson (White)</t>
+  </si>
+  <si>
+    <t>Hermitage Gérard Chave (White)</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape blanc 2006 Domaine Marcoux (White)</t>
+  </si>
+  <si>
+    <t>Palette Château Simone (White)</t>
+  </si>
+  <si>
+    <t>Coteaux du Cap Corse Clos Nicrosi (White)</t>
+  </si>
+  <si>
+    <t>Sancerre Monts Damnés François Cotat (White)</t>
+  </si>
+  <si>
+    <t>Pouilly-Fumé Silex Didier Dagueneau (White)</t>
+  </si>
+  <si>
+    <t>Vouvray réserve P. Foreau Clos Naudin sweet (White)</t>
+  </si>
+  <si>
+    <t>Savennières Thomas Boudignon (White)</t>
+  </si>
+  <si>
+    <t>Montlouis François Chidaine (White)</t>
+  </si>
+  <si>
+    <t>Sauternes Château d’Yquem (White)</t>
+  </si>
+  <si>
+    <t>Pessac-Léognan Laville Haut-Brion (White)</t>
+  </si>
+  <si>
+    <t>Riesling Clos Sainte-Hune Trimbach (White)</t>
+  </si>
+  <si>
+    <t>Zind-Humbrecht (White)</t>
+  </si>
+  <si>
+    <t>Riesling Grand Cru Kastelberg Marc Kreydenweiss (White)</t>
+  </si>
+  <si>
+    <t>Georg Breuer Berg Schlossberg (White)</t>
+  </si>
+  <si>
+    <t>Egon Müller Scharzhofberger (White)</t>
+  </si>
+  <si>
+    <t>Willi Schaefer Dromprost (White)</t>
+  </si>
+  <si>
+    <t>Franz Xavier Pichler Dürnsteiner Kellerberg (White)</t>
+  </si>
+  <si>
+    <t>Tahbilk Vineyard (White)</t>
+  </si>
+  <si>
+    <t>Newton Vineyard (White)</t>
+  </si>
+  <si>
+    <t>Kim Crawford Wines (White)</t>
+  </si>
+  <si>
+    <t>Peter Michael Winery (White)</t>
+  </si>
+  <si>
+    <t>Josko Gravner Breg Gravner (White)</t>
+  </si>
+  <si>
+    <t>Trebbiano d’Abruzzo Valentini (White)</t>
+  </si>
+  <si>
+    <t>Cullen Wines (White)</t>
+  </si>
+  <si>
+    <t>Pierro (White)</t>
+  </si>
+  <si>
+    <t>Tyrell’s Wines (White)</t>
+  </si>
+  <si>
+    <t>000 Add (Red)</t>
   </si>
 </sst>
 </file>
@@ -3205,7 +3370,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B41" t="s">
         <v>115</v>
@@ -3213,7 +3378,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B42" t="s">
         <v>115</v>
@@ -3221,39 +3386,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B44" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B46" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B47" t="s">
         <v>118</v>
@@ -3261,47 +3426,47 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B49" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B50" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B51" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B52" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B53" t="s">
         <v>213</v>
@@ -3309,15 +3474,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B55" t="s">
         <v>151</v>
@@ -3325,7 +3490,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
@@ -3333,63 +3498,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
+        <v>378</v>
+      </c>
+      <c r="B57" t="s">
         <v>379</v>
-      </c>
-      <c r="B57" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B58" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B59" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B60" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B61" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B62" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B63" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B64" t="s">
         <v>119</v>
@@ -3397,26 +3562,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B65" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B66" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B67" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3426,54 +3591,285 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2" t="s">
+        <v>596</v>
+      </c>
+      <c r="J2" t="s">
+        <v>399</v>
+      </c>
+      <c r="K2">
+        <v>6495</v>
+      </c>
+      <c r="L2" t="s">
         <v>351</v>
       </c>
-      <c r="B1">
-        <v>4981</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="M2" t="s">
         <v>352</v>
       </c>
-      <c r="D1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>381</v>
-      </c>
-      <c r="B2">
-        <v>5357</v>
-      </c>
-      <c r="C2" t="s">
-        <v>352</v>
-      </c>
-      <c r="D2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>401</v>
-      </c>
-      <c r="B3">
-        <v>6495</v>
-      </c>
-      <c r="C3" t="s">
-        <v>352</v>
-      </c>
-      <c r="D3" t="s">
-        <v>353</v>
+        <v>621</v>
+      </c>
+      <c r="B3" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>622</v>
+      </c>
+      <c r="B4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>623</v>
+      </c>
+      <c r="B5" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B6" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>625</v>
+      </c>
+      <c r="B7" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>626</v>
+      </c>
+      <c r="B8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>627</v>
+      </c>
+      <c r="B9" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>628</v>
+      </c>
+      <c r="B10" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>629</v>
+      </c>
+      <c r="B11" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>630</v>
+      </c>
+      <c r="B12" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>631</v>
+      </c>
+      <c r="B13" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>632</v>
+      </c>
+      <c r="B14" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>633</v>
+      </c>
+      <c r="B15" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>634</v>
+      </c>
+      <c r="B16" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>635</v>
+      </c>
+      <c r="B17" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>636</v>
+      </c>
+      <c r="B18" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>637</v>
+      </c>
+      <c r="B19" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>638</v>
+      </c>
+      <c r="B20" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>639</v>
+      </c>
+      <c r="B21" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>640</v>
+      </c>
+      <c r="B22" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>641</v>
+      </c>
+      <c r="B23" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>642</v>
+      </c>
+      <c r="B24" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>643</v>
+      </c>
+      <c r="B25" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>644</v>
+      </c>
+      <c r="B26" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>645</v>
+      </c>
+      <c r="B27" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>646</v>
+      </c>
+      <c r="B28" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>647</v>
+      </c>
+      <c r="B29" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>648</v>
+      </c>
+      <c r="B30" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>649</v>
+      </c>
+      <c r="B31" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>650</v>
+      </c>
+      <c r="B32" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -3947,7 +4343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
@@ -3955,79 +4351,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B4" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B7" t="s">
         <v>405</v>
-      </c>
-      <c r="B7" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B10" t="s">
         <v>211</v>
@@ -4035,79 +4431,79 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B11" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B12" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B13" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B14" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B16" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B18" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B20" t="s">
         <v>224</v>
@@ -4115,68 +4511,68 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B22" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B23" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B24" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B25" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B26" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B27" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B28" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B29" t="s">
         <v>224</v>
@@ -4184,23 +4580,23 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B30" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B31" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B32" t="s">
         <v>110</v>
@@ -4208,55 +4604,55 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B33" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B34" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B35" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B36" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B37" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B38" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B39" t="s">
         <v>212</v>
@@ -4264,31 +4660,31 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B40" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B41" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B42" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -4296,42 +4692,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B44" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B45" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B46" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B47" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B48" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4424,207 +4820,207 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B60" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B61" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B62" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B63" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B64" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B65" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B66" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B68" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B69" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B70" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B71" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B72" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B73" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B74" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B76" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B77" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B78" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B79" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B80" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B81" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B82" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B83" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B84" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B85" t="s">
         <v>125</v>
@@ -4632,250 +5028,250 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B86" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B87" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B88" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B89" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B90" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B91" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B92" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B93" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B94" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B95" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B96" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B97" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B98" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B99" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B100" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B101" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B102" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B103" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B104" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B105" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B106" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B107" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B108" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B109" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B110" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B111" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B112" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B113" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B114" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B115" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B116" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: First version of flashcards made
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Nobles varieties" sheetId="11" r:id="rId3"/>
     <sheet name="Wine &amp; naming convention" sheetId="12" r:id="rId4"/>
     <sheet name="Varieties of designations" sheetId="4" r:id="rId5"/>
-    <sheet name="Wine to discover (todo)" sheetId="13" r:id="rId6"/>
+    <sheet name="Wine to discover" sheetId="13" r:id="rId6"/>
     <sheet name="Wine Storage &amp; Service" sheetId="8" r:id="rId7"/>
     <sheet name="Tastes &amp; aromas of varieties" sheetId="5" r:id="rId8"/>
     <sheet name="Wine &amp; food pairing" sheetId="7" r:id="rId9"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="692">
   <si>
     <t>Step 1</t>
   </si>
@@ -1082,12 +1082,6 @@
     <t>Gamay, Pinot noir</t>
   </si>
   <si>
-    <t>Kindle</t>
-  </si>
-  <si>
-    <t>Region / Appellation</t>
-  </si>
-  <si>
     <t>Gavi, Piedmont (White)</t>
   </si>
   <si>
@@ -1224,9 +1218,6 @@
   </si>
   <si>
     <t>Müller-Thurgau, Riesling, Sylvaner, Kerner, Scheurebe and Spätburgunder (Pinot Noir)</t>
-  </si>
-  <si>
-    <t>Red wines</t>
   </si>
   <si>
     <t>Wine with strong acidity</t>
@@ -1984,7 +1975,136 @@
     <t>Tyrell’s Wines (White)</t>
   </si>
   <si>
-    <t>000 Add (Red)</t>
+    <t>Saumur-Champigny Clos Rougeard-Foucault &amp; fils</t>
+  </si>
+  <si>
+    <t>Saumur-Champigny Thierry Germain</t>
+  </si>
+  <si>
+    <t>Chinon Bernard</t>
+  </si>
+  <si>
+    <t>Saint-Julien Léoville Barton</t>
+  </si>
+  <si>
+    <t>Savigny-Lès-Beaune 1er Cru Domaine de la Vougeraie</t>
+  </si>
+  <si>
+    <t>Pommard Grands Épenots Domaine de Courcel</t>
+  </si>
+  <si>
+    <t>Crozes Hermitage Emmanuel Darnaud</t>
+  </si>
+  <si>
+    <t>Côte-Rôtie Domaine Jamet</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape Château Rayas</t>
+  </si>
+  <si>
+    <t>Châteauneuf-du-Pape Henri Bonneau</t>
+  </si>
+  <si>
+    <t>Bandol Château de Pibarnon</t>
+  </si>
+  <si>
+    <t>Barolo Giovanni Rosso</t>
+  </si>
+  <si>
+    <t>Barolo Roberto Voerzio</t>
+  </si>
+  <si>
+    <t>Chianti Classico La Massa</t>
+  </si>
+  <si>
+    <t>Brunello di Montalcino riserva Case Basse di Gianfranco Soldera</t>
+  </si>
+  <si>
+    <t>Alvaro Palacios</t>
+  </si>
+  <si>
+    <t>Vega Sicilia</t>
+  </si>
+  <si>
+    <t>Don Melchior</t>
+  </si>
+  <si>
+    <t>Cheval des Andes</t>
+  </si>
+  <si>
+    <t>Henschke Hill of Grace</t>
+  </si>
+  <si>
+    <t>Cordoba</t>
+  </si>
+  <si>
+    <t>Beaux Frères</t>
+  </si>
+  <si>
+    <t>Sloan Wines</t>
+  </si>
+  <si>
+    <t>Screaming Eagle</t>
+  </si>
+  <si>
+    <t>Dunn Vineyards Napa Valley</t>
+  </si>
+  <si>
+    <t>Colgin Cellars Tychson Hill Vineyard</t>
+  </si>
+  <si>
+    <t>Abreu</t>
+  </si>
+  <si>
+    <t>Cabernet franc, Loire, France</t>
+  </si>
+  <si>
+    <t>Baudry, Cabernet franc, Loire, France</t>
+  </si>
+  <si>
+    <t>Cabernet sauvignon, merlot, Médoc, France</t>
+  </si>
+  <si>
+    <t>Pinot noir, Bourgogne, France</t>
+  </si>
+  <si>
+    <t>Syrah, Côtes du Rhône nord, France</t>
+  </si>
+  <si>
+    <t>Grenache, Côtes du Rhône sud, France</t>
+  </si>
+  <si>
+    <t>Mourvèdre, Provence, France</t>
+  </si>
+  <si>
+    <t>Sangiovese, Toscane, Italy</t>
+  </si>
+  <si>
+    <t>Nebbiolo, Piémont, Italy</t>
+  </si>
+  <si>
+    <t>Carignan, Priorat, Spain</t>
+  </si>
+  <si>
+    <t>Tempranillo, Ribera del Duero, Spain</t>
+  </si>
+  <si>
+    <t>Cabernet sauvignon, Chile</t>
+  </si>
+  <si>
+    <t>Malbec, Mendoza, Argentina</t>
+  </si>
+  <si>
+    <t>Syrah, Australia</t>
+  </si>
+  <si>
+    <t>Pinotage, Stellenbosch, South Africa</t>
+  </si>
+  <si>
+    <t>Pinot noir, Oregon, USA</t>
+  </si>
+  <si>
+    <t>Cabernet sauvignon, Napa Valley Rutherford, California</t>
   </si>
 </sst>
 </file>
@@ -3370,7 +3490,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B41" t="s">
         <v>115</v>
@@ -3378,7 +3498,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B42" t="s">
         <v>115</v>
@@ -3386,39 +3506,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B43" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B44" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B46" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B47" t="s">
         <v>118</v>
@@ -3426,47 +3546,47 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B48" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B49" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B50" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B51" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B52" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B53" t="s">
         <v>213</v>
@@ -3474,15 +3594,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B54" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B55" t="s">
         <v>151</v>
@@ -3490,7 +3610,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
@@ -3498,63 +3618,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B57" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B58" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B59" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B60" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B61" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B62" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B63" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B64" t="s">
         <v>119</v>
@@ -3562,26 +3682,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B65" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B66" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B67" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -3591,285 +3711,484 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>618</v>
+      </c>
+      <c r="B3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
         <v>619</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
         <v>620</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>621</v>
+      </c>
+      <c r="B6" t="s">
         <v>596</v>
       </c>
-      <c r="J2" t="s">
-        <v>399</v>
-      </c>
-      <c r="K2">
-        <v>6495</v>
-      </c>
-      <c r="L2" t="s">
-        <v>351</v>
-      </c>
-      <c r="M2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>621</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>622</v>
+      </c>
+      <c r="B7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>623</v>
+      </c>
+      <c r="B8" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>622</v>
-      </c>
-      <c r="B4" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>623</v>
-      </c>
-      <c r="B5" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>624</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
         <v>625</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>626</v>
+      </c>
+      <c r="B11" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>627</v>
+      </c>
+      <c r="B12" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>626</v>
-      </c>
-      <c r="B8" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>627</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>628</v>
+      </c>
+      <c r="B13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>629</v>
+      </c>
+      <c r="B14" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>630</v>
+      </c>
+      <c r="B15" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>628</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>631</v>
+      </c>
+      <c r="B16" t="s">
         <v>603</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>629</v>
-      </c>
-      <c r="B11" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>630</v>
-      </c>
-      <c r="B12" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>631</v>
-      </c>
-      <c r="B13" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>632</v>
-      </c>
-      <c r="B14" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>633</v>
-      </c>
-      <c r="B15" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>634</v>
-      </c>
-      <c r="B16" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="B17" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="B18" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B19" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="B20" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="B21" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B22" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B23" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="B24" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B25" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="B26" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B27" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B28" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B29" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="B30" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B31" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
+        <v>647</v>
+      </c>
+      <c r="B32" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>648</v>
+      </c>
+      <c r="B33" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>649</v>
+      </c>
+      <c r="B34" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
         <v>650</v>
       </c>
-      <c r="B32" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>651</v>
+      </c>
+      <c r="B36" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>652</v>
+      </c>
+      <c r="B37" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>653</v>
+      </c>
+      <c r="B38" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>654</v>
+      </c>
+      <c r="B39" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>655</v>
+      </c>
+      <c r="B40" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>656</v>
+      </c>
+      <c r="B41" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>657</v>
+      </c>
+      <c r="B42" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>658</v>
+      </c>
+      <c r="B43" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>659</v>
+      </c>
+      <c r="B44" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>660</v>
+      </c>
+      <c r="B45" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>661</v>
+      </c>
+      <c r="B46" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>662</v>
+      </c>
+      <c r="B47" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>663</v>
+      </c>
+      <c r="B48" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>664</v>
+      </c>
+      <c r="B49" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>665</v>
+      </c>
+      <c r="B50" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>666</v>
+      </c>
+      <c r="B51" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>667</v>
+      </c>
+      <c r="B52" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>668</v>
+      </c>
+      <c r="B53" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>669</v>
+      </c>
+      <c r="B54" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>670</v>
+      </c>
+      <c r="B55" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>671</v>
+      </c>
+      <c r="B56" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>672</v>
+      </c>
+      <c r="B57" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>673</v>
+      </c>
+      <c r="B58" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>674</v>
+      </c>
+      <c r="B59" t="s">
+        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -4351,79 +4670,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B5" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B6" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B7" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B9" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B10" t="s">
         <v>211</v>
@@ -4431,79 +4750,79 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B11" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B12" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B13" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B15" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B16" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B18" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B19" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B20" t="s">
         <v>224</v>
@@ -4511,68 +4830,68 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B22" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B23" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B24" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B25" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B26" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B27" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B28" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B29" t="s">
         <v>224</v>
@@ -4580,23 +4899,23 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B30" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B32" t="s">
         <v>110</v>
@@ -4604,55 +4923,55 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B33" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B34" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B35" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B36" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B37" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B38" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B39" t="s">
         <v>212</v>
@@ -4660,31 +4979,31 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B40" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B41" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B42" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -4692,42 +5011,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B44" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B45" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B46" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B47" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B48" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4820,207 +5139,207 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B60" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B61" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B62" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B63" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B64" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B65" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B66" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B68" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B69" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B70" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B71" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B72" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B73" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B74" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B76" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B77" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B78" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B79" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B80" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B81" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B82" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B83" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B84" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B85" t="s">
         <v>125</v>
@@ -5028,250 +5347,250 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B86" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B87" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B88" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B89" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B90" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B91" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B92" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B93" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B94" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B95" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B96" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B97" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B98" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B99" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B100" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B101" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B102" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B103" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B104" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B105" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B106" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B107" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B108" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B109" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B110" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B111" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B112" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B113" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B114" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B115" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B116" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: Farenheight conversion added
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -824,27 +824,6 @@
     <t>Red wine temperature</t>
   </si>
   <si>
-    <t>16 - 18 ° C</t>
-  </si>
-  <si>
-    <t>14 - 16 ° C</t>
-  </si>
-  <si>
-    <t>9 - 13 ° C</t>
-  </si>
-  <si>
-    <t>10 - 12 ° C</t>
-  </si>
-  <si>
-    <t>9 - 12 ° C</t>
-  </si>
-  <si>
-    <t>14 - 16 ° C (Sauterne); 16 - 18 ° C (Porto)</t>
-  </si>
-  <si>
-    <t>8 ° C</t>
-  </si>
-  <si>
     <t>Bottle's label mandatory information</t>
   </si>
   <si>
@@ -2108,6 +2087,27 @@
   </si>
   <si>
     <t>Floral aromas, lemongrass, herbs and fruity aromas, apple, grapefruit, with nut taste</t>
+  </si>
+  <si>
+    <t>16 - 18 ° C / 60.8 - 64.4 ° F</t>
+  </si>
+  <si>
+    <t>14 - 16 ° C / 57.2 - 60.8 ° F</t>
+  </si>
+  <si>
+    <t>9 - 13 ° C / 48.2 - 55.4 ° F</t>
+  </si>
+  <si>
+    <t>10 - 12 ° C / 50 - 53.6 ° F</t>
+  </si>
+  <si>
+    <t>9 - 12 ° C / 48.2 - 53.6 ° F</t>
+  </si>
+  <si>
+    <t>8 ° C / 46.4 ° F</t>
+  </si>
+  <si>
+    <t>14 - 16 ° C / 57.2 - 60.8 ° F(Sauterne); 16 - 18 ° C / 60.8 - 64.4 ° C (Porto)</t>
   </si>
 </sst>
 </file>
@@ -2827,10 +2827,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B25" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2907,10 +2907,10 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B35" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3076,87 +3076,87 @@
         <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B14" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B15" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B17" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="B19" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B2" t="s">
         <v>124</v>
@@ -3191,7 +3191,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="B3" t="s">
         <v>173</v>
@@ -3202,7 +3202,7 @@
         <v>216</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3263,7 +3263,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B12" t="s">
         <v>234</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
@@ -3343,31 +3343,31 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B22" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B24" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -3375,15 +3375,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B26" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B27" t="s">
         <v>145</v>
@@ -3391,23 +3391,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B28" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B29" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B30" t="s">
         <v>127</v>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B31" t="s">
         <v>169</v>
@@ -3423,7 +3423,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B32" t="s">
         <v>127</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B33" t="s">
         <v>113</v>
@@ -3439,23 +3439,23 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B34" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B35" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B36" t="s">
         <v>169</v>
@@ -3463,31 +3463,31 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B37" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B38" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B39" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="B40" t="s">
         <v>124</v>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B41" t="s">
         <v>115</v>
@@ -3503,7 +3503,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="B42" t="s">
         <v>115</v>
@@ -3511,39 +3511,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B43" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B44" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B45" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B46" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="B47" t="s">
         <v>118</v>
@@ -3551,47 +3551,47 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B48" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
+        <v>354</v>
+      </c>
+      <c r="B49" t="s">
         <v>361</v>
-      </c>
-      <c r="B49" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B50" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B51" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="B52" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="B53" t="s">
         <v>213</v>
@@ -3599,15 +3599,15 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
+        <v>359</v>
+      </c>
+      <c r="B54" t="s">
         <v>366</v>
-      </c>
-      <c r="B54" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B55" t="s">
         <v>151</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B56" t="s">
         <v>115</v>
@@ -3623,63 +3623,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B57" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B58" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B59" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B60" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B61" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B62" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B63" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B64" t="s">
         <v>119</v>
@@ -3687,26 +3687,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B65" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B66" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B67" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -3718,7 +3718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -3737,7 +3737,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3753,7 +3753,7 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3833,7 +3833,7 @@
         <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3865,7 +3865,7 @@
         <v>150</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3881,7 +3881,7 @@
         <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3889,7 +3889,7 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3905,7 +3905,7 @@
         <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3921,7 +3921,7 @@
         <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3945,7 +3945,7 @@
         <v>173</v>
       </c>
       <c r="B28" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3961,7 +3961,7 @@
         <v>175</v>
       </c>
       <c r="B30" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3977,7 +3977,7 @@
         <v>177</v>
       </c>
       <c r="B32" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4022,26 +4022,26 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B38" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B39" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B40" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4049,7 +4049,7 @@
         <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -4061,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4128,7 +4128,7 @@
         <v>264</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>686</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4136,7 +4136,7 @@
         <v>258</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>687</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4144,7 +4144,7 @@
         <v>259</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>688</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4152,7 +4152,7 @@
         <v>260</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4160,7 +4160,7 @@
         <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>269</v>
+        <v>690</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4168,7 +4168,7 @@
         <v>262</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>692</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4176,7 +4176,7 @@
         <v>263</v>
       </c>
       <c r="B14" t="s">
-        <v>271</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -4196,79 +4196,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B1" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B3" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B4" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="B5" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="B6" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="B7" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B8" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B9" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B10" t="s">
         <v>211</v>
@@ -4276,79 +4276,79 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="B11" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B12" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="B14" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B15" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B16" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B17" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="B18" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="B19" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B20" t="s">
         <v>224</v>
@@ -4356,68 +4356,68 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B22" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B23" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B24" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B25" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B26" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="B27" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="B28" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B29" t="s">
         <v>224</v>
@@ -4425,23 +4425,23 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B30" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B31" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B32" t="s">
         <v>110</v>
@@ -4449,55 +4449,55 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="B33" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B34" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B35" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B36" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B37" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B38" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B39" t="s">
         <v>212</v>
@@ -4505,31 +4505,31 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B40" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B41" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B42" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -4537,42 +4537,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B44" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B45" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B46" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B47" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B48" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4657,215 +4657,215 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="B59" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B60" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="B61" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="B62" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="B63" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="B64" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B65" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="B66" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B68" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B69" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="B70" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B71" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="B72" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="B73" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B74" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B76" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B77" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="B78" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="B79" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B80" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B81" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B82" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="B83" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="B84" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="B85" t="s">
         <v>125</v>
@@ -4873,250 +4873,250 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="B86" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="B87" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="B88" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="B89" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="B90" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="B91" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="B92" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="B93" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="B94" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="B95" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="B96" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="B97" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="B98" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="B99" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="B100" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="B101" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="B102" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="B103" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="B104" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B105" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="B106" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="B107" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="B108" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="B109" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="B110" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="B111" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="B112" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="B113" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="B114" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="B115" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="B116" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -5136,474 +5136,474 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="B1" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="B2" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="B3" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="B4" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B5" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B6" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="B7" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="B8" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="B9" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="B10" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="B11" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="B12" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="B13" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="B14" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="B15" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="B16" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="B17" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="B18" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="B19" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="B20" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="B21" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="B22" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="B23" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="B24" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="B25" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="B26" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="B27" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="B28" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="B29" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="B30" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="B31" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="B32" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="B33" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="B34" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="B35" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="B36" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="B37" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="B38" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="B39" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="B40" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="B41" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="B42" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="B43" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="B44" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="B45" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="B46" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="B47" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="B48" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="B49" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="B50" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="B51" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="B52" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="B53" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="B54" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="B55" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="B56" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="B57" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="B58" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="B59" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Tanin replaced with tannin
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -278,9 +278,6 @@
     <t>Acidity</t>
   </si>
   <si>
-    <t>Tanin</t>
-  </si>
-  <si>
     <t>Balance</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>The bitterness of the red wine, it comes from the skin. If you eat the skin only of a grape you will find this taste. It generate the dry taste.</t>
   </si>
   <si>
-    <t>A wine is balanced if sweet, acidity, tanin, and alcohol are compensating each other</t>
-  </si>
-  <si>
     <t>The way the wine is doing in your palate</t>
   </si>
   <si>
@@ -581,21 +575,9 @@
     <t>Hare civet, Truffle risotto</t>
   </si>
   <si>
-    <t>Strong tanin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
-  </si>
-  <si>
-    <t>Low to medium acidity; Medium tanin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>Rich wine; High level of alcohol; Medium to high level of tanin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
-  </si>
-  <si>
     <t>Powerful wines; Can age well (Red wine)</t>
   </si>
   <si>
-    <t>Light wines; Delicates, fruity; Good acidity and low tanin; (Red wine)</t>
-  </si>
-  <si>
     <t>Powerful aromas and spicy; Sweet (Red wine)</t>
   </si>
   <si>
@@ -767,9 +749,6 @@
     <t>Bottles should be kept lying flat to maintain the cork in contact with the wine in order to prevent drying out.</t>
   </si>
   <si>
-    <t>The more the wine is young and has a lot of tanin the longer it should be airy; In general 1 hour is enough; The older it is the more careful you should be;</t>
-  </si>
-  <si>
     <t>If the wine is dark you can give it some air; If it's brick red or grenat, it reached maturity so no need of aeration</t>
   </si>
   <si>
@@ -791,18 +770,9 @@
     <t>Fortified wines need at least 8 hours of aeration; For old porto 4 hours is needed</t>
   </si>
   <si>
-    <t>Wine aeration for wine with low level of tanin</t>
-  </si>
-  <si>
-    <t>No need of long period of aeration for wine with a medium body and low level of tanin such as Pinot noir, Beaujolais, some Côte du Rhône, Dolcetto Barbera, light Chianti, Zinfandel red</t>
-  </si>
-  <si>
     <t>Wine aeration for cheap wine</t>
   </si>
   <si>
-    <t>For the wine cheaper than 5 € there is no need of aeration usually because there is a low level of tanin</t>
-  </si>
-  <si>
     <t>Great white wine temperature</t>
   </si>
   <si>
@@ -920,33 +890,18 @@
     <t>Dry apricot aromas, violet, musc, tobacco, and licorice (White wine)</t>
   </si>
   <si>
-    <t>Elegant tanin structure, nice aromas, very fruity: cassis, currant), violet, vegetal; good ageing capacity (Red wine)</t>
-  </si>
-  <si>
-    <t>Strong tanin taste, strong to medium strenght, cassis aromas, and sometime vegetal aromas, violet, or sometime other fruits; Can age (Red wine)</t>
-  </si>
-  <si>
     <t>Cinsault</t>
   </si>
   <si>
     <t>Strong wine, age fast, floral aromas</t>
   </si>
   <si>
-    <t>Light color; Low tanin; Red fruits aromas (Red wine)</t>
-  </si>
-  <si>
     <t>Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
   </si>
   <si>
-    <t>Deep color, deep body, strong level of alcohol and low tanin taste; Red fruits, Plum, chocolate or mushrooms aromas;(Red wine)</t>
-  </si>
-  <si>
     <t>Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries, cherry and earthy or wooden aromas (Red wine)</t>
   </si>
   <si>
-    <t>Dark color; Very robust; Strong tanin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
-  </si>
-  <si>
     <t>Merlot, Cabernet-Sauvignon, Cabernet-Franc, Malbec, Petit Verdot</t>
   </si>
   <si>
@@ -1046,9 +1001,6 @@
     <t>Bordeaux (Red)</t>
   </si>
   <si>
-    <t>Lamb, game meat, beef, roasted, grilled, stewed; when tanin are round it goes well with chocolate desserts, brownies</t>
-  </si>
-  <si>
     <t>Mâcon (Red), Bourgogne, France</t>
   </si>
   <si>
@@ -1205,9 +1157,6 @@
     <t>Crusty or chewy meals, not liquid</t>
   </si>
   <si>
-    <t>Wine with a lot of tanin</t>
-  </si>
-  <si>
     <t>Fatty dish, or puff pastry</t>
   </si>
   <si>
@@ -1218,9 +1167,6 @@
   </si>
   <si>
     <t>Avoid sweet desserts, better go for desserts with a bit of acidity with agrums, mango, pineapple, or apricot, or with a blue cheese like roquefort</t>
-  </si>
-  <si>
-    <t>Old wine with tanin leaving with age</t>
   </si>
   <si>
     <t>Meat in a casserole, confit or pulled</t>
@@ -2108,6 +2054,60 @@
   </si>
   <si>
     <t>14 - 16 ° C / 57.2 - 60.8 ° F(Sauterne); 16 - 18 ° C / 60.8 - 64.4 ° C (Porto)</t>
+  </si>
+  <si>
+    <t>The more the wine is young and has a lot of tannin the longer it should be airy; In general 1 hour is enough; The older it is the more careful you should be;</t>
+  </si>
+  <si>
+    <t>Wine aeration for wine with low level of tannin</t>
+  </si>
+  <si>
+    <t>No need of long period of aeration for wine with a medium body and low level of tannin such as Pinot noir, Beaujolais, some Côte du Rhône, Dolcetto Barbera, light Chianti, Zinfandel red</t>
+  </si>
+  <si>
+    <t>For the wine cheaper than 5 € there is no need of aeration usually because there is a low level of tannin</t>
+  </si>
+  <si>
+    <t>Strong tannin taste, strong to medium strenght, cassis aromas, and sometime vegetal aromas, violet, or sometime other fruits; Can age (Red wine)</t>
+  </si>
+  <si>
+    <t>Deep color, deep body, strong level of alcohol and low tannin taste; Red fruits, Plum, chocolate or mushrooms aromas;(Red wine)</t>
+  </si>
+  <si>
+    <t>Strong tannin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
+  </si>
+  <si>
+    <t>Low to medium acidity; Medium tannin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Dark color; Very robust; Strong tannin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
+  </si>
+  <si>
+    <t>Rich wine; High level of alcohol; Medium to high level of tannin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
+  </si>
+  <si>
+    <t>Light color; Low tannin; Red fruits aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>Light wines; Delicates, fruity; Good acidity and low tannin; (Red wine)</t>
+  </si>
+  <si>
+    <t>Elegant tannin structure, nice aromas, very fruity: cassis, currant), violet, vegetal; good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>Wine with a lot of tannin</t>
+  </si>
+  <si>
+    <t>Old wine with tannin leaving with age</t>
+  </si>
+  <si>
+    <t>Lamb, game meat, beef, roasted, grilled, stewed; when tannin are round it goes well with chocolate desserts, brownies</t>
+  </si>
+  <si>
+    <t>tannin</t>
+  </si>
+  <si>
+    <t>A wine is balanced if sweet, acidity, tannin, and alcohol are compensating each other</t>
   </si>
 </sst>
 </file>
@@ -2430,7 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2545,7 +2545,7 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2590,34 +2590,34 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2629,7 +2629,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2827,10 +2829,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B25" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2838,7 +2840,7 @@
         <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2846,71 +2848,71 @@
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>691</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>692</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B35" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2930,66 +2932,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3009,154 +3011,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" t="s">
         <v>203</v>
-      </c>
-      <c r="B7" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" t="s">
         <v>204</v>
-      </c>
-      <c r="B8" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
-        <v>684</v>
+        <v>666</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B10" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B12" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B13" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B18" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B19" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3175,538 +3177,538 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B11" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B18" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="B22" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="B23" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="B24" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="B26" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="B28" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="B29" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="B34" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="B35" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="B36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="B37" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B39" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="B43" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="B44" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="B45" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="B46" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="B48" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="B49" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="B50" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="B51" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="B52" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="B54" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B57" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="B58" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="B59" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="B60" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B61" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="B62" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B63" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="B65" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="B66" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="B67" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -3726,330 +3728,330 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>298</v>
+        <v>679</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>303</v>
+        <v>680</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>681</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>185</v>
+        <v>682</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B25" t="s">
-        <v>305</v>
+        <v>683</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>684</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
-        <v>301</v>
+        <v>685</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B29" t="s">
-        <v>188</v>
+        <v>686</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B30" t="s">
-        <v>297</v>
+        <v>687</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B32" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B33" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B35" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B36" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B38" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B39" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="B40" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>685</v>
+        <v>667</v>
       </c>
     </row>
   </sheetData>
@@ -4061,122 +4063,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>675</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>676</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>677</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>257</v>
+        <v>678</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B8" t="s">
-        <v>686</v>
+        <v>668</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B9" t="s">
-        <v>687</v>
+        <v>669</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s">
-        <v>688</v>
+        <v>670</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>689</v>
+        <v>671</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>690</v>
+        <v>672</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B13" t="s">
-        <v>692</v>
+        <v>674</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B14" t="s">
-        <v>691</v>
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -4188,348 +4190,348 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="B1" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="B3" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="B4" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="B5" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="B6" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>392</v>
+        <v>688</v>
       </c>
       <c r="B7" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="B8" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="B9" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="B11" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="B12" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="B13" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="B14" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="B15" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="B16" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="B17" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="B18" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="B19" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="B22" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="B23" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="B24" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="B25" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="B26" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="B27" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="B28" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="B30" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="B31" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="B33" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="B34" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="B35" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="B36" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="B37" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="B38" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="B39" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="B40" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>397</v>
+        <v>689</v>
       </c>
       <c r="B41" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="B42" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -4537,586 +4539,586 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="B44" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="B45" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="B46" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="B47" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="B48" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s">
-        <v>339</v>
+        <v>690</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="B60" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="B61" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="B62" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="B63" t="s">
-        <v>501</v>
+        <v>483</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="B64" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="B65" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="B66" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="B68" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>485</v>
+        <v>467</v>
       </c>
       <c r="B69" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="B70" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="B71" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="B72" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="B73" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="B74" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="B76" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="B77" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="B78" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B79" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="B80" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="B81" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="B82" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
       <c r="B83" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="B84" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
       <c r="B85" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
       <c r="B86" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>529</v>
+        <v>511</v>
       </c>
       <c r="B87" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
       <c r="B88" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
       <c r="B89" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="B90" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
       <c r="B91" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
       <c r="B92" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="B93" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="B94" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
       <c r="B95" t="s">
-        <v>546</v>
+        <v>528</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
       <c r="B96" t="s">
-        <v>547</v>
+        <v>529</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="B97" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
       <c r="B98" t="s">
-        <v>568</v>
+        <v>550</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>550</v>
+        <v>532</v>
       </c>
       <c r="B99" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
       <c r="B100" t="s">
-        <v>570</v>
+        <v>552</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="B101" t="s">
-        <v>569</v>
+        <v>551</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
+        <v>535</v>
+      </c>
+      <c r="B102" t="s">
         <v>553</v>
-      </c>
-      <c r="B102" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
+        <v>536</v>
+      </c>
+      <c r="B103" t="s">
         <v>554</v>
-      </c>
-      <c r="B103" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
+        <v>537</v>
+      </c>
+      <c r="B104" t="s">
         <v>555</v>
-      </c>
-      <c r="B104" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
+        <v>538</v>
+      </c>
+      <c r="B105" t="s">
         <v>556</v>
-      </c>
-      <c r="B105" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
+        <v>539</v>
+      </c>
+      <c r="B106" t="s">
         <v>557</v>
-      </c>
-      <c r="B106" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
+        <v>540</v>
+      </c>
+      <c r="B107" t="s">
         <v>558</v>
-      </c>
-      <c r="B107" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
+        <v>541</v>
+      </c>
+      <c r="B108" t="s">
         <v>559</v>
-      </c>
-      <c r="B108" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
+        <v>542</v>
+      </c>
+      <c r="B109" t="s">
         <v>560</v>
-      </c>
-      <c r="B109" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>561</v>
+        <v>543</v>
       </c>
       <c r="B110" t="s">
-        <v>576</v>
+        <v>558</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>562</v>
+        <v>544</v>
       </c>
       <c r="B111" t="s">
-        <v>579</v>
+        <v>561</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>563</v>
+        <v>545</v>
       </c>
       <c r="B112" t="s">
-        <v>580</v>
+        <v>562</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>564</v>
+        <v>546</v>
       </c>
       <c r="B113" t="s">
-        <v>581</v>
+        <v>563</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>565</v>
+        <v>547</v>
       </c>
       <c r="B114" t="s">
-        <v>582</v>
+        <v>564</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>567</v>
+        <v>549</v>
       </c>
       <c r="B115" t="s">
-        <v>576</v>
+        <v>558</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
       <c r="B116" t="s">
-        <v>583</v>
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -5136,474 +5138,474 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
       <c r="B1" t="s">
-        <v>584</v>
+        <v>566</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>609</v>
+        <v>591</v>
       </c>
       <c r="B2" t="s">
-        <v>585</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>610</v>
+        <v>592</v>
       </c>
       <c r="B3" t="s">
-        <v>586</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>611</v>
+        <v>593</v>
       </c>
       <c r="B4" t="s">
-        <v>587</v>
+        <v>569</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>612</v>
+        <v>594</v>
       </c>
       <c r="B5" t="s">
-        <v>587</v>
+        <v>569</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="B6" t="s">
-        <v>588</v>
+        <v>570</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
       <c r="B7" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
       <c r="B8" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
       <c r="B9" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>617</v>
+        <v>599</v>
       </c>
       <c r="B10" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>618</v>
+        <v>600</v>
       </c>
       <c r="B11" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>619</v>
+        <v>601</v>
       </c>
       <c r="B12" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>620</v>
+        <v>602</v>
       </c>
       <c r="B13" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>621</v>
+        <v>603</v>
       </c>
       <c r="B14" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>622</v>
+        <v>604</v>
       </c>
       <c r="B15" t="s">
-        <v>594</v>
+        <v>576</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>623</v>
+        <v>605</v>
       </c>
       <c r="B16" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>624</v>
+        <v>606</v>
       </c>
       <c r="B17" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>625</v>
+        <v>607</v>
       </c>
       <c r="B18" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>626</v>
+        <v>608</v>
       </c>
       <c r="B19" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>627</v>
+        <v>609</v>
       </c>
       <c r="B20" t="s">
-        <v>597</v>
+        <v>579</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>628</v>
+        <v>610</v>
       </c>
       <c r="B21" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>629</v>
+        <v>611</v>
       </c>
       <c r="B22" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>630</v>
+        <v>612</v>
       </c>
       <c r="B23" t="s">
-        <v>599</v>
+        <v>581</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>631</v>
+        <v>613</v>
       </c>
       <c r="B24" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>632</v>
+        <v>614</v>
       </c>
       <c r="B25" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>633</v>
+        <v>615</v>
       </c>
       <c r="B26" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>634</v>
+        <v>616</v>
       </c>
       <c r="B27" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>635</v>
+        <v>617</v>
       </c>
       <c r="B28" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>636</v>
+        <v>618</v>
       </c>
       <c r="B29" t="s">
-        <v>605</v>
+        <v>587</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>637</v>
+        <v>619</v>
       </c>
       <c r="B30" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>638</v>
+        <v>620</v>
       </c>
       <c r="B31" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>639</v>
+        <v>621</v>
       </c>
       <c r="B32" t="s">
-        <v>606</v>
+        <v>588</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>640</v>
+        <v>622</v>
       </c>
       <c r="B33" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>641</v>
+        <v>623</v>
       </c>
       <c r="B34" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>642</v>
+        <v>624</v>
       </c>
       <c r="B35" t="s">
-        <v>668</v>
+        <v>650</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>643</v>
+        <v>625</v>
       </c>
       <c r="B36" t="s">
-        <v>669</v>
+        <v>651</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>644</v>
+        <v>626</v>
       </c>
       <c r="B37" t="s">
-        <v>670</v>
+        <v>652</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>645</v>
+        <v>627</v>
       </c>
       <c r="B38" t="s">
-        <v>670</v>
+        <v>652</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="B39" t="s">
-        <v>671</v>
+        <v>653</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>647</v>
+        <v>629</v>
       </c>
       <c r="B40" t="s">
-        <v>671</v>
+        <v>653</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>648</v>
+        <v>630</v>
       </c>
       <c r="B41" t="s">
-        <v>672</v>
+        <v>654</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>649</v>
+        <v>631</v>
       </c>
       <c r="B42" t="s">
-        <v>672</v>
+        <v>654</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>650</v>
+        <v>632</v>
       </c>
       <c r="B43" t="s">
-        <v>673</v>
+        <v>655</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>651</v>
+        <v>633</v>
       </c>
       <c r="B44" t="s">
-        <v>675</v>
+        <v>657</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>652</v>
+        <v>634</v>
       </c>
       <c r="B45" t="s">
-        <v>675</v>
+        <v>657</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>653</v>
+        <v>635</v>
       </c>
       <c r="B46" t="s">
-        <v>674</v>
+        <v>656</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>654</v>
+        <v>636</v>
       </c>
       <c r="B47" t="s">
-        <v>674</v>
+        <v>656</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>655</v>
+        <v>637</v>
       </c>
       <c r="B48" t="s">
-        <v>676</v>
+        <v>658</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
       <c r="B49" t="s">
-        <v>677</v>
+        <v>659</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>657</v>
+        <v>639</v>
       </c>
       <c r="B50" t="s">
-        <v>678</v>
+        <v>660</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>658</v>
+        <v>640</v>
       </c>
       <c r="B51" t="s">
-        <v>679</v>
+        <v>661</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>659</v>
+        <v>641</v>
       </c>
       <c r="B52" t="s">
-        <v>680</v>
+        <v>662</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>660</v>
+        <v>642</v>
       </c>
       <c r="B53" t="s">
-        <v>681</v>
+        <v>663</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>661</v>
+        <v>643</v>
       </c>
       <c r="B54" t="s">
-        <v>682</v>
+        <v>664</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>662</v>
+        <v>644</v>
       </c>
       <c r="B55" t="s">
-        <v>683</v>
+        <v>665</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>663</v>
+        <v>645</v>
       </c>
       <c r="B56" t="s">
-        <v>683</v>
+        <v>665</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>664</v>
+        <v>646</v>
       </c>
       <c r="B57" t="s">
-        <v>683</v>
+        <v>665</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
+        <v>647</v>
+      </c>
+      <c r="B58" t="s">
         <v>665</v>
-      </c>
-      <c r="B58" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>666</v>
+        <v>648</v>
       </c>
       <c r="B59" t="s">
-        <v>683</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Grammar corrected for the decks, excepted tastes and aromas
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="891" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Wine making" sheetId="2" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Grapes are pressed. Only the juice is kept. Skins and seeds are removed.</t>
   </si>
   <si>
-    <t>The wine can be put in barrel to get in contact with the wood.</t>
-  </si>
-  <si>
     <t>5. Packaging</t>
   </si>
   <si>
@@ -95,15 +92,9 @@
     <t>Red color</t>
   </si>
   <si>
-    <t>The yiest of the juice starts to turn the sugar into alcohol.</t>
-  </si>
-  <si>
     <t>The wine goes red through the tannins of the skin (for Red Wine). You can make White wine with red grapes since you remove the skin</t>
   </si>
   <si>
-    <t>Why is sulphite added?</t>
-  </si>
-  <si>
     <t>To stop the wine from turning into vinegar</t>
   </si>
   <si>
@@ -125,9 +116,6 @@
     <t>More than 15%</t>
   </si>
   <si>
-    <t>Fortified wine (like porto wine) are made by adding alcohol at the end to stop the fermentation process</t>
-  </si>
-  <si>
     <t>Table wine alcohol level</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>Sparkling wine</t>
   </si>
   <si>
-    <t>During the fermentation, gaz is made, by blocking it into the bottle with the cap, the gaz enters into the wine to turn it into sparkle wine</t>
-  </si>
-  <si>
     <t>Two basic rules</t>
   </si>
   <si>
@@ -194,9 +179,6 @@
     <t>The older is a wine (white or red), the closer to the brown will the color be</t>
   </si>
   <si>
-    <t>First sniff, swirling and Second sniff</t>
-  </si>
-  <si>
     <t>Is the wine presentable? Fresh nose or aged-developed bouquet? OK to proceed? Any FAULTS? Corked, vinegary, oxidized / stale, stinky / eggy, sulfites</t>
   </si>
   <si>
@@ -212,9 +194,6 @@
     <t>Needs a good wine glass, makes the flavor easier to smell</t>
   </si>
   <si>
-    <t xml:space="preserve">Fruity / floral / spicy / berry / ripeness-level: under ripe through jammy, raisiny / estery / herbaceous / vegetal / grassy / nutty / minerally? Also think about intensity. Woody: fresh woody, vanilla, caramel, brown sugar, smoky-char,coconut </t>
-  </si>
-  <si>
     <t>Basic Tastes</t>
   </si>
   <si>
@@ -257,15 +236,6 @@
     <t>Tricks for looking</t>
   </si>
   <si>
-    <t>Put a white background, a paper is good, and a reflection of sun light would be the best</t>
-  </si>
-  <si>
-    <t>Don't wear a perfume, train identifying every flavor to train your nose</t>
-  </si>
-  <si>
-    <t>Find the basic tastes, the retro odors, and identify the mouthfeel (body), and mesure the persistence</t>
-  </si>
-  <si>
     <t>Persistence</t>
   </si>
   <si>
@@ -281,9 +251,6 @@
     <t>Balance</t>
   </si>
   <si>
-    <t>Lenght</t>
-  </si>
-  <si>
     <t>Depth</t>
   </si>
   <si>
@@ -299,48 +266,24 @@
     <t>It is the opposite of dry. If you eat a grape and you remove the skin you will find what sweet is. Be careful sweet doesn't mean fruity.</t>
   </si>
   <si>
-    <t>The sourness of the wine. In white wine it compensate the sweet taste. It generates saliva in your mouth.</t>
-  </si>
-  <si>
-    <t>The bitterness of the red wine, it comes from the skin. If you eat the skin only of a grape you will find this taste. It generate the dry taste.</t>
-  </si>
-  <si>
     <t>The way the wine is doing in your palate</t>
   </si>
   <si>
     <t>The layers of taste and aromas of the wine</t>
   </si>
   <si>
-    <t>A wine is complex if it has a good lenght and depth</t>
-  </si>
-  <si>
-    <t>If it taste like a rotten fruit, like vinegar, chemical, oxyde, burnt or cork</t>
-  </si>
-  <si>
     <t>If the tastes are similar to the other ones of the same race</t>
   </si>
   <si>
-    <t>Often use for wine ageing, and for white wine it can also be used during the fermentation</t>
-  </si>
-  <si>
     <t>Vinifera</t>
   </si>
   <si>
     <t>The type of grapes that can be used to produce wine. There are more than 10 000 varieties.</t>
   </si>
   <si>
-    <t>Caracteristics of grapes</t>
-  </si>
-  <si>
     <t>Colors, aromas, acidity, skin thickness. It makes the wine taste different</t>
   </si>
   <si>
-    <t>Caracterestic of vines</t>
-  </si>
-  <si>
-    <t>Density of grapes, quantity of leafs</t>
-  </si>
-  <si>
     <t>Nobles varieties</t>
   </si>
   <si>
@@ -392,9 +335,6 @@
     <t>Wood piece</t>
   </si>
   <si>
-    <t>Some cheap wines uses wood pieces instead of oak barrel to simulate the wooden taste</t>
-  </si>
-  <si>
     <t>Chardonnay</t>
   </si>
   <si>
@@ -749,9 +689,6 @@
     <t>Bottles should be kept lying flat to maintain the cork in contact with the wine in order to prevent drying out.</t>
   </si>
   <si>
-    <t>If the wine is dark you can give it some air; If it's brick red or grenat, it reached maturity so no need of aeration</t>
-  </si>
-  <si>
     <t>Wine aeration (Red)</t>
   </si>
   <si>
@@ -767,9 +704,6 @@
     <t>Wine aeration (Fortified wine)</t>
   </si>
   <si>
-    <t>Fortified wines need at least 8 hours of aeration; For old porto 4 hours is needed</t>
-  </si>
-  <si>
     <t>Wine aeration for cheap wine</t>
   </si>
   <si>
@@ -849,9 +783,6 @@
   </si>
   <si>
     <t>Millésime</t>
-  </si>
-  <si>
-    <t>A wine can have a millesime mention if 95% of the grapes come from the same year in USA, and 85% in Europe</t>
   </si>
   <si>
     <t>Tasting order</t>
@@ -2056,15 +1987,6 @@
     <t>14 - 16 ° C / 57.2 - 60.8 ° F(Sauterne); 16 - 18 ° C / 60.8 - 64.4 ° C (Porto)</t>
   </si>
   <si>
-    <t>The more the wine is young and has a lot of tannin the longer it should be airy; In general 1 hour is enough; The older it is the more careful you should be;</t>
-  </si>
-  <si>
-    <t>Wine aeration for wine with low level of tannin</t>
-  </si>
-  <si>
-    <t>No need of long period of aeration for wine with a medium body and low level of tannin such as Pinot noir, Beaujolais, some Côte du Rhône, Dolcetto Barbera, light Chianti, Zinfandel red</t>
-  </si>
-  <si>
     <t>For the wine cheaper than 5 € there is no need of aeration usually because there is a low level of tannin</t>
   </si>
   <si>
@@ -2104,10 +2026,88 @@
     <t>Lamb, game meat, beef, roasted, grilled, stewed; when tannin are round it goes well with chocolate desserts, brownies</t>
   </si>
   <si>
-    <t>tannin</t>
-  </si>
-  <si>
     <t>A wine is balanced if sweet, acidity, tannin, and alcohol are compensating each other</t>
+  </si>
+  <si>
+    <t>The yeast of the juice starts to turn the sugar into alcohol.</t>
+  </si>
+  <si>
+    <t>Fortified wine (like Porto wine) are made by adding alcohol at the end to stop the fermentation process</t>
+  </si>
+  <si>
+    <t>During the fermentation, gas is made, by blocking it into the bottle with the cap, the gas enters into the wine to turn it into sparkle wine</t>
+  </si>
+  <si>
+    <t>The wine can be put in a barrel to get in contact with the wood.</t>
+  </si>
+  <si>
+    <t>Some cheap wines use wood pieces instead of an oak barrel to simulate the wooden taste</t>
+  </si>
+  <si>
+    <t>The density of grapes, the number of leafs</t>
+  </si>
+  <si>
+    <t>Often use for wine ageing, and for white wine, it can also be used during the fermentation</t>
+  </si>
+  <si>
+    <t>Why is sulfite added?</t>
+  </si>
+  <si>
+    <t>Characteristics of grapes</t>
+  </si>
+  <si>
+    <t>Characteristics of vines</t>
+  </si>
+  <si>
+    <t>Tannin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruity / floral / spicy / berry / ripeness-level: under ripe through jammy, raisiny / estery / herbaceous / vegetal / grassy / nutty / minerally. Also, think about intensity. Woody: fresh woody, vanilla, caramel, brown sugar, smoky-char,coconut </t>
+  </si>
+  <si>
+    <t>Don't wear a perfume, train to identify every flavor to train your nose</t>
+  </si>
+  <si>
+    <t>The sourness of the wine. In white wine, it compensates for the sweet taste. It generates saliva in your mouth.</t>
+  </si>
+  <si>
+    <t>The bitterness of the red wine, it comes from the skin. If you eat the skin only of a grape you will find this taste. It generates the dry taste.</t>
+  </si>
+  <si>
+    <t>The first sniff, swirling, and the second sniff</t>
+  </si>
+  <si>
+    <t>Find the basic tastes, the retro odors, and identify the mouthfeel (body), and measure the persistence</t>
+  </si>
+  <si>
+    <t>Put a white background, a paper is good, and a reflection of sunlight would be the best</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>A wine is complex if it has a good length and depth</t>
+  </si>
+  <si>
+    <t>If it tastes like a rotten fruit, like vinegar, chemical, oxide, burnt or cork</t>
+  </si>
+  <si>
+    <t>A wine can have a millésime mention if 95% of the grapes come from the same year in the USA, and 85% in Europe</t>
+  </si>
+  <si>
+    <t>The more the wine is young and has a lot of tannins the longer it should be airy; In general 1 hour is enough; The older it is the more careful you should be;</t>
+  </si>
+  <si>
+    <t>If the wine is dark you can give it some air; If it's brick red or garnet it reached maturity so no need for aeration</t>
+  </si>
+  <si>
+    <t>No need for a long period of aeration for wine with a medium body and low level of tannin such as Pinot noir, Beaujolais, some Côte du Rhône, Dolcetto Barbera, light Chianti, Zinfandel red</t>
+  </si>
+  <si>
+    <t>Fortified wines need at least 8 hours of aeration; For old Porto, 4 hours is needed</t>
+  </si>
+  <si>
+    <t>Wine aeration for wine with a low level of tannin</t>
   </si>
 </sst>
 </file>
@@ -2430,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2505,7 +2505,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>666</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2513,111 +2513,111 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>669</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>673</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>672</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>667</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>674</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>675</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>671</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>
@@ -2629,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2640,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2648,7 +2648,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2656,7 +2656,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2664,255 +2664,255 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>677</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>682</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>678</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>683</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="B25" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>679</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>691</v>
+        <v>676</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>680</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>692</v>
+        <v>665</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>684</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>685</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>686</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="B35" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2925,73 +2925,73 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3011,154 +3011,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B9" t="s">
-        <v>666</v>
+        <v>643</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B15" t="s">
-        <v>267</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="B17" t="s">
-        <v>271</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="B18" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="B19" t="s">
-        <v>274</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -3171,544 +3171,544 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="B10" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B17" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="B20" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="B22" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="B23" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="B24" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
       <c r="B26" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="B27" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="B28" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="B29" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="B34" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="B35" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="B37" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="B38" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
       <c r="B39" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
       <c r="B43" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="B45" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
       <c r="B46" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="B48" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="B49" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="B50" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="B51" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="B52" t="s">
-        <v>349</v>
+        <v>326</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="B53" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="B54" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="B55" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="B57" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="B58" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="B59" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="B60" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
       <c r="B61" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="B62" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="B63" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="B64" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="B65" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="B66" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="B67" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3720,338 +3720,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
         <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>679</v>
+        <v>653</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>680</v>
+        <v>654</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>681</v>
+        <v>655</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>682</v>
+        <v>656</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
-        <v>683</v>
+        <v>657</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>684</v>
+        <v>658</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>685</v>
+        <v>659</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
-        <v>686</v>
+        <v>660</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B30" t="s">
-        <v>687</v>
+        <v>661</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B31" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="B39" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="B40" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>667</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -4064,121 +4064,121 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>675</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>689</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>691</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>676</v>
+        <v>692</v>
       </c>
       <c r="B6" t="s">
-        <v>677</v>
+        <v>690</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="B7" t="s">
-        <v>678</v>
+        <v>652</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>668</v>
+        <v>645</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>669</v>
+        <v>646</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="B10" t="s">
-        <v>670</v>
+        <v>647</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
       <c r="B11" t="s">
-        <v>671</v>
+        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>672</v>
+        <v>649</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>674</v>
+        <v>651</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>673</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -4190,7 +4190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -4198,927 +4198,927 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="B1" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="B4" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="B5" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="B6" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>688</v>
+        <v>662</v>
       </c>
       <c r="B7" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="B8" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="B9" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="B11" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="B12" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="B13" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="B14" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="B15" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="B16" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="B17" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="B18" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
       <c r="B19" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="B20" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="B22" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="B23" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
       <c r="B24" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="B25" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
       <c r="B26" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="B27" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
       <c r="B28" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="B29" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
       <c r="B30" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="B31" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
       <c r="B33" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="B34" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="B35" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
       <c r="B36" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="B37" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="B38" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="B40" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>689</v>
+        <v>663</v>
       </c>
       <c r="B41" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="B42" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="B44" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="B45" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="B46" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="B47" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="B48" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="B58" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="B59" t="s">
-        <v>690</v>
+        <v>664</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
       <c r="B60" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="B61" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="B62" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="B63" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
       <c r="B64" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
       <c r="B65" t="s">
-        <v>486</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
       <c r="B66" t="s">
-        <v>487</v>
+        <v>464</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="B68" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
+        <v>444</v>
+      </c>
+      <c r="B69" t="s">
         <v>467</v>
-      </c>
-      <c r="B69" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
+        <v>445</v>
+      </c>
+      <c r="B70" t="s">
         <v>468</v>
-      </c>
-      <c r="B70" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
+        <v>446</v>
+      </c>
+      <c r="B71" t="s">
         <v>469</v>
-      </c>
-      <c r="B71" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
+        <v>447</v>
+      </c>
+      <c r="B72" t="s">
         <v>470</v>
-      </c>
-      <c r="B72" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
       <c r="B73" t="s">
-        <v>494</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>473</v>
+        <v>450</v>
       </c>
       <c r="B74" t="s">
-        <v>495</v>
+        <v>472</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>496</v>
+        <v>473</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
       <c r="B76" t="s">
-        <v>497</v>
+        <v>474</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="B77" t="s">
-        <v>498</v>
+        <v>475</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="B78" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
       <c r="B79" t="s">
-        <v>500</v>
+        <v>477</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
       <c r="B80" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="B81" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
       <c r="B82" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
       <c r="B83" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>506</v>
+        <v>483</v>
       </c>
       <c r="B84" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="B85" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>509</v>
+        <v>486</v>
       </c>
       <c r="B86" t="s">
-        <v>510</v>
+        <v>487</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="B87" t="s">
-        <v>512</v>
+        <v>489</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>513</v>
+        <v>490</v>
       </c>
       <c r="B88" t="s">
-        <v>514</v>
+        <v>491</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>515</v>
+        <v>492</v>
       </c>
       <c r="B89" t="s">
-        <v>519</v>
+        <v>496</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>516</v>
+        <v>493</v>
       </c>
       <c r="B90" t="s">
-        <v>520</v>
+        <v>497</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>517</v>
+        <v>494</v>
       </c>
       <c r="B91" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>518</v>
+        <v>495</v>
       </c>
       <c r="B92" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="B93" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>525</v>
+        <v>502</v>
       </c>
       <c r="B94" t="s">
-        <v>526</v>
+        <v>503</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>527</v>
+        <v>504</v>
       </c>
       <c r="B95" t="s">
-        <v>528</v>
+        <v>505</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>524</v>
+        <v>501</v>
       </c>
       <c r="B96" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="B97" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>531</v>
+        <v>508</v>
       </c>
       <c r="B98" t="s">
-        <v>550</v>
+        <v>527</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>532</v>
+        <v>509</v>
       </c>
       <c r="B99" t="s">
-        <v>551</v>
+        <v>528</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>533</v>
+        <v>510</v>
       </c>
       <c r="B100" t="s">
-        <v>552</v>
+        <v>529</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>534</v>
+        <v>511</v>
       </c>
       <c r="B101" t="s">
-        <v>551</v>
+        <v>528</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>535</v>
+        <v>512</v>
       </c>
       <c r="B102" t="s">
-        <v>553</v>
+        <v>530</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>536</v>
+        <v>513</v>
       </c>
       <c r="B103" t="s">
-        <v>554</v>
+        <v>531</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>537</v>
+        <v>514</v>
       </c>
       <c r="B104" t="s">
-        <v>555</v>
+        <v>532</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>538</v>
+        <v>515</v>
       </c>
       <c r="B105" t="s">
-        <v>556</v>
+        <v>533</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>539</v>
+        <v>516</v>
       </c>
       <c r="B106" t="s">
-        <v>557</v>
+        <v>534</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="B107" t="s">
-        <v>558</v>
+        <v>535</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="B108" t="s">
-        <v>559</v>
+        <v>536</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
       <c r="B109" t="s">
-        <v>560</v>
+        <v>537</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>543</v>
+        <v>520</v>
       </c>
       <c r="B110" t="s">
-        <v>558</v>
+        <v>535</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>544</v>
+        <v>521</v>
       </c>
       <c r="B111" t="s">
-        <v>561</v>
+        <v>538</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>545</v>
+        <v>522</v>
       </c>
       <c r="B112" t="s">
-        <v>562</v>
+        <v>539</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="B113" t="s">
-        <v>563</v>
+        <v>540</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>547</v>
+        <v>524</v>
       </c>
       <c r="B114" t="s">
-        <v>564</v>
+        <v>541</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>549</v>
+        <v>526</v>
       </c>
       <c r="B115" t="s">
-        <v>558</v>
+        <v>535</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>548</v>
+        <v>525</v>
       </c>
       <c r="B116" t="s">
-        <v>565</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -5138,474 +5138,474 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>590</v>
+        <v>567</v>
       </c>
       <c r="B1" t="s">
-        <v>566</v>
+        <v>543</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>591</v>
+        <v>568</v>
       </c>
       <c r="B2" t="s">
-        <v>567</v>
+        <v>544</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>592</v>
+        <v>569</v>
       </c>
       <c r="B3" t="s">
-        <v>568</v>
+        <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>593</v>
+        <v>570</v>
       </c>
       <c r="B4" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>594</v>
+        <v>571</v>
       </c>
       <c r="B5" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="B6" t="s">
-        <v>570</v>
+        <v>547</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>596</v>
+        <v>573</v>
       </c>
       <c r="B7" t="s">
-        <v>572</v>
+        <v>549</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>597</v>
+        <v>574</v>
       </c>
       <c r="B8" t="s">
-        <v>571</v>
+        <v>548</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>598</v>
+        <v>575</v>
       </c>
       <c r="B9" t="s">
-        <v>573</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="B10" t="s">
-        <v>574</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>600</v>
+        <v>577</v>
       </c>
       <c r="B11" t="s">
-        <v>574</v>
+        <v>551</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="B12" t="s">
-        <v>575</v>
+        <v>552</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>602</v>
+        <v>579</v>
       </c>
       <c r="B13" t="s">
-        <v>575</v>
+        <v>552</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>603</v>
+        <v>580</v>
       </c>
       <c r="B14" t="s">
-        <v>575</v>
+        <v>552</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>604</v>
+        <v>581</v>
       </c>
       <c r="B15" t="s">
-        <v>576</v>
+        <v>553</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>605</v>
+        <v>582</v>
       </c>
       <c r="B16" t="s">
-        <v>577</v>
+        <v>554</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>606</v>
+        <v>583</v>
       </c>
       <c r="B17" t="s">
-        <v>578</v>
+        <v>555</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>607</v>
+        <v>584</v>
       </c>
       <c r="B18" t="s">
-        <v>578</v>
+        <v>555</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>608</v>
+        <v>585</v>
       </c>
       <c r="B19" t="s">
-        <v>578</v>
+        <v>555</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>609</v>
+        <v>586</v>
       </c>
       <c r="B20" t="s">
-        <v>579</v>
+        <v>556</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>610</v>
+        <v>587</v>
       </c>
       <c r="B21" t="s">
-        <v>580</v>
+        <v>557</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>611</v>
+        <v>588</v>
       </c>
       <c r="B22" t="s">
-        <v>580</v>
+        <v>557</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>612</v>
+        <v>589</v>
       </c>
       <c r="B23" t="s">
-        <v>581</v>
+        <v>558</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>613</v>
+        <v>590</v>
       </c>
       <c r="B24" t="s">
-        <v>582</v>
+        <v>559</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>614</v>
+        <v>591</v>
       </c>
       <c r="B25" t="s">
-        <v>583</v>
+        <v>560</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>615</v>
+        <v>592</v>
       </c>
       <c r="B26" t="s">
-        <v>584</v>
+        <v>561</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>616</v>
+        <v>593</v>
       </c>
       <c r="B27" t="s">
-        <v>585</v>
+        <v>562</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>617</v>
+        <v>594</v>
       </c>
       <c r="B28" t="s">
-        <v>586</v>
+        <v>563</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>618</v>
+        <v>595</v>
       </c>
       <c r="B29" t="s">
-        <v>587</v>
+        <v>564</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>619</v>
+        <v>596</v>
       </c>
       <c r="B30" t="s">
-        <v>589</v>
+        <v>566</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>620</v>
+        <v>597</v>
       </c>
       <c r="B31" t="s">
-        <v>589</v>
+        <v>566</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>621</v>
+        <v>598</v>
       </c>
       <c r="B32" t="s">
-        <v>588</v>
+        <v>565</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>622</v>
+        <v>599</v>
       </c>
       <c r="B33" t="s">
-        <v>649</v>
+        <v>626</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>623</v>
+        <v>600</v>
       </c>
       <c r="B34" t="s">
-        <v>649</v>
+        <v>626</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>624</v>
+        <v>601</v>
       </c>
       <c r="B35" t="s">
-        <v>650</v>
+        <v>627</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>625</v>
+        <v>602</v>
       </c>
       <c r="B36" t="s">
-        <v>651</v>
+        <v>628</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>626</v>
+        <v>603</v>
       </c>
       <c r="B37" t="s">
-        <v>652</v>
+        <v>629</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>627</v>
+        <v>604</v>
       </c>
       <c r="B38" t="s">
-        <v>652</v>
+        <v>629</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>628</v>
+        <v>605</v>
       </c>
       <c r="B39" t="s">
-        <v>653</v>
+        <v>630</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>629</v>
+        <v>606</v>
       </c>
       <c r="B40" t="s">
-        <v>653</v>
+        <v>630</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>630</v>
+        <v>607</v>
       </c>
       <c r="B41" t="s">
-        <v>654</v>
+        <v>631</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
+        <v>608</v>
+      </c>
+      <c r="B42" t="s">
         <v>631</v>
-      </c>
-      <c r="B42" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
+        <v>609</v>
+      </c>
+      <c r="B43" t="s">
         <v>632</v>
-      </c>
-      <c r="B43" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>633</v>
+        <v>610</v>
       </c>
       <c r="B44" t="s">
-        <v>657</v>
+        <v>634</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
+        <v>611</v>
+      </c>
+      <c r="B45" t="s">
         <v>634</v>
-      </c>
-      <c r="B45" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>635</v>
+        <v>612</v>
       </c>
       <c r="B46" t="s">
-        <v>656</v>
+        <v>633</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>636</v>
+        <v>613</v>
       </c>
       <c r="B47" t="s">
-        <v>656</v>
+        <v>633</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>637</v>
+        <v>614</v>
       </c>
       <c r="B48" t="s">
-        <v>658</v>
+        <v>635</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>638</v>
+        <v>615</v>
       </c>
       <c r="B49" t="s">
-        <v>659</v>
+        <v>636</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>639</v>
+        <v>616</v>
       </c>
       <c r="B50" t="s">
-        <v>660</v>
+        <v>637</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>640</v>
+        <v>617</v>
       </c>
       <c r="B51" t="s">
-        <v>661</v>
+        <v>638</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>641</v>
+        <v>618</v>
       </c>
       <c r="B52" t="s">
-        <v>662</v>
+        <v>639</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>642</v>
+        <v>619</v>
       </c>
       <c r="B53" t="s">
-        <v>663</v>
+        <v>640</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>643</v>
+        <v>620</v>
       </c>
       <c r="B54" t="s">
-        <v>664</v>
+        <v>641</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>644</v>
+        <v>621</v>
       </c>
       <c r="B55" t="s">
-        <v>665</v>
+        <v>642</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>645</v>
+        <v>622</v>
       </c>
       <c r="B56" t="s">
-        <v>665</v>
+        <v>642</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>646</v>
+        <v>623</v>
       </c>
       <c r="B57" t="s">
-        <v>665</v>
+        <v>642</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>647</v>
+        <v>624</v>
       </c>
       <c r="B58" t="s">
-        <v>665</v>
+        <v>642</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>648</v>
+        <v>625</v>
       </c>
       <c r="B59" t="s">
-        <v>665</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Template created for wine type
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -419,9 +419,6 @@
     <t>Trebbiano</t>
   </si>
   <si>
-    <t>From the oak: Smoked, Grilled, Nuts, Vanilla; From the grapes: Apple, tropical fruits, ananas; Sometime: Earthy, Minerals, Mushrooms (White wine)</t>
-  </si>
-  <si>
     <t>Darker than most of the white wines; Medium body; Low acidity; Neutral aromas of fruits' skin such as peach or orange (White wine)</t>
   </si>
   <si>
@@ -2108,6 +2105,9 @@
   </si>
   <si>
     <t>Wine aeration for wine with a low level of tannin</t>
+  </si>
+  <si>
+    <t>&lt;div&gt; &lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt; Smoked, grilled, nuts, vanilla, apple, tropical fruits, pineapple, earthy, minerals, mushrooms&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -2505,7 +2505,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2513,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2534,7 +2534,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2545,7 +2545,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2561,7 +2561,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2569,7 +2569,7 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2598,7 +2598,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B22" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2617,7 +2617,7 @@
         <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -2629,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2712,7 +2712,7 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2736,7 +2736,7 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2744,7 +2744,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2816,7 +2816,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2824,15 +2824,15 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" t="s">
         <v>254</v>
-      </c>
-      <c r="B25" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2848,15 +2848,15 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B28" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2864,12 +2864,12 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B30" t="s">
         <v>79</v>
@@ -2888,7 +2888,7 @@
         <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2904,15 +2904,15 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
+        <v>251</v>
+      </c>
+      <c r="B35" t="s">
         <v>252</v>
-      </c>
-      <c r="B35" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3011,154 +3011,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
         <v>169</v>
-      </c>
-      <c r="B1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
         <v>171</v>
-      </c>
-      <c r="B2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" t="s">
         <v>173</v>
-      </c>
-      <c r="B3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
         <v>175</v>
-      </c>
-      <c r="B4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
         <v>233</v>
-      </c>
-      <c r="B10" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
         <v>235</v>
-      </c>
-      <c r="B11" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -3177,15 +3177,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
@@ -3193,39 +3193,39 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s">
         <v>102</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
         <v>102</v>
@@ -3241,39 +3241,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s">
         <v>90</v>
@@ -3281,15 +3281,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
         <v>102</v>
@@ -3297,79 +3297,79 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
@@ -3377,15 +3377,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B27" t="s">
         <v>123</v>
@@ -3393,23 +3393,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B30" t="s">
         <v>105</v>
@@ -3417,15 +3417,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
@@ -3441,55 +3441,55 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B35" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B40" t="s">
         <v>102</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B41" t="s">
         <v>94</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B42" t="s">
         <v>94</v>
@@ -3513,39 +3513,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B46" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
@@ -3553,63 +3553,63 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B48" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B49" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B50" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B51" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B52" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B54" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B55" t="s">
         <v>129</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -3625,63 +3625,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
+        <v>328</v>
+      </c>
+      <c r="B57" t="s">
         <v>329</v>
-      </c>
-      <c r="B57" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
+        <v>330</v>
+      </c>
+      <c r="B58" t="s">
         <v>331</v>
-      </c>
-      <c r="B58" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
+        <v>332</v>
+      </c>
+      <c r="B59" t="s">
         <v>333</v>
-      </c>
-      <c r="B59" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B60" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>336</v>
+      </c>
+      <c r="B61" t="s">
         <v>337</v>
-      </c>
-      <c r="B61" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
+        <v>338</v>
+      </c>
+      <c r="B62" t="s">
         <v>339</v>
-      </c>
-      <c r="B62" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
+        <v>340</v>
+      </c>
+      <c r="B63" t="s">
         <v>341</v>
-      </c>
-      <c r="B63" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B64" t="s">
         <v>98</v>
@@ -3689,26 +3689,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
+        <v>343</v>
+      </c>
+      <c r="B65" t="s">
         <v>344</v>
-      </c>
-      <c r="B65" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B66" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
+        <v>347</v>
+      </c>
+      <c r="B67" t="s">
         <v>348</v>
-      </c>
-      <c r="B67" t="s">
-        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3731,7 +3731,7 @@
         <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>692</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3739,7 +3739,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3747,7 +3747,7 @@
         <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3755,7 +3755,7 @@
         <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3763,7 +3763,7 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3771,7 +3771,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3779,7 +3779,7 @@
         <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3787,7 +3787,7 @@
         <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3795,7 +3795,7 @@
         <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3803,7 +3803,7 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3811,7 +3811,7 @@
         <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3819,7 +3819,7 @@
         <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3827,7 +3827,7 @@
         <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3835,7 +3835,7 @@
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3843,7 +3843,7 @@
         <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3851,7 +3851,7 @@
         <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3859,7 +3859,7 @@
         <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3867,7 +3867,7 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3875,23 +3875,23 @@
         <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3899,15 +3899,15 @@
         <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3915,135 +3915,135 @@
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B30" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" t="s">
         <v>256</v>
-      </c>
-      <c r="B38" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
+        <v>257</v>
+      </c>
+      <c r="B39" t="s">
         <v>258</v>
-      </c>
-      <c r="B39" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>263</v>
+      </c>
+      <c r="B40" t="s">
         <v>264</v>
-      </c>
-      <c r="B40" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4051,7 +4051,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -4071,114 +4071,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" t="s">
         <v>218</v>
-      </c>
-      <c r="B1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" t="s">
         <v>222</v>
-      </c>
-      <c r="B4" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B8" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B12" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -4198,252 +4198,252 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B3" t="s">
         <v>375</v>
-      </c>
-      <c r="B3" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B4" t="s">
         <v>377</v>
-      </c>
-      <c r="B4" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>350</v>
+      </c>
+      <c r="B6" t="s">
         <v>351</v>
-      </c>
-      <c r="B6" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B24" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B25" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B30" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B31" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
@@ -4451,87 +4451,87 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B33" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B34" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B36" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B38" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>354</v>
+      </c>
+      <c r="B40" t="s">
         <v>355</v>
-      </c>
-      <c r="B40" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B41" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
+        <v>357</v>
+      </c>
+      <c r="B42" t="s">
         <v>358</v>
-      </c>
-      <c r="B42" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
@@ -4539,42 +4539,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B44" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B45" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>364</v>
+      </c>
+      <c r="B46" t="s">
         <v>365</v>
-      </c>
-      <c r="B46" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
+        <v>366</v>
+      </c>
+      <c r="B47" t="s">
         <v>367</v>
-      </c>
-      <c r="B47" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
+        <v>368</v>
+      </c>
+      <c r="B48" t="s">
         <v>369</v>
-      </c>
-      <c r="B48" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4651,223 +4651,223 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B59" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B60" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>437</v>
+      </c>
+      <c r="B61" t="s">
         <v>438</v>
-      </c>
-      <c r="B61" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B62" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B63" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
+        <v>460</v>
+      </c>
+      <c r="B64" t="s">
         <v>461</v>
-      </c>
-      <c r="B64" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B65" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B66" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B68" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B69" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B70" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B71" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B72" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B74" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B76" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B77" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B78" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B79" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B80" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B81" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B82" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B83" t="s">
         <v>481</v>
-      </c>
-      <c r="B83" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
+        <v>482</v>
+      </c>
+      <c r="B84" t="s">
         <v>483</v>
-      </c>
-      <c r="B84" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B85" t="s">
         <v>103</v>
@@ -4875,250 +4875,250 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
+        <v>485</v>
+      </c>
+      <c r="B86" t="s">
         <v>486</v>
-      </c>
-      <c r="B86" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
+        <v>487</v>
+      </c>
+      <c r="B87" t="s">
         <v>488</v>
-      </c>
-      <c r="B87" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
+        <v>489</v>
+      </c>
+      <c r="B88" t="s">
         <v>490</v>
-      </c>
-      <c r="B88" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B89" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B90" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B91" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B92" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B93" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
+        <v>501</v>
+      </c>
+      <c r="B94" t="s">
         <v>502</v>
-      </c>
-      <c r="B94" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
+        <v>503</v>
+      </c>
+      <c r="B95" t="s">
         <v>504</v>
-      </c>
-      <c r="B95" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B96" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B97" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B98" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B99" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B100" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B101" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B102" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B103" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B104" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B105" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B106" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B107" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B108" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B109" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B110" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B111" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B112" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B113" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B114" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B115" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B116" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -5138,474 +5138,474 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B8" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B14" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B18" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B20" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B21" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B22" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B23" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B24" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B25" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B26" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B27" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B28" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B29" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B32" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B33" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B34" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B35" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B36" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B37" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B38" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B39" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B40" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B41" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B42" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B43" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B44" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B45" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B46" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B47" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B48" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B49" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B50" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B51" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B52" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B53" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B54" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B55" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B56" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B57" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B58" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B59" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: Template implemented for 10 varieties
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -419,27 +419,6 @@
     <t>Trebbiano</t>
   </si>
   <si>
-    <t>Darker than most of the white wines; Medium body; Low acidity; Neutral aromas of fruits' skin such as peach or orange (White wine)</t>
-  </si>
-  <si>
-    <t>Very acid, Aromas and flavours: herbal, minerals, grass, fruits such as melon In California it has Oak taste (White wine)</t>
-  </si>
-  <si>
-    <t>Good acidity (White wine)</t>
-  </si>
-  <si>
-    <t>Delicate, subtil, with flower flavours (White wine)</t>
-  </si>
-  <si>
-    <t>Very fresh, mineral, intense, white flowers and white fruits aromas (White wine)</t>
-  </si>
-  <si>
-    <t>White pepper, mellifère (nectar plants) aromas (White wine)</t>
-  </si>
-  <si>
-    <t>Exotic or salin aromas (White wine)</t>
-  </si>
-  <si>
     <t>Sweet but always lively with candied pinapple, vanilla, and white truffle aromas (White wine)</t>
   </si>
   <si>
@@ -804,12 +783,6 @@
   </si>
   <si>
     <t>Makes dry wines; Floral with cloves notes</t>
-  </si>
-  <si>
-    <t>Light and refreshing; Strong acidity; Aromas of Fruits: lemon, grapefruit, peach, apple, lime, lemongrass; flowers and minerals (White wine)</t>
-  </si>
-  <si>
-    <t>Intense color and aromas; Rose, litchi, cinnamon, pepper aromas (White wine)</t>
   </si>
   <si>
     <t>Low acidity, lanolin, citrus, honey and vegetal flavours (White wine)</t>
@@ -2108,6 +2081,33 @@
   </si>
   <si>
     <t>&lt;div&gt; &lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt; Smoked, grilled, nuts, vanilla, apple, tropical fruits, pineapple, earthy, minerals, mushrooms&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;White, intense&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Rose, litchi, cinnamon, pepper aromas&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Intense aromas&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White, darker than most of the white wines&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Neutral aromas of fruits' skin such as peach or orange&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Medium body&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruits, lemon, grapefruit, peach, apple, lime, lemongrass, flowers and minerals&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Light and refreshing&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Very acid&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Herbal, minerals, grass, fruits such as melon In California it has Oak taste&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Good acidity&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Flowers&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Delicate, subtil&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Mineral, intense, white flowers and white fruits&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Very fresh, intense&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;White pepper, mellifère (nectar plants)&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Exotic or salin&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -2505,7 +2505,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2513,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>668</v>
+        <v>659</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2534,7 +2534,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2545,7 +2545,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>671</v>
+        <v>662</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2561,7 +2561,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>666</v>
+        <v>657</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2569,7 +2569,7 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>667</v>
+        <v>658</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2598,7 +2598,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>673</v>
+        <v>664</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="B22" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2617,7 +2617,7 @@
         <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>669</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -2712,7 +2712,7 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>680</v>
+        <v>671</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2736,7 +2736,7 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>676</v>
+        <v>667</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2744,7 +2744,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>681</v>
+        <v>672</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2816,7 +2816,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>677</v>
+        <v>668</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2824,15 +2824,15 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>682</v>
+        <v>673</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2848,15 +2848,15 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>678</v>
+        <v>669</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="B28" t="s">
-        <v>679</v>
+        <v>670</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2864,12 +2864,12 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>683</v>
+        <v>674</v>
       </c>
       <c r="B30" t="s">
         <v>79</v>
@@ -2888,7 +2888,7 @@
         <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>684</v>
+        <v>675</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2904,15 +2904,15 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>685</v>
+        <v>676</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B35" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3011,154 +3011,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B10" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B14" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B15" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>
@@ -3177,15 +3177,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
@@ -3193,39 +3193,39 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
         <v>102</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B8" t="s">
         <v>102</v>
@@ -3241,39 +3241,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B13" t="s">
         <v>90</v>
@@ -3281,15 +3281,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B14" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B15" t="s">
         <v>102</v>
@@ -3297,79 +3297,79 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B21" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B22" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B23" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B24" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
@@ -3377,15 +3377,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B26" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B27" t="s">
         <v>123</v>
@@ -3393,23 +3393,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B28" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B29" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B30" t="s">
         <v>105</v>
@@ -3417,15 +3417,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
@@ -3441,55 +3441,55 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
+        <v>277</v>
+      </c>
+      <c r="B34" t="s">
         <v>286</v>
-      </c>
-      <c r="B34" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
+        <v>278</v>
+      </c>
+      <c r="B35" t="s">
         <v>287</v>
-      </c>
-      <c r="B35" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B37" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B38" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B39" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B40" t="s">
         <v>102</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B41" t="s">
         <v>94</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B42" t="s">
         <v>94</v>
@@ -3513,39 +3513,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B43" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B44" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B45" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B46" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
@@ -3553,63 +3553,63 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
+        <v>304</v>
+      </c>
+      <c r="B48" t="s">
         <v>313</v>
-      </c>
-      <c r="B48" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B49" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B50" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B51" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B52" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B53" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B54" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B55" t="s">
         <v>129</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -3625,63 +3625,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B57" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B58" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B61" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B62" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B63" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B64" t="s">
         <v>98</v>
@@ -3689,26 +3689,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B65" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B66" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B67" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3731,7 +3731,7 @@
         <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>692</v>
+        <v>683</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3739,7 +3739,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>684</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3747,7 +3747,7 @@
         <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>685</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3755,7 +3755,7 @@
         <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>259</v>
+        <v>686</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3763,7 +3763,7 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>687</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3771,7 +3771,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>688</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3779,7 +3779,7 @@
         <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>689</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3787,7 +3787,7 @@
         <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3795,7 +3795,7 @@
         <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>691</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3803,7 +3803,7 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>692</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3811,7 +3811,7 @@
         <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3819,7 +3819,7 @@
         <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3827,7 +3827,7 @@
         <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3835,7 +3835,7 @@
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3843,7 +3843,7 @@
         <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3851,7 +3851,7 @@
         <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3859,7 +3859,7 @@
         <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3867,7 +3867,7 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3875,23 +3875,23 @@
         <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3899,15 +3899,15 @@
         <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3915,135 +3915,135 @@
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B28" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B30" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B32" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B35" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B36" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B38" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B39" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B40" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4051,11 +4051,12 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4071,114 +4072,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
-        <v>687</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
-        <v>688</v>
+        <v>679</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B5" t="s">
-        <v>690</v>
+        <v>681</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>691</v>
+        <v>682</v>
       </c>
       <c r="B6" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B8" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B10" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B14" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -4198,252 +4199,252 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="B1" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B3" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B6" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
       <c r="B7" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B8" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B9" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B11" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B12" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B13" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="B14" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B15" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="B16" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B17" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="B18" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="B19" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="B22" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="B23" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="B24" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="B25" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="B26" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="B27" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="B28" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B30" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B31" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
@@ -4451,87 +4452,87 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B33" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="B34" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="B35" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B36" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="B37" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="B38" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B40" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>662</v>
+        <v>653</v>
       </c>
       <c r="B41" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B42" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
@@ -4539,42 +4540,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="B44" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="B45" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B46" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B47" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="B48" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4651,223 +4652,223 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" t="s">
         <v>153</v>
-      </c>
-      <c r="B58" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B59" t="s">
-        <v>663</v>
+        <v>654</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="B60" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="B61" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="B62" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="B63" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="B64" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="B65" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="B66" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="B68" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B69" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B70" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="B71" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B72" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B73" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B74" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B76" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B77" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B78" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B79" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B80" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="B81" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B82" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="B83" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="B84" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="B85" t="s">
         <v>103</v>
@@ -4875,250 +4876,250 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="B86" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="B87" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="B88" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="B89" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="B90" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="B91" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="B92" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="B93" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="B94" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="B95" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="B96" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="B97" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="B98" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B99" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="B100" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="B101" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="B102" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="B103" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="B104" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="B105" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="B106" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="B107" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="B108" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="B109" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="B110" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="B111" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="B112" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="B113" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="B114" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
+        <v>516</v>
+      </c>
+      <c r="B115" t="s">
         <v>525</v>
-      </c>
-      <c r="B115" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="B116" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -5138,474 +5139,474 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="B1" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="B2" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="B3" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="B4" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="B5" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="B6" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="B7" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="B8" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="B9" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="B10" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="B11" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="B12" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="B14" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="B15" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="B16" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="B17" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="B18" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="B19" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="B20" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="B21" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="B22" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="B23" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="B24" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="B25" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="B26" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="B27" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>593</v>
+        <v>584</v>
       </c>
       <c r="B28" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="B29" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="B30" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="B31" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
       <c r="B32" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="B33" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
       <c r="B34" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="B35" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="B36" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="B37" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="B38" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="B39" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="B40" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="B41" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="B42" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="B43" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="B44" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="B45" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="B46" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="B47" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="B48" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="B49" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B50" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="B51" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="B52" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="B53" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
       <c r="B54" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="B55" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="B56" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
       <c r="B57" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
       <c r="B58" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="B59" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: More varieties structured
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -419,27 +419,6 @@
     <t>Trebbiano</t>
   </si>
   <si>
-    <t>Sweet but always lively with candied pinapple, vanilla, and white truffle aromas (White wine)</t>
-  </si>
-  <si>
-    <t>Smooth aromas, candied pinapple  (White wine)</t>
-  </si>
-  <si>
-    <t>Floral aromas, Mellifère and a little bit mineral (White wine)</t>
-  </si>
-  <si>
-    <t>Fresh (White wine)</t>
-  </si>
-  <si>
-    <t>Floral aromas (White wine)</t>
-  </si>
-  <si>
-    <t>Neutral aromas, strong acidity, and low sweetness (White wine)</t>
-  </si>
-  <si>
-    <t>Strong acidity, low level of sweet, neutral taste (White wine)</t>
-  </si>
-  <si>
     <t>Cabernet-Sauvignon</t>
   </si>
   <si>
@@ -491,27 +470,6 @@
     <t>Hare civet, Truffle risotto</t>
   </si>
   <si>
-    <t>Powerful wines; Can age well (Red wine)</t>
-  </si>
-  <si>
-    <t>Powerful aromas and spicy; Sweet (Red wine)</t>
-  </si>
-  <si>
-    <t>Fruits and violet aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>Spicy and fruity aromas; Good ageing capacity (Red wine)</t>
-  </si>
-  <si>
-    <t>Subtil and delicate; Similar to cabernet franc (Red wine)</t>
-  </si>
-  <si>
-    <t>Strong, structured, robust, pulpy fruits, rich, sappy with bitter almond notes  (Red wine)</t>
-  </si>
-  <si>
-    <t>Kirsch aromas (Red wine)</t>
-  </si>
-  <si>
     <t>AOP / PDO</t>
   </si>
   <si>
@@ -776,31 +734,10 @@
     <t>Aligoté</t>
   </si>
   <si>
-    <t>To drink young; Fresh, fruity</t>
-  </si>
-  <si>
     <t>Marsanne</t>
   </si>
   <si>
-    <t>Makes dry wines; Floral with cloves notes</t>
-  </si>
-  <si>
-    <t>Low acidity, lanolin, citrus, honey and vegetal flavours (White wine)</t>
-  </si>
-  <si>
-    <t>Dry apricot aromas, violet, musc, tobacco, and licorice (White wine)</t>
-  </si>
-  <si>
     <t>Cinsault</t>
-  </si>
-  <si>
-    <t>Strong wine, age fast, floral aromas</t>
-  </si>
-  <si>
-    <t>Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
-  </si>
-  <si>
-    <t>Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries, cherry and earthy or wooden aromas (Red wine)</t>
   </si>
   <si>
     <t>Merlot, Cabernet-Sauvignon, Cabernet-Franc, Malbec, Petit Verdot</t>
@@ -1933,9 +1870,6 @@
     <t>Country; Region ; District; Sub-district; Town Vineyard or plot.</t>
   </si>
   <si>
-    <t>Floral aromas, lemongrass, herbs and fruity aromas, apple, grapefruit, with nut taste</t>
-  </si>
-  <si>
     <t>16 - 18 ° C / 60.8 - 64.4 ° F</t>
   </si>
   <si>
@@ -1960,33 +1894,6 @@
     <t>For the wine cheaper than 5 € there is no need of aeration usually because there is a low level of tannin</t>
   </si>
   <si>
-    <t>Strong tannin taste, strong to medium strenght, cassis aromas, and sometime vegetal aromas, violet, or sometime other fruits; Can age (Red wine)</t>
-  </si>
-  <si>
-    <t>Deep color, deep body, strong level of alcohol and low tannin taste; Red fruits, Plum, chocolate or mushrooms aromas;(Red wine)</t>
-  </si>
-  <si>
-    <t>Strong tannin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
-  </si>
-  <si>
-    <t>Low to medium acidity; Medium tannin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>Dark color; Very robust; Strong tannin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
-  </si>
-  <si>
-    <t>Rich wine; High level of alcohol; Medium to high level of tannin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
-  </si>
-  <si>
-    <t>Light color; Low tannin; Red fruits aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>Light wines; Delicates, fruity; Good acidity and low tannin; (Red wine)</t>
-  </si>
-  <si>
-    <t>Elegant tannin structure, nice aromas, very fruity: cassis, currant), violet, vegetal; good ageing capacity (Red wine)</t>
-  </si>
-  <si>
     <t>Wine with a lot of tannin</t>
   </si>
   <si>
@@ -2095,9 +2002,6 @@
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Very acid&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Herbal, minerals, grass, fruits such as melon In California it has Oak taste&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Good acidity&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Flowers&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Delicate, subtil&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
@@ -2108,6 +2012,102 @@
   </si>
   <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Exotic or salin&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong tannin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries, cherry and earthy or wooden aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Low to medium acidity; Medium tannin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Dark color; Very robust; Strong tannin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Rich wine; High level of alcohol; Medium to high level of tannin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful wines; Can age well (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Light color; Low tannin; Red fruits aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Light wines; Delicates, fruity; Good acidity and low tannin; (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Elegant tannin structure, nice aromas, very fruity: cassis, currant), violet, vegetal; good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful aromas and spicy; Sweet (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Fruits and violet aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Spicy and fruity aromas; Good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Subtil and delicate; Similar to cabernet franc (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong, structured, robust, pulpy fruits, rich, sappy with bitter almond notes  (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Kirsch aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;To drink young; Fresh, fruity</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Makes dry wines; Floral with cloves notes</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong wine, age fast, floral aromas</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Floral aromas, lemongrass, herbs and fruity aromas, apple, grapefruit, with nut taste</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;candied pinapple&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Smouth&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Floral, mellifère, little bit mineral&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Sweet but always lively&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;candied pinapple, vanilla, and white truffle&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Good acidity&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Dry apricot, violet, musc, tobacco, licorice&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Fresh&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Fresh&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Floral&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong acidity, and low sweetness&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Neutral&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Lanolin, citrus, honey and vegetal&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong acidity, low level of sweet&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Neutral&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red (can age)&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong tannin taste&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;cassis and sometime vegetal violet, or sometime other fruits&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Strong to medium strength&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, deep color&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Red fruits, Plum, chocolate or mushrooms&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Deep body, strong level of alcohol and low tannin taste&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -2505,7 +2505,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>656</v>
+        <v>625</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2513,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>659</v>
+        <v>628</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2534,7 +2534,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>663</v>
+        <v>632</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2545,7 +2545,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>662</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2561,7 +2561,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>657</v>
+        <v>626</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2569,7 +2569,7 @@
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>658</v>
+        <v>627</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2598,7 +2598,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>664</v>
+        <v>633</v>
       </c>
       <c r="B21" t="s">
         <v>84</v>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>665</v>
+        <v>634</v>
       </c>
       <c r="B22" t="s">
-        <v>661</v>
+        <v>630</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2617,7 +2617,7 @@
         <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>660</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>
@@ -2712,7 +2712,7 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>671</v>
+        <v>640</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2736,7 +2736,7 @@
         <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>667</v>
+        <v>636</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2744,7 +2744,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>672</v>
+        <v>641</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2816,7 +2816,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>668</v>
+        <v>637</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2824,15 +2824,15 @@
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>673</v>
+        <v>642</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2848,15 +2848,15 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>669</v>
+        <v>638</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>666</v>
+        <v>635</v>
       </c>
       <c r="B28" t="s">
-        <v>670</v>
+        <v>639</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2864,12 +2864,12 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>655</v>
+        <v>624</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>674</v>
+        <v>643</v>
       </c>
       <c r="B30" t="s">
         <v>79</v>
@@ -2888,7 +2888,7 @@
         <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>675</v>
+        <v>644</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -2904,15 +2904,15 @@
         <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>676</v>
+        <v>645</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B35" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3011,154 +3011,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>633</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="B17" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B19" t="s">
-        <v>677</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>
@@ -3177,15 +3177,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
@@ -3193,39 +3193,39 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
         <v>102</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
         <v>102</v>
@@ -3241,39 +3241,39 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="B10" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B13" t="s">
         <v>90</v>
@@ -3281,15 +3281,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
         <v>102</v>
@@ -3297,79 +3297,79 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="B25" t="s">
         <v>90</v>
@@ -3377,15 +3377,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="B26" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="B27" t="s">
         <v>123</v>
@@ -3393,23 +3393,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B29" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B30" t="s">
         <v>105</v>
@@ -3417,15 +3417,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
@@ -3441,55 +3441,55 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B34" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="B35" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="B37" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="B38" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B39" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="B40" t="s">
         <v>102</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="B41" t="s">
         <v>94</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
         <v>94</v>
@@ -3513,39 +3513,39 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="B43" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="B44" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="B45" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B46" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="B47" t="s">
         <v>97</v>
@@ -3553,63 +3553,63 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="B48" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="B49" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="B50" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="B51" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="B52" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="B54" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
       <c r="B55" t="s">
         <v>129</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="B56" t="s">
         <v>94</v>
@@ -3625,63 +3625,63 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="B57" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="B58" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="B59" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="B60" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B61" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="B62" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="B63" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="B64" t="s">
         <v>98</v>
@@ -3689,26 +3689,26 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="B65" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="B66" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="B67" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3720,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3731,7 +3731,7 @@
         <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>683</v>
+        <v>652</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3739,7 +3739,7 @@
         <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>684</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3747,7 +3747,7 @@
         <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>685</v>
+        <v>654</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3755,7 +3755,7 @@
         <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>686</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3763,7 +3763,7 @@
         <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>687</v>
+        <v>656</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3771,7 +3771,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3779,7 +3779,7 @@
         <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3787,7 +3787,7 @@
         <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>690</v>
+        <v>658</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3795,7 +3795,7 @@
         <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>691</v>
+        <v>659</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3803,7 +3803,7 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>692</v>
+        <v>660</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3811,7 +3811,7 @@
         <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>683</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3819,7 +3819,7 @@
         <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>681</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3827,7 +3827,7 @@
         <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>682</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3835,7 +3835,7 @@
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>685</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3843,7 +3843,7 @@
         <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>686</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3851,7 +3851,7 @@
         <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>687</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3859,7 +3859,7 @@
         <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>688</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3867,7 +3867,7 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>252</v>
+        <v>689</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3875,23 +3875,23 @@
         <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>690</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>643</v>
+        <v>691</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>644</v>
+        <v>692</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3899,15 +3899,15 @@
         <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>645</v>
+        <v>661</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>257</v>
+        <v>662</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3915,135 +3915,135 @@
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>646</v>
+        <v>663</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>647</v>
+        <v>664</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>648</v>
+        <v>665</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>666</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>649</v>
+        <v>667</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>650</v>
+        <v>668</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>651</v>
+        <v>669</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>155</v>
+        <v>670</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>256</v>
+        <v>671</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>156</v>
+        <v>672</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>673</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>674</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>159</v>
+        <v>675</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>160</v>
+        <v>676</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B38" t="s">
-        <v>249</v>
+        <v>677</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B39" t="s">
-        <v>251</v>
+        <v>678</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>255</v>
+        <v>679</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4051,7 +4051,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>634</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -4072,114 +4072,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>678</v>
+        <v>647</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
-        <v>679</v>
+        <v>648</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>681</v>
+        <v>650</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>682</v>
+        <v>651</v>
       </c>
       <c r="B6" t="s">
-        <v>680</v>
+        <v>649</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>642</v>
+        <v>620</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="B8" t="s">
-        <v>635</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B9" t="s">
-        <v>636</v>
+        <v>614</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>637</v>
+        <v>615</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
-        <v>638</v>
+        <v>616</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B12" t="s">
-        <v>639</v>
+        <v>617</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
-        <v>641</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B14" t="s">
-        <v>640</v>
+        <v>618</v>
       </c>
     </row>
   </sheetData>
@@ -4199,252 +4199,252 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="B1" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="B2" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="B3" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="B5" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="B6" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>652</v>
+        <v>621</v>
       </c>
       <c r="B7" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="B8" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="B11" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="B12" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="B13" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="B14" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="B15" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="B16" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="B17" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="B18" t="s">
-        <v>409</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="B19" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="B22" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="B23" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="B24" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="B25" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="B26" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="B27" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="B28" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="B29" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
       <c r="B30" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="B31" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
@@ -4452,87 +4452,87 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="B33" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="B34" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="B35" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="B36" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="B37" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="B38" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="B40" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>653</v>
+        <v>622</v>
       </c>
       <c r="B41" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="B42" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="B43" t="s">
         <v>31</v>
@@ -4540,42 +4540,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="B44" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="B45" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="B46" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="B47" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="B48" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4652,223 +4652,223 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" t="s">
         <v>146</v>
-      </c>
-      <c r="B58" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="B59" t="s">
-        <v>654</v>
+        <v>623</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="B60" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="B61" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="B62" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="B63" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="B64" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="B65" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B66" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="B68" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B69" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="B70" t="s">
-        <v>458</v>
+        <v>437</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="B71" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="B72" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="B73" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="B74" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="B76" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
       <c r="B77" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
       <c r="B78" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="B79" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="B80" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="B81" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="B82" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="B83" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="B84" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="B85" t="s">
         <v>103</v>
@@ -4876,250 +4876,250 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="B86" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="B87" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="B88" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="B89" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="B90" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="B91" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
       <c r="B92" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="B93" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="B94" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="B95" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="B96" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B97" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="B98" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="B99" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="B100" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="B101" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="B102" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="B103" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="B104" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="B105" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="B106" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="B107" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="B108" t="s">
-        <v>526</v>
+        <v>505</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="B109" t="s">
-        <v>527</v>
+        <v>506</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="B110" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
       <c r="B111" t="s">
-        <v>528</v>
+        <v>507</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
       <c r="B112" t="s">
-        <v>529</v>
+        <v>508</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="B113" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
       <c r="B114" t="s">
-        <v>531</v>
+        <v>510</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="B115" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>515</v>
+        <v>494</v>
       </c>
       <c r="B116" t="s">
-        <v>532</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -5139,474 +5139,474 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="B1" t="s">
-        <v>533</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>558</v>
+        <v>537</v>
       </c>
       <c r="B2" t="s">
-        <v>534</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>559</v>
+        <v>538</v>
       </c>
       <c r="B3" t="s">
-        <v>535</v>
+        <v>514</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>539</v>
       </c>
       <c r="B4" t="s">
-        <v>536</v>
+        <v>515</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>561</v>
+        <v>540</v>
       </c>
       <c r="B5" t="s">
-        <v>536</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>562</v>
+        <v>541</v>
       </c>
       <c r="B6" t="s">
-        <v>537</v>
+        <v>516</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>563</v>
+        <v>542</v>
       </c>
       <c r="B7" t="s">
-        <v>539</v>
+        <v>518</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>564</v>
+        <v>543</v>
       </c>
       <c r="B8" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>565</v>
+        <v>544</v>
       </c>
       <c r="B9" t="s">
-        <v>540</v>
+        <v>519</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>566</v>
+        <v>545</v>
       </c>
       <c r="B10" t="s">
-        <v>541</v>
+        <v>520</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>567</v>
+        <v>546</v>
       </c>
       <c r="B11" t="s">
-        <v>541</v>
+        <v>520</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>568</v>
+        <v>547</v>
       </c>
       <c r="B12" t="s">
-        <v>542</v>
+        <v>521</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>569</v>
+        <v>548</v>
       </c>
       <c r="B13" t="s">
-        <v>542</v>
+        <v>521</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>549</v>
       </c>
       <c r="B14" t="s">
-        <v>542</v>
+        <v>521</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>571</v>
+        <v>550</v>
       </c>
       <c r="B15" t="s">
-        <v>543</v>
+        <v>522</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>572</v>
+        <v>551</v>
       </c>
       <c r="B16" t="s">
-        <v>544</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>573</v>
+        <v>552</v>
       </c>
       <c r="B17" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>574</v>
+        <v>553</v>
       </c>
       <c r="B18" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>575</v>
+        <v>554</v>
       </c>
       <c r="B19" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>576</v>
+        <v>555</v>
       </c>
       <c r="B20" t="s">
-        <v>546</v>
+        <v>525</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>577</v>
+        <v>556</v>
       </c>
       <c r="B21" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="B22" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>579</v>
+        <v>558</v>
       </c>
       <c r="B23" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="B24" t="s">
-        <v>549</v>
+        <v>528</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>581</v>
+        <v>560</v>
       </c>
       <c r="B25" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="B26" t="s">
-        <v>551</v>
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="B27" t="s">
-        <v>552</v>
+        <v>531</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>584</v>
+        <v>563</v>
       </c>
       <c r="B28" t="s">
-        <v>553</v>
+        <v>532</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>585</v>
+        <v>564</v>
       </c>
       <c r="B29" t="s">
-        <v>554</v>
+        <v>533</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>586</v>
+        <v>565</v>
       </c>
       <c r="B30" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>587</v>
+        <v>566</v>
       </c>
       <c r="B31" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>588</v>
+        <v>567</v>
       </c>
       <c r="B32" t="s">
-        <v>555</v>
+        <v>534</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>589</v>
+        <v>568</v>
       </c>
       <c r="B33" t="s">
-        <v>616</v>
+        <v>595</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
       <c r="B34" t="s">
-        <v>616</v>
+        <v>595</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>591</v>
+        <v>570</v>
       </c>
       <c r="B35" t="s">
-        <v>617</v>
+        <v>596</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>592</v>
+        <v>571</v>
       </c>
       <c r="B36" t="s">
-        <v>618</v>
+        <v>597</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>593</v>
+        <v>572</v>
       </c>
       <c r="B37" t="s">
-        <v>619</v>
+        <v>598</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>594</v>
+        <v>573</v>
       </c>
       <c r="B38" t="s">
-        <v>619</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>595</v>
+        <v>574</v>
       </c>
       <c r="B39" t="s">
-        <v>620</v>
+        <v>599</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>596</v>
+        <v>575</v>
       </c>
       <c r="B40" t="s">
-        <v>620</v>
+        <v>599</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>597</v>
+        <v>576</v>
       </c>
       <c r="B41" t="s">
-        <v>621</v>
+        <v>600</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>598</v>
+        <v>577</v>
       </c>
       <c r="B42" t="s">
-        <v>621</v>
+        <v>600</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>599</v>
+        <v>578</v>
       </c>
       <c r="B43" t="s">
-        <v>622</v>
+        <v>601</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>600</v>
+        <v>579</v>
       </c>
       <c r="B44" t="s">
-        <v>624</v>
+        <v>603</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>601</v>
+        <v>580</v>
       </c>
       <c r="B45" t="s">
-        <v>624</v>
+        <v>603</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>581</v>
+      </c>
+      <c r="B46" t="s">
         <v>602</v>
-      </c>
-      <c r="B46" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>603</v>
+        <v>582</v>
       </c>
       <c r="B47" t="s">
-        <v>623</v>
+        <v>602</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
+        <v>583</v>
+      </c>
+      <c r="B48" t="s">
         <v>604</v>
-      </c>
-      <c r="B48" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
+        <v>584</v>
+      </c>
+      <c r="B49" t="s">
         <v>605</v>
-      </c>
-      <c r="B49" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
+        <v>585</v>
+      </c>
+      <c r="B50" t="s">
         <v>606</v>
-      </c>
-      <c r="B50" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
+        <v>586</v>
+      </c>
+      <c r="B51" t="s">
         <v>607</v>
-      </c>
-      <c r="B51" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
+        <v>587</v>
+      </c>
+      <c r="B52" t="s">
         <v>608</v>
-      </c>
-      <c r="B52" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
+        <v>588</v>
+      </c>
+      <c r="B53" t="s">
         <v>609</v>
-      </c>
-      <c r="B53" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
+        <v>589</v>
+      </c>
+      <c r="B54" t="s">
         <v>610</v>
-      </c>
-      <c r="B54" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
+        <v>590</v>
+      </c>
+      <c r="B55" t="s">
         <v>611</v>
-      </c>
-      <c r="B55" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>612</v>
+        <v>591</v>
       </c>
       <c r="B56" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>613</v>
+        <v>592</v>
       </c>
       <c r="B57" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>614</v>
+        <v>593</v>
       </c>
       <c r="B58" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>615</v>
+        <v>594</v>
       </c>
       <c r="B59" t="s">
-        <v>632</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:construction: More varities structured
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -2014,66 +2014,6 @@
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Exotic or salin&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong tannin and acidity; Strong alcohol level that makes it smoother; Dark when it's young, and starts to get some orange shading when it ages; Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar, 0 (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Delicate and stimulating; Paler than Merlot or Cabernet; Low to medium acidity; Fruity aromas: Red berries, cherry and earthy or wooden aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Low to medium acidity; Medium tannin; Fruity aromas, cherry; Floral aromas, violet; Sometime hazelnut aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Dark color; Very robust; Strong tannin level; Aromas: violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime Strawberry; (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Rich wine; High level of alcohol; Medium to high level of tannin; Aromas: blackberry, raspberry, spicy notes, jam (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful wines; Can age well (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Light color; Low tannin; Red fruits aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Light wines; Delicates, fruity; Good acidity and low tannin; (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Elegant tannin structure, nice aromas, very fruity: cassis, currant), violet, vegetal; good ageing capacity (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful aromas and spicy; Sweet (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Fruits and violet aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Spicy and fruity aromas; Good ageing capacity (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Subtil and delicate; Similar to cabernet franc (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong, structured, robust, pulpy fruits, rich, sappy with bitter almond notes  (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Kirsch aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;To drink young; Fresh, fruity</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Makes dry wines; Floral with cloves notes</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong wine, age fast, floral aromas</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Floral aromas, lemongrass, herbs and fruity aromas, apple, grapefruit, with nut taste</t>
-  </si>
-  <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;candied pinapple&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Smouth&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
@@ -2108,6 +2048,66 @@
   </si>
   <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, deep color&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Red fruits, Plum, chocolate or mushrooms&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Deep body, strong level of alcohol and low tannin taste&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, dark when it's young, and starts to get some orange shading when it ages&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong tannin and acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Strong alcohol level that makes it smoother&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful aromas and spicy; Sweet (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Fruits and violet aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Spicy and fruity aromas; Good ageing capacity (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Subtil and delicate; Similar to cabernet franc (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong, structured, robust, pulpy fruits, rich, sappy with bitter almond notes  (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Kirsch aromas (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;To drink young; Fresh, fruity</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Makes dry wines; Floral with cloves notes</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong wine, age fast, floral aromas</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Floral aromas, lemongrass, herbs and fruity aromas, apple, grapefruit, with nut taste</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, paler than Merlot or Cabernet&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low to medium acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruity, Red berries, cherry and earthy or wooden&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Delicate and stimulating&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low to medium acidity; medium tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruity aromas, cherry; floral aromas, violet; sometime hazelnut&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, darl color&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong tannin level&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;violet, cherry, smoked meat, grilled pepper, tar, burnt rubber, sometime strawberry&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Very robust&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Medium to high level of tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Blackberry, raspberry, spicy notes, jam&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Rich wine, high level of alcohol&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, can age well&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Powerful wines&lt;/p&gt;&lt;/div&gt;;  (Red wine)</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, light color&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Red fruits&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Good acidity and low tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruity&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Light wines, delicates&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red,  good ageing capacity&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Elegant tannin structure&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Very fruity: cassis, currant, violet, vegetal&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3771,7 +3771,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>684</v>
+        <v>664</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3811,7 +3811,7 @@
         <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>683</v>
+        <v>663</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3819,7 +3819,7 @@
         <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>681</v>
+        <v>661</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3827,7 +3827,7 @@
         <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>682</v>
+        <v>662</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3835,7 +3835,7 @@
         <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>685</v>
+        <v>665</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3843,7 +3843,7 @@
         <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>686</v>
+        <v>666</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3851,7 +3851,7 @@
         <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>687</v>
+        <v>667</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3859,7 +3859,7 @@
         <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>688</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3867,7 +3867,7 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>689</v>
+        <v>669</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3875,7 +3875,7 @@
         <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>690</v>
+        <v>670</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3883,7 +3883,7 @@
         <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>691</v>
+        <v>671</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3891,7 +3891,7 @@
         <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>692</v>
+        <v>672</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3899,7 +3899,7 @@
         <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>661</v>
+        <v>673</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3907,7 +3907,7 @@
         <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>662</v>
+        <v>685</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3915,7 +3915,7 @@
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>663</v>
+        <v>686</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3923,7 +3923,7 @@
         <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>664</v>
+        <v>687</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3931,7 +3931,7 @@
         <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>665</v>
+        <v>688</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3939,7 +3939,7 @@
         <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>666</v>
+        <v>689</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3947,7 +3947,7 @@
         <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>667</v>
+        <v>690</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3955,7 +3955,7 @@
         <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>668</v>
+        <v>691</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3963,7 +3963,7 @@
         <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>669</v>
+        <v>692</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3971,7 +3971,7 @@
         <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3979,7 +3979,7 @@
         <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3987,7 +3987,7 @@
         <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3995,7 +3995,7 @@
         <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4003,7 +4003,7 @@
         <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4011,7 +4011,7 @@
         <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4019,7 +4019,7 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4027,7 +4027,7 @@
         <v>234</v>
       </c>
       <c r="B38" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4035,7 +4035,7 @@
         <v>235</v>
       </c>
       <c r="B39" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4043,7 +4043,7 @@
         <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4051,7 +4051,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:sparkles: All the varieties has been restructured
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -2053,39 +2053,6 @@
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, dark when it's young, and starts to get some orange shading when it ages&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Strong tannin and acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruits aromas: strawberry, jam; Earthy and wooden aromas: tar&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Strong alcohol level that makes it smoother&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful aromas and spicy; Sweet (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Powerful and rich with great fineness; fruity aromas: plum, spicy such as cinamon (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Fruits and violet aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Spicy and fruity aromas; Good ageing capacity (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Subtil and delicate; Similar to cabernet franc (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong, structured, robust, pulpy fruits, rich, sappy with bitter almond notes  (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Kirsch aromas (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;To drink young; Fresh, fruity</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Makes dry wines; Floral with cloves notes</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Strong wine, age fast, floral aromas</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;Floral aromas, lemongrass, herbs and fruity aromas, apple, grapefruit, with nut taste</t>
-  </si>
-  <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, paler than Merlot or Cabernet&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low to medium acidity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruity, Red berries, cherry and earthy or wooden&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Delicate and stimulating&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
@@ -2108,6 +2075,39 @@
   </si>
   <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red,  good ageing capacity&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Elegant tannin structure&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Very fruity: cassis, currant, violet, vegetal&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Spicy and sweet&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Powerful &lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;fruity, plum, spicy, cinamon&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Powerful and rich with great fineness&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruits and violet&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, wine similar to cabernet franc&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Subtil and delicate&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, good ageing capacity&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Spicy and fruity&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Pulpy fruits, rich, sappy with bitter almond notes&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Strong, structured, robust&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Kirsch&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, to drink young&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruity&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Fresh&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Dry&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Floral with cloves notes&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, age fast&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Floral&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Strong&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Floral, lemongrass, herbs and fruity, apple, grapefruit, with nut taste&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3907,7 +3907,7 @@
         <v>132</v>
       </c>
       <c r="B23" t="s">
-        <v>685</v>
+        <v>674</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3915,7 +3915,7 @@
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>686</v>
+        <v>675</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3923,7 +3923,7 @@
         <v>133</v>
       </c>
       <c r="B25" t="s">
-        <v>687</v>
+        <v>676</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3931,7 +3931,7 @@
         <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>688</v>
+        <v>677</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3939,7 +3939,7 @@
         <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3947,7 +3947,7 @@
         <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>690</v>
+        <v>679</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3955,7 +3955,7 @@
         <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3963,7 +3963,7 @@
         <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>692</v>
+        <v>681</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3971,7 +3971,7 @@
         <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3979,7 +3979,7 @@
         <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3987,7 +3987,7 @@
         <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>676</v>
+        <v>684</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3995,7 +3995,7 @@
         <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4003,7 +4003,7 @@
         <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>678</v>
+        <v>685</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4011,7 +4011,7 @@
         <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>679</v>
+        <v>687</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4019,7 +4019,7 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>680</v>
+        <v>688</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4027,7 +4027,7 @@
         <v>234</v>
       </c>
       <c r="B38" t="s">
-        <v>681</v>
+        <v>689</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4035,7 +4035,7 @@
         <v>235</v>
       </c>
       <c r="B39" t="s">
-        <v>682</v>
+        <v>690</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4043,7 +4043,7 @@
         <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>683</v>
+        <v>691</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4051,7 +4051,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:bug: Little bug fixes
</commit_message>
<xml_diff>
--- a/src/FlashCards.xlsx
+++ b/src/FlashCards.xlsx
@@ -2065,18 +2065,9 @@
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Medium to high level of tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Blackberry, raspberry, spicy notes, jam&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Rich wine, high level of alcohol&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, can age well&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Powerful wines&lt;/p&gt;&lt;/div&gt;;  (Red wine)</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, light color&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Red fruits&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Good acidity and low tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Fruity&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Light wines, delicates&lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
-    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red,  good ageing capacity&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Elegant tannin structure&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Very fruity: cassis, currant, violet, vegetal&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;&lt;/p&gt;&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Spicy and sweet&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Powerful &lt;/p&gt;&lt;/div&gt;</t>
   </si>
   <si>
@@ -2108,6 +2099,15 @@
   </si>
   <si>
     <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;White&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Floral, lemongrass, herbs and fruity, apple, grapefruit, with nut taste&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, can age well&lt;/p&gt;&lt;p&gt;👄&lt;strong&gt;Mouthfeel - &lt;/strong&gt;Powerful wines&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red, light color&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Low tannin&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Red fruits&lt;/p&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;p&gt;🍷&lt;strong&gt;Wine color - &lt;/strong&gt;Red,  good ageing capacity&lt;/p&gt;&lt;p&gt;👅&lt;strong&gt;Basic tastes - &lt;/strong&gt;Elegant tannin structure&lt;/p&gt;&lt;p&gt;🍓&lt;strong&gt;Aromas - &lt;/strong&gt;Very fruity: cassis, currant, violet, vegetal&lt;/p&gt;&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3721,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3806,7 +3806,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>118</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3947,7 +3947,7 @@
         <v>136</v>
       </c>
       <c r="B28" t="s">
-        <v>679</v>
+        <v>691</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3955,7 +3955,7 @@
         <v>137</v>
       </c>
       <c r="B29" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3963,7 +3963,7 @@
         <v>138</v>
       </c>
       <c r="B30" t="s">
-        <v>681</v>
+        <v>692</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3971,7 +3971,7 @@
         <v>139</v>
       </c>
       <c r="B31" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3979,7 +3979,7 @@
         <v>140</v>
       </c>
       <c r="B32" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3987,7 +3987,7 @@
         <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3995,7 +3995,7 @@
         <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4003,7 +4003,7 @@
         <v>143</v>
       </c>
       <c r="B35" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4011,7 +4011,7 @@
         <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4019,7 +4019,7 @@
         <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4027,7 +4027,7 @@
         <v>234</v>
       </c>
       <c r="B38" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4035,7 +4035,7 @@
         <v>235</v>
       </c>
       <c r="B39" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4043,7 +4043,7 @@
         <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -4051,7 +4051,7 @@
         <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>